<commit_message>
Compeleted implementation of Excel reporter
</commit_message>
<xml_diff>
--- a/AxeAccessibilityDriver/AxeAccessibilityDriver/AODA_Template.xlsx
+++ b/AxeAccessibilityDriver/AxeAccessibilityDriver/AODA_Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DUONGCH\Projects\AxeAccessibilityDriver\AxeAccessibilityDriver\AxeAccessibilityDriver\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40DEE297-A189-401F-9CA0-BBA0D78E68F7}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{742EF0C8-6EB1-44D1-A0ED-0C9622A6974A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="760" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="760" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="5" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="252">
   <si>
     <t>1.1.1</t>
   </si>
@@ -294,9 +294,6 @@
     <t>Web Accessibility falls within the information and communications standard of Accessibility for Ontarians with Disabilities Act (AODA). Section 14, Accessible websites and web content outlines the following requirements ("success criteria") from Web Content Accessibility Guidelines (WCAG) 2.0. Each criterion is categorized as either a level “A” or “AA”.</t>
   </si>
   <si>
-    <t>…</t>
-  </si>
-  <si>
     <t>Evaluation Date:</t>
   </si>
   <si>
@@ -2294,54 +2291,6 @@
     <t xml:space="preserve">  </t>
   </si>
   <si>
-    <t>to be determined</t>
-  </si>
-  <si>
-    <t>http://intra.dev.edcs7.csc.gov.on.ca:82/uat1111/bi/?perspective=classicviewer&amp;id=i50BE89F36FE54165B4E6E1D6E697D591&amp;isViewer=false&amp;isNewFromModule=false&amp;isNewFromPackage=false&amp;isNewDataSetFromModule=false&amp;isNewDataSetFromPackage=false&amp;isTemplate=false&amp;isDataset=false&amp;UIProfile=Titan&amp;cmProperties%5Bid%5D=i50BE89F36FE54165B4E6E1D6E697D591&amp;cmProperties%5BdefaultName%5D=Help+Page&amp;cmProperties%5Btype%5D=report&amp;cmProperties%5Bpermissions%5D%5B%5D=execute&amp;cmProperties%5Bpermissions%5D%5B%5D=read&amp;cmProperties%5Bpermissions%5D%5B%5D=traverse&amp;rsFinalRunOptions%5Bformat%5D=HTML&amp;rsFinalRunOptions%5Ba11y%5D=true&amp;rsFinalRunOptions%5Bbidi%5D=false&amp;rsFinalRunOptions%5BrunInAdvancedViewer%5D=false&amp;rsFinalRunOptions%5BDownload%5D=false&amp;rsFinalRunOptions%5Bprompt%5D=true&amp;rsFinalRunOptions%5BisApplication%5D=false</t>
-  </si>
-  <si>
-    <t>Ensures every id attribute value used in ARIA and in labels is unique</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Ensures &lt;img&gt; elements have alternate text or a role of none or presentation</t>
-  </si>
-  <si>
-    <t>http://intra.dev.edcs7.csc.gov.on.ca:82/uat1111/bi/v1/disp</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Ensures every HTML document has a lang attribute</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Ensures that lists are structured correctly</t>
-  </si>
-  <si>
-    <t>http://intra.dev.edcs7.csc.gov.on.ca:82/uat1111/bi/?perspective=classicviewer&amp;id=iBED499536FAD473C8A83A8C9EC9356DF&amp;isViewer=false&amp;isNewFromModule=false&amp;isNewFromPackage=false&amp;isNewDataSetFromModule=false&amp;isNewDataSetFromPackage=false&amp;isTemplate=false&amp;isDataset=false&amp;UIProfile=Titan&amp;cmProperties%5Bid%5D=iBED499536FAD473C8A83A8C9EC9356DF&amp;cmProperties%5BdefaultName%5D=CGRT_Main_Menu&amp;cmProperties%5Btype%5D=report&amp;cmProperties%5Bpermissions%5D%5B%5D=execute&amp;cmProperties%5Bpermissions%5D%5B%5D=read&amp;cmProperties%5Bpermissions%5D%5B%5D=traverse&amp;rsFinalRunOptions%5Bformat%5D=HTML&amp;rsFinalRunOptions%5Ba11y%5D=true&amp;rsFinalRunOptions%5Bbidi%5D=false&amp;rsFinalRunOptions%5BrunInAdvancedViewer%5D=false&amp;rsFinalRunOptions%5BDownload%5D=false&amp;rsFinalRunOptions%5Bprompt%5D=true&amp;rsFinalRunOptions%5BisApplication%5D=false</t>
-  </si>
-  <si>
-    <t>Ensures links have discernible text</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://intra.dev.edcs7.csc.gov.on.ca:82/uat1111/bi/?perspective=classicviewer&amp;pathRef=.public_folders%2FCGRT+Project%2FReports%2FCollege+Graduation+Rate+Report&amp;id=iC12ED54445264C6796833B12B83EB83A&amp;objRef=iC12ED54445264C6796833B12B83EB83A&amp;type=report&amp;prompt=false&amp;drillFormLabel=drillForm1563375283129&amp;action=run&amp;format=HTML&amp;cmProperties%5Bid%5D=iC12ED54445264C6796833B12B83EB83A&amp;cmProperties%5BdefaultName%5D=College+Graduation+Rate+Report&amp;cmProperties%5Btype%5D=report&amp;cmProperties%5Bpermissions%5D%5B%5D=execute&amp;cmProperties%5Bpermissions%5D%5B%5D=read&amp;cmProperties%5Bpermissions%5D%5B%5D=traverse                                                                                                                                                                                                                                                                                                                                                                                                     http://intra.dev.edcs7.csc.gov.on.ca:82/uat1111/bi/?perspective=classicviewer&amp;pathRef=.public_folders%2FCGRT+Project%2FReports%2FCollege+Graduation+Rate+Report&amp;id=iC12ED54445264C6796833B12B83EB83A&amp;objRef=iC12ED54445264C6796833B12B83EB83A&amp;type=report&amp;prompt=false&amp;drillFormLabel=drillForm1563375305286&amp;action=run&amp;format=HTML&amp;cmProperties%5Bid%5D=iC12ED54445264C6796833B12B83EB83A&amp;cmProperties%5BdefaultName%5D=College+Graduation+Rate+Report&amp;cmProperties%5Btype%5D=report&amp;cmProperties%5Bpermissions%5D%5B%5D=execute&amp;cmProperties%5Bpermissions%5D%5B%5D=read&amp;cmProperties%5Bpermissions%5D%5B%5D=traverse                                                                                                                                                                                                                                                                                                                                                                                                http://intra.dev.edcs7.csc.gov.on.ca:82/uat1111/bi/?perspective=classicviewer&amp;pathRef=.public_folders%2FCGRT+Project%2FReports%2FCollege+Graduation+Rate+Report&amp;id=iC12ED54445264C6796833B12B83EB83A&amp;objRef=iC12ED54445264C6796833B12B83EB83A&amp;type=report&amp;prompt=false&amp;drillFormLabel=drillForm1563375311111&amp;action=run&amp;format=HTML&amp;cmProperties%5Bid%5D=iC12ED54445264C6796833B12B83EB83A&amp;cmProperties%5BdefaultName%5D=College+Graduation+Rate+Report&amp;cmProperties%5Btype%5D=report&amp;cmProperties%5Bpermissions%5D%5B%5D=execute&amp;cmProperties%5Bpermissions%5D%5B%5D=read&amp;cmProperties%5Bpermissions%5D%5B%5D=traverse                                                                                                                                                                                                                                                                                                                                                                                                       http://intra.dev.edcs7.csc.gov.on.ca:82/uat1111/bi/?perspective=classicviewer&amp;pathRef=.public_folders%2FCGRT+Project%2FReports%2FCollege+Graduation+Rate+Report&amp;id=iC12ED54445264C6796833B12B83EB83A&amp;objRef=iC12ED54445264C6796833B12B83EB83A&amp;type=report&amp;prompt=false&amp;drillFormLabel=drillForm1563375604210&amp;action=run&amp;format=HTML&amp;cmProperties%5Bid%5D=iC12ED54445264C6796833B12B83EB83A&amp;cmProperties%5BdefaultName%5D=College+Graduation+Rate+Report&amp;cmProperties%5Btype%5D=report&amp;cmProperties%5Bpermissions%5D%5B%5D=execute&amp;cmProperties%5Bpermissions%5D%5B%5D=read&amp;cmProperties%5Bpermissions%5D%5B%5D=traverse                                                                                                                                                                                                                                                                                                                                                                                                   http://intra.dev.edcs7.csc.gov.on.ca:82/uat1111/bi/?perspective=classicviewer&amp;pathRef=.public_folders%2FCGRT+Project%2FReports%2FCollege+Incomplete+Rate+Report&amp;id=i77708950B2C3418A878B67CC809B30C4&amp;objRef=i77708950B2C3418A878B67CC809B30C4&amp;type=report&amp;prompt=false&amp;drillFormLabel=drillForm1563375638525&amp;action=run&amp;format=HTML&amp;cmProperties%5Bid%5D=i77708950B2C3418A878B67CC809B30C4&amp;cmProperties%5BdefaultName%5D=College+Incomplete+Rate+Report&amp;cmProperties%5Btype%5D=report&amp;cmProperties%5Bpermissions%5D%5B%5D=execute&amp;cmProperties%5Bpermissions%5D%5B%5D=read&amp;cmProperties%5Bpermissions%5D%5B%5D=traverse                                                                                                                                                                                http://intra.dev.edcs7.csc.gov.on.ca:82/uat1111/bi/?perspective=classicviewer&amp;pathRef=.public_folders%2FCGRT+Project%2FReports%2FCollege+Graduation+Rate+Report&amp;id=iC12ED54445264C6796833B12B83EB83A&amp;objRef=iC12ED54445264C6796833B12B83EB83A&amp;type=report&amp;prompt=false&amp;drillFormLabel=drillForm1563375614296&amp;action=run&amp;format=HTML&amp;cmProperties%5Bid%5D=iC12ED54445264C6796833B12B83EB83A&amp;cmProperties%5BdefaultName%5D=College+Graduation+Rate+Report&amp;cmProperties%5Btype%5D=report&amp;cmProperties%5Bpermissions%5D%5B%5D=execute&amp;cmProperties%5Bpermissions%5D%5B%5D=read&amp;cmProperties%5Bpermissions%5D%5B%5D=traverse                                                                                                                                                                                                                                                                                                                                                                                                        http://intra.dev.edcs7.csc.gov.on.ca:82/uat1111/bi/?perspective=classicviewer&amp;pathRef=.public_folders%2FCGRT+Project%2FReports%2FExclusions+Report&amp;id=i4CBEEE004D2845418EB14D7B05A836EE&amp;objRef=i4CBEEE004D2845418EB14D7B05A836EE&amp;type=report&amp;prompt=false&amp;drillFormLabel=drillForm1563375641080&amp;action=run&amp;format=HTML&amp;cmProperties%5Bid%5D=i4CBEEE004D2845418EB14D7B05A836EE&amp;cmProperties%5BdefaultName%5D=Exclusions+Report&amp;cmProperties%5Btype%5D=report&amp;cmProperties%5Bpermissions%5D%5B%5D=execute&amp;cmProperties%5Bpermissions%5D%5B%5D=read&amp;cmProperties%5Bpermissions%5D%5B%5D=traverse                                        http://intra.dev.edcs7.csc.gov.on.ca:82/uat1111/bi/?perspective=classicviewer&amp;id=iA1E86DF277984E8583016BDAE5180892&amp;isViewer=false&amp;isNewFromModule=false&amp;isNewFromPackage=false&amp;isNewDataSetFromModule=false&amp;isNewDataSetFromPackage=false&amp;isTemplate=false&amp;isDataset=false&amp;UIProfile=Titan&amp;cmProperties%5Bid%5D=iA1E86DF277984E8583016BDAE5180892&amp;cmProperties%5BdefaultName%5D=CGRT+Prompt+Page+Template+Report&amp;cmProperties%5Btype%5D=report&amp;cmProperties%5Bpermissions%5D%5B%5D=execute&amp;cmProperties%5Bpermissions%5D%5B%5D=read&amp;cmProperties%5Bpermissions%5D%5B%5D=traverse&amp;rsFinalRunOptions%5Bformat%5D=HTML&amp;rsFinalRunOptions%5Ba11y%5D=true&amp;rsFinalRunOptions%5Bbidi%5D=false&amp;rsFinalRunOptions%5BrunInAdvancedViewer%5D=false&amp;rsFinalRunOptions%5BDownload%5D=false&amp;rsFinalRunOptions%5Bprompt%5D=true&amp;rsFinalRunOptions%5BisApplication%5D=false                      http://intra.dev.edcs7.csc.gov.on.ca:82/uat1111/bi/?perspective=classicviewer&amp;id=i8164CD2759274482A7907BB25C194718  &amp;isViewer=false&amp;isNewFromModule=false&amp;isNewFromPackage=false&amp;isNewDataSetFromModule=false&amp;isNewDataSetFromPackage=false&amp;isTemplate=false&amp;isDataset=false&amp;UIProfile=Titan&amp;cmProperties%5Bid%5D=i8164CD2759274482A7907BB25C194718&amp;cmProperties%5BdefaultName%5D=Template+TAB4_CGRT&amp;cmProperties%5Btype%5D=report&amp;cmProperties%5Bpermissions%5D%5B%5D=execute&amp;cmProperties%5Bpermissions%5D%5B%5D=read&amp;cmProperties%5Bpermissions%5D%5B%5D=traverse&amp;cmProperties%5Bpermissions%5D%5B%5D=write&amp;rsFinalRunOptions%5Bformat%5D=HTML&amp;rsFinalRunOptions%5Ba11y%5D=true&amp;rsFinalRunOptions%5Bbidi%5D=false&amp;rsFinalRunOptions%5BrunInAdvancedViewer%5D=false&amp;rsFinalRunOptions%5BDownload%5D=false&amp;rsFinalRunOptions%5Bprompt%5D=true&amp;rsFinalRunOptions%5BisApplication%5D=false                                                                                                                                   </t>
-  </si>
-  <si>
-    <t>Ensures &lt;meta name="viewport"&gt; does not disable text scaling and zooming</t>
-  </si>
-  <si>
-    <t>http://intra.dev.edcs7.csc.gov.on.ca:82/uat1111/bi/?perspective=classicviewer&amp;id=iBED499536FAD473C8A83A8C9EC9356DF&amp;isViewer=false&amp;isNewFromModule=false&amp;isNewFromPackage=false&amp;isNewDataSetFromModule=false&amp;isNewDataSetFromPackage=false&amp;isTemplate=false&amp;isDataset=false&amp;UIProfile=Titan&amp;cmProperties%5Bid%5D=iBED499536FAD473C8A83A8C9EC9356DF&amp;cmProperties%5BdefaultName%5D=CGRT_Main_Menu&amp;cmProperties%5Btype%5D=report&amp;cmProperties%5Bpermissions%5D%5B%5D=execute&amp;cmProperties%5Bpermissions%5D%5B%5D=read&amp;cmProperties%5Bpermissions%5D%5B%5D=traverse&amp;rsFinalRunOptions%5Bformat%5D=HTML&amp;rsFinalRunOptions%5Ba11y%5D=true&amp;rsFinalRunOptions%5Bbidi%5D=false&amp;rsFinalRunOptions%5BrunInAdvancedViewer%5D=false&amp;rsFinalRunOptions%5BDownload%5D=false&amp;rsFinalRunOptions%5Bprompt%5D=true&amp;rsFinalRunOptions%5BisApplication%5D=false                                                                                                                                                                                                                                                                                                                                                                                       http://intra.dev.edcs7.csc.gov.on.ca:82/uat1111/bi/?perspective=classicviewer&amp;pathRef=.public_folders%2FCGRT+Project%2FReports%2FTAB_Reports%2FCGRT101+-+TAB+1%3A+Students+Eligible+for+General+Purpose+Grant+Funding&amp;id=i0914B5B236D246229C7C4B073E67F472&amp;objRef=i0914B5B236D246229C7C4B073E67F472&amp;type=report&amp;prompt=&amp;drillFormLabel=drillForm1563377505708&amp;action=run&amp;format=HTML&amp;cmProperties%5Bid%5D=i0914B5B236D246229C7C4B073E67F472&amp;cmProperties%5BdefaultName%5D=CGRT101+-+TAB+1%3A+Students+Eligible+for+General+Purpose+Grant+Funding&amp;cmProperties%5Btype%5D=report&amp;cmProperties%5Bpermissions%5D%5B%5D=execute&amp;cmProperties%5Bpermissions%5D%5B%5D=read&amp;cmProperties%5Bpermissions%5D%5B%5D=traverse                                           http://intra.dev.edcs7.csc.gov.on.ca:82/uat1111/bi/?perspective=classicviewer&amp;pathRef=.public_folders%2FCGRT+Project%2FReports%2FTAB_Reports%2FCGRT102+-+TAB+2%3A+Students+Funded+Through+the+Second+Career+Initiative&amp;id=i8F2579D71F2F435697AA2CA0E834A46E&amp;objRef=i8F2579D71F2F435697AA2CA0E834A46E&amp;type=report&amp;prompt=&amp;drillFormLabel=drillForm1563377639806&amp;action=run&amp;format=HTML&amp;cmProperties%5Bid%5D=i8F2579D71F2F435697AA2CA0E834A46E&amp;cmProperties%5BdefaultName%5D=CGRT102+-+TAB+2%3A+Students+Funded+Through+the+Second+Career+Initiative&amp;cmProperties%5Btype%5D=report&amp;cmProperties%5Bpermissions%5D%5B%5D=execute&amp;cmProperties%5Bpermissions%5D%5B%5D=read&amp;cmProperties%5Bpermissions%5D%5B%5D=traverse                                                                                                                                                                                                                                                                                                                        http://intra.dev.edcs7.csc.gov.on.ca:82/uat1111/bi/?perspective=classicviewer&amp;pathRef=.public_folders%2FCGRT+Project%2FReports%2FTAB_Reports%2FCGRT104+-+TAB+4%3A+International+Students&amp;id=i8967F506D93C4AF78EDAE0308BC1F784&amp;objRef=i8967F506D93C4AF78EDAE0308BC1F784&amp;type=report&amp;prompt=&amp;drillFormLabel=drillForm1563377642329&amp;action=run&amp;format=HTML&amp;cmProperties%5Bid%5D=i8967F506D93C4AF78EDAE0308BC1F784&amp;cmProperties%5BdefaultName%5D=CGRT104+-+TAB+4%3A+International+Students&amp;cmProperties%5Btype%5D=report&amp;cmProperties%5Bpermissions%5D%5B%5D=execute&amp;cmProperties%5Bpermissions%5D%5B%5D=read&amp;cmProperties%5Bpermissions%5D%5B%5D=traverse                                                                                                          http://intra.dev.edcs7.csc.gov.on.ca:82/uat1111/bi/?perspective=classicviewer&amp;pathRef=.public_folders%2FCGRT+Project%2FReports%2FCollege+Graduation+Rate+Report&amp;id=iC12ED54445264C6796833B12B83EB83A&amp;objRef=iC12ED54445264C6796833B12B83EB83A&amp;type=report&amp;prompt=false&amp;drillFormLabel=drillForm1563377657241&amp;action=run&amp;format=HTML&amp;cmProperties%5Bid%5D=iC12ED54445264C6796833B12B83EB83A&amp;cmProperties%5BdefaultName%5D=College+Graduation+Rate+Report&amp;cmProperties%5Btype%5D=report&amp;cmProperties%5Bpermissions%5D%5B%5D=execute&amp;cmProperties%5Bpermissions%5D%5B%5D=read&amp;cmProperties%5Bpermissions%5D%5B%5D=traverse                                                                                                                                                                                                                                                                                                                                                                                               http://intra.dev.edcs7.csc.gov.on.ca:82/uat1111/bi/?perspective=classicviewer&amp;id=i8164CD2759274482A7907BB25C194718&amp;isViewer=false&amp;isNewFromModule=false&amp;isNewFromPackage=false&amp;isNewDataSetFromModule=false&amp;isNewDataSetFromPackage=false&amp;isTemplate=false&amp;isDataset=false&amp;UIProfile=Titan&amp;cmProperties%5Bid%5D=i8164CD2759274482A7907BB25C194718&amp;cmProperties%5BdefaultName%5D=Template+TAB4_CGRT&amp;cmProperties%5Btype%5D=report&amp;cmProperties%5Bpermissions%5D%5B%5D=execute&amp;cmProperties%5Bpermissions%5D%5B%5D=read&amp;cmProperties%5Bpermissions%5D%5B%5D=traverse&amp;cmProperties%5Bpermissions%5D%5B%5D=write&amp;rsFinalRunOptions%5Bformat%5D=HTML&amp;rsFinalRunOptions%5Ba11y%5D=true&amp;rsFinalRunOptions%5Bbidi%5D=false&amp;rsFinalRunOptions%5BrunInAdvancedViewer%5D=false&amp;rsFinalRunOptions%5BDownload%5D=false&amp;rsFinalRunOptions%5Bprompt%5D=true&amp;rsFinalRunOptions%5BisApplication%5D=false      http://intra.dev.edcs7.csc.gov.on.ca:82/uat1111/bi/?perspective=classicviewer&amp;id=i50BE89F36FE54165B4E6E1D6E697D591&amp;isViewer=false&amp;isNewFromModule=false&amp;isNewFromPackage=false&amp;isNewDataSetFromModule=false&amp;isNewDataSetFromPackage=false&amp;isTemplate=false&amp;isDataset=false&amp;UIProfile=Titan&amp;cmProperties%5Bid%5D=i50BE89F36FE54165B4E6E1D6E697D591&amp;cmProperties%5BdefaultName%5D=Help+Page&amp;cmProperties%5Btype%5D=report&amp;cmProperties%5Bpermissions%5D%5B%5D=execute&amp;cmProperties%5Bpermissions%5D%5B%5D=read&amp;cmProperties%5Bpermissions%5D%5B%5D=traverse&amp;rsFinalRunOptions%5Bformat%5D=HTML&amp;rsFinalRunOptions%5Ba11y%5D=true&amp;rsFinalRunOptions%5Bbidi%5D=false&amp;rsFinalRunOptions%5BrunInAdvancedViewer%5D=false&amp;rsFinalRunOptions%5BDownload%5D=false&amp;rsFinalRunOptions%5Bprompt%5D=true&amp;rsFinalRunOptions%5BisApplication%5D=false                                                                         http://intra.dev.edcs7.csc.gov.on.ca:82/uat1111/bi/?perspective=classicviewer&amp;id=i4CBEEE004D2845418EB14D7B05A836EE&amp;isViewer=false&amp;isNewFromModule=false&amp;isNewFromPackage=false&amp;isNewDataSetFromModule=false&amp;isNewDataSetFromPackage=false&amp;isTemplate=false&amp;isDataset=false&amp;UIProfile=Titan&amp;cmProperties%5Bid%5D=i4CBEEE004D2845418EB14D7B05A836EE&amp;cmProperties%5BdefaultName%5D=Exclusions+Report&amp;cmProperties%5Btype%5D=report&amp;cmProperties%5Bpermissions%5D%5B%5D=execute&amp;cmProperties%5Bpermissions%5D%5B%5D=read&amp;cmProperties%5Bpermissions%5D%5B%5D=traverse&amp;rsFinalRunOptions%5Bformat%5D=HTML&amp;rsFinalRunOptions%5Ba11y%5D=true&amp;rsFinalRunOptions%5Bbidi%5D=false&amp;rsFinalRunOptions%5BrunInAdvancedViewer%5D=false&amp;rsFinalRunOptions%5BDownload%5D=false&amp;rsFinalRunOptions%5Bprompt%5D=true&amp;rsFinalRunOptions%5BisApplication%5D=false                                                                                                                                                                                                                                                                                                                                                                                   http://intra.dev.edcs7.csc.gov.on.ca:82/uat1111/bi/?perspective=classicviewer&amp;id=iA1E86DF277984E8583016BDAE5180892&amp;isViewer=false&amp;isNewFromModule=false&amp;isNewFromPackage=false&amp;isNewDataSetFromModule=false&amp;isNewDataSetFromPackage=false&amp;isTemplate=false&amp;isDataset=false&amp;UIProfile=Titan&amp;cmProperties%5Bid%5D=iA1E86DF277984E8583016BDAE5180892&amp;cmProperties%5BdefaultName%5D=CGRT+Prompt+Page+Template+Report&amp;cmProperties%5Btype%5D=report&amp;cmProperties%5Bpermissions%5D%5B%5D=execute&amp;cmProperties%5Bpermissions%5D%5B%5D=read&amp;cmProperties%5Bpermissions%5D%5B%5D=traverse&amp;rsFinalRunOptions%5Bformat%5D=HTML&amp;rsFinalRunOptions%5Ba11y%5D=true&amp;rsFinalRunOptions%5Bbidi%5D=false&amp;rsFinalRunOptions%5BrunInAdvancedViewer%5D=false&amp;rsFinalRunOptions%5BDownload%5D=false&amp;rsFinalRunOptions%5Bprompt%5D=true&amp;rsFinalRunOptions%5BisApplication%5D=false</t>
-  </si>
-  <si>
-    <t>Ensures &lt;iframe&gt; and &lt;frame&gt; elements contain a non-empty title attribute</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://intra.dev.edcs7.csc.gov.on.ca:82/uat1111/bi/?perspective=classicviewer&amp;id=iBED499536FAD473C8A83A8C9EC9356DF&amp;isViewer=false&amp;isNewFromModule=false&amp;isNewFromPackage=false&amp;isNewDataSetFromModule=false&amp;isNewDataSetFromPackage=false&amp;isTemplate=false&amp;isDataset=false&amp;UIProfile=Titan&amp;cmProperties%5Bid%5D=iBED499536FAD473C8A83A8C9EC9356DF&amp;cmProperties%5BdefaultName%5D=CGRT_Main_Menu&amp;cmProperties%5Btype%5D=report&amp;cmProperties%5Bpermissions%5D%5B%5D=execute&amp;cmProperties%5Bpermissions%5D%5B%5D=read&amp;cmProperties%5Bpermissions%5D%5B%5D=traverse&amp;rsFinalRunOptions%5Bformat%5D=HTML&amp;rsFinalRunOptions%5Ba11y%5D=true&amp;rsFinalRunOptions%5Bbidi%5D=false&amp;rsFinalRunOptions%5BrunInAdvancedViewer%5D=false&amp;rsFinalRunOptions%5BDownload%5D=false&amp;rsFinalRunOptions%5Bprompt%5D=true&amp;rsFinalRunOptions%5BisApplication%5D=false                                                                                                                                                                                                                                                                                                                                                                                          http://intra.dev.edcs7.csc.gov.on.ca:82/uat1111/bi/?perspective=classicviewer&amp;pathRef=.public_folders%2FCGRT+Project%2FReports%2FTAB_Reports%2FCGRT101+-+TAB+1%3A+Students+Eligible+for+General+Purpose+Grant+Funding&amp;id=i0914B5B236D246229C7C4B073E67F472&amp;objRef=i0914B5B236D246229C7C4B073E67F472&amp;type=report&amp;prompt=&amp;drillFormLabel=drillForm1563385180062&amp;action=run&amp;format=HTML&amp;cmProperties%5Bid%5D=i0914B5B236D246229C7C4B073E67F472&amp;cmProperties%5BdefaultName%5D=CGRT101+-+TAB+1%3A+Students+Eligible+for+General+Purpose+Grant+Funding&amp;cmProperties%5Btype%5D=report&amp;cmProperties%5Bpermissions%5D%5B%5D=execute&amp;cmProperties%5Bpermissions%5D%5B%5D=read&amp;cmProperties%5Bpermissions%5D%5B%5D=traverse            http://intra.dev.edcs7.csc.gov.on.ca:82/uat1111/bi/?perspective=classicviewer&amp;pathRef=.public_folders%2FCGRT+Project%2FReports%2FTAB_Reports%2FCGRT102+-+TAB+2%3A+Students+Funded+Through+the+Second+Career+Initiative&amp;id=i8F2579D71F2F435697AA2CA0E834A46E&amp;objRef=i8F2579D71F2F435697AA2CA0E834A46E&amp;type=report&amp;prompt=&amp;drillFormLabel=drillForm1563385540749&amp;action=run&amp;format=HTML&amp;cmProperties%5Bid%5D=i8F2579D71F2F435697AA2CA0E834A46E&amp;cmProperties%5BdefaultName%5D=CGRT102+-+TAB+2%3A+Students+Funded+Through+the+Second+Career+Initiative&amp;cmProperties%5Btype%5D=report&amp;cmProperties%5Bpermissions%5D%5B%5D=execute&amp;cmProperties%5Bpermissions%5D%5B%5D=read&amp;cmProperties%5Bpermissions%5D%5B%5D=traverse                                                                                                                                                                                                                                                                                                                          http://intra.dev.edcs7.csc.gov.on.ca:82/uat1111/bi/?perspective=classicviewer&amp;pathRef=.public_folders%2FCGRT+Project%2FReports%2FTAB_Reports%2FCGRT104+-+TAB+4%3A+International+Students&amp;id=i8967F506D93C4AF78EDAE0308BC1F784&amp;objRef=i8967F506D93C4AF78EDAE0308BC1F784&amp;type=report&amp;prompt=&amp;drillFormLabel=drillForm1563385576519&amp;action=run&amp;format=HTML&amp;cmProperties%5Bid%5D=i8967F506D93C4AF78EDAE0308BC1F784&amp;cmProperties%5BdefaultName%5D=CGRT104+-+TAB+4%3A+International+Students&amp;cmProperties%5Btype%5D=report&amp;cmProperties%5Bpermissions%5D%5B%5D=execute&amp;cmProperties%5Bpermissions%5D%5B%5D=read&amp;cmProperties%5Bpermissions%5D%5B%5D=traverse                                                    http://intra.dev.edcs7.csc.gov.on.ca:82/uat1111/bi/v1/disp                                                                                                                                                                                                                                                                                                                                     http://intra.dev.edcs7.csc.gov.on.ca:82/uat1111/bi/?perspective=classicviewer&amp;pathRef=.public_folders%2FCGRT+Project%2FReports%2FCollege+Graduation+Rate+Report&amp;id=iC12ED54445264C6796833B12B83EB83A&amp;objRef=iC12ED54445264C6796833B12B83EB83A&amp;type=report&amp;prompt=false&amp;drillFormLabel=drillForm1563385651881&amp;action=run&amp;format=HTML&amp;cmProperties%5Bid%5D=iC12ED54445264C6796833B12B83EB83A&amp;cmProperties%5BdefaultName%5D=College+Graduation+Rate+Report&amp;cmProperties%5Btype%5D=report&amp;cmProperties%5Bpermissions%5D%5B%5D=execute&amp;cmProperties%5Bpermissions%5D%5B%5D=read&amp;cmProperties%5Bpermissions%5D%5B%5D=traverse                                                                                                                                                                                                                                                                                                                                                                                                    http://intra.dev.edcs7.csc.gov.on.ca:82/uat1111/bi/?perspective=classicviewer&amp;id=iE3D324C33DAB46EF9426451D040C6161&amp;isViewer=false&amp;isNewFromModule=false&amp;isNewFromPackage=false&amp;isNewDataSetFromModule=false&amp;isNewDataSetFromPackage=false&amp;isTemplate=false&amp;isDataset=false&amp;UIProfile=Titan&amp;cmProperties%5Bid%5D=iE3D324C33DAB46EF9426451D040C6161&amp;cmProperties%5BdefaultName%5D=Template+TAB1_CGRT&amp;cmProperties%5Btype%5D=report&amp;cmProperties%5Bpermissions%5D%5B%5D=execute&amp;cmProperties%5Bpermissions%5D%5B%5D=read&amp;cmProperties%5Bpermissions%5D%5B%5D=traverse&amp;cmProperties%5Bpermissions%5D%5B%5D=write&amp;rsFinalRunOptions%5Bformat%5D=HTML&amp;rsFinalRunOptions%5Ba11y%5D=true&amp;rsFinalRunOptions%5Bbidi%5D=false&amp;rsFinalRunOptions%5BrunInAdvancedViewer%5D=false&amp;rsFinalRunOptions%5BDownload%5D=false&amp;rsFinalRunOptions%5Bprompt%5D=true&amp;rsFinalRunOptions%5BisApplication%5D=false http://intra.dev.edcs7.csc.gov.on.ca:82/uat1111/bi/?perspective=classicviewer&amp;id=i432FE3420E4347059D217CCACCEDCC28&amp;isViewer=false&amp;isNewFromModule=false&amp;isNewFromPackage=false&amp;isNewDataSetFromModule=false&amp;isNewDataSetFromPackage=false&amp;isTemplate=false&amp;isDataset=false&amp;UIProfile=Titan&amp;cmProperties%5Bid%5D=i432FE3420E4347059D217CCACCEDCC28&amp;cmProperties%5BdefaultName%5D=Template+TAB2_CGRT&amp;cmProperties%5Btype%5D=report&amp;cmProperties%5Bpermissions%5D%5B%5D=execute&amp;cmProperties%5Bpermissions%5D%5B%5D=read&amp;cmProperties%5Bpermissions%5D%5B%5D=traverse&amp;cmProperties%5Bpermissions%5D%5B%5D=write&amp;rsFinalRunOptions%5Bformat%5D=HTML&amp;rsFinalRunOptions%5Ba11y%5D=true&amp;rsFinalRunOptions%5Bbidi%5D=false&amp;rsFinalRunOptions%5BrunInAdvancedViewer%5D=false&amp;rsFinalRunOptions%5BDownload%5D=false&amp;rsFinalRunOptions%5Bprompt%5D=true&amp;rsFinalRunOptions%5BisApplication%5D=false    http://intra.dev.edcs7.csc.gov.on.ca:82/uat1111/bi/?perspective=classicviewer&amp;id=i8164CD2759274482A7907BB25C194718&amp;isViewer=false&amp;isNewFromModule=false&amp;isNewFromPackage=false&amp;isNewDataSetFromModule=false&amp;isNewDataSetFromPackage=false&amp;isTemplate=false&amp;isDataset=false&amp;UIProfile=Titan&amp;cmProperties%5Bid%5D=i8164CD2759274482A7907BB25C194718&amp;cmProperties%5BdefaultName%5D=Template+TAB4_CGRT&amp;cmProperties%5Btype%5D=report&amp;cmProperties%5Bpermissions%5D%5B%5D=execute&amp;cmProperties%5Bpermissions%5D%5B%5D=read&amp;cmProperties%5Bpermissions%5D%5B%5D=traverse&amp;cmProperties%5Bpermissions%5D%5B%5D=write&amp;rsFinalRunOptions%5Bformat%5D=HTML&amp;rsFinalRunOptions%5Ba11y%5D=true&amp;rsFinalRunOptions%5Bbidi%5D=false&amp;rsFinalRunOptions%5BrunInAdvancedViewer%5D=false&amp;rsFinalRunOptions%5BDownload%5D=false&amp;rsFinalRunOptions%5Bprompt%5D=true&amp;rsFinalRunOptions%5BisApplication%5D=falsehttp://intra.dev.edcs7.csc.gov.on.ca:82/uat1111/bi/?perspective=classicviewer&amp;id=i50BE89F36FE54165B4E6E1D6E697D591&amp;isViewer=false&amp;isNewFromModule=false&amp;isNewFromPackage=false&amp;isNewDataSetFromModule=false&amp;isNewDataSetFromPackage=false&amp;isTemplate=false&amp;isDataset=false&amp;UIProfile=Titan&amp;cmProperties%5Bid%5D=i50BE89F36FE54165B4E6E1D6E697D591&amp;cmProperties%5BdefaultName%5D=Help+Page&amp;cmProperties%5Btype%5D=report&amp;cmProperties%5Bpermissions%5D%5B%5D=execute&amp;cmProperties%5Bpermissions%5D%5B%5D=read&amp;cmProperties%5Bpermissions%5D%5B%5D=traverse&amp;rsFinalRunOptions%5Bformat%5D=HTML&amp;rsFinalRunOptions%5Ba11y%5D=true&amp;rsFinalRunOptions%5Bbidi%5D=false&amp;rsFinalRunOptions%5BrunInAdvancedViewer%5D=false&amp;rsFinalRunOptions%5BDownload%5D=false&amp;rsFinalRunOptions%5Bprompt%5D=true&amp;rsFinalRunOptions%5BisApplication%5D=false                                                                  http://intra.dev.edcs7.csc.gov.on.ca:82/uat1111/bi/?perspective=classicviewer&amp;id=i4CBEEE004D2845418EB14D7B05A836EE&amp;isViewer=false&amp;isNewFromModule=false&amp;isNewFromPackage=false&amp;isNewDataSetFromModule=false&amp;isNewDataSetFromPackage=false&amp;isTemplate=false&amp;isDataset=false&amp;UIProfile=Titan&amp;cmProperties%5Bid%5D=i4CBEEE004D2845418EB14D7B05A836EE&amp;cmProperties%5BdefaultName%5D=Exclusions+Report&amp;cmProperties%5Btype%5D=report&amp;cmProperties%5Bpermissions%5D%5B%5D=execute&amp;cmProperties%5Bpermissions%5D%5B%5D=read&amp;cmProperties%5Bpermissions%5D%5B%5D=traverse&amp;rsFinalRunOptions%5Bformat%5D=HTML&amp;rsFinalRunOptions%5Ba11y%5D=true&amp;rsFinalRunOptions%5Bbidi%5D=false&amp;rsFinalRunOptions%5BrunInAdvancedViewer%5D=false&amp;rsFinalRunOptions%5BDownload%5D=false&amp;rsFinalRunOptions%5Bprompt%5D=true&amp;rsFinalRunOptions%5BisApplication%5D=false                                                                                                                                                                                                                                                                                                                                                                                         http://intra.dev.edcs7.csc.gov.on.ca:82/uat1111/bi/?perspective=classicviewer&amp;id=i77708950B2C3418A878B67CC809B30C4&amp;isViewer=false&amp;isNewFromModule=false&amp;isNewFromPackage=false&amp;isNewDataSetFromModule=false&amp;isNewDataSetFromPackage=false&amp;isTemplate=false&amp;isDataset=false&amp;UIProfile=Titan&amp;cmProperties%5Bid%5D=i77708950B2C3418A878B67CC809B30C4&amp;cmProperties%5BdefaultName%5D=College+Incomplete+Rate+Report&amp;cmProperties%5Btype%5D=report&amp;cmProperties%5Bpermissions%5D%5B%5D=execute&amp;cmProperties%5Bpermissions%5D%5B%5D=read&amp;cmProperties%5Bpermissions%5D%5B%5D=traverse&amp;rsFinalRunOptions%5Bformat%5D=HTML&amp;rsFinalRunOptions%5Ba11y%5D=true&amp;rsFinalRunOptions%5Bbidi%5D=false&amp;rsFinalRunOptions%5BrunInAdvancedViewer%5D=false&amp;rsFinalRunOptions%5BDownload%5D=false&amp;rsFinalRunOptions%5Bprompt%5D=true&amp;rsFinalRunOptions%5BisApplication%5D=false                                              http://intra.dev.edcs7.csc.gov.on.ca:82/uat1111/bi/?perspective=classicviewer&amp;id=iA1E86DF277984E8583016BDAE5180892&amp;isViewer=false&amp;isNewFromModule=false&amp;isNewFromPackage=false&amp;isNewDataSetFromModule=false&amp;isNewDataSetFromPackage=false&amp;isTemplate=false&amp;isDataset=false&amp;UIProfile=Titan&amp;cmProperties%5Bid%5D=iA1E86DF277984E8583016BDAE5180892&amp;cmProperties%5BdefaultName%5D=CGRT+Prompt+Page+Template+Report&amp;cmProperties%5Btype%5D=report&amp;cmProperties%5Bpermissions%5D%5B%5D=execute&amp;cmProperties%5Bpermissions%5D%5B%5D=read&amp;cmProperties%5Bpermissions%5D%5B%5D=traverse&amp;rsFinalRunOptions%5Bformat%5D=HTML&amp;rsFinalRunOptions%5Ba11y%5D=true&amp;rsFinalRunOptions%5Bbidi%5D=false&amp;rsFinalRunOptions%5BrunInAdvancedViewer%5D=false&amp;rsFinalRunOptions%5BDownload%5D=false&amp;rsFinalRunOptions%5Bprompt%5D=true&amp;rsFinalRunOptions%5BisApplication%5D=false      </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Ensures the contrast between foreground and background colors meets WCAG 2 AA contrast ratio thresholds</t>
-  </si>
-  <si>
-    <t>http://intra.dev.edcs7.csc.gov.on.ca:82/uat1111/bi/?perspective=classicviewer&amp;pathRef=.public_folders%2FCGRT+Project%2FReports%2FTAB_Reports%2FCGRT101+-+TAB+1%3A+Students+Eligible+for+General+Purpose+Grant+Funding&amp;id=i0914B5B236D246229C7C4B073E67F472&amp;objRef=i0914B5B236D246229C7C4B073E67F472&amp;type=report&amp;prompt=&amp;drillFormLabel=drillForm1563385180062&amp;action=run&amp;format=HTML&amp;cmProperties%5Bid%5D=i0914B5B236D246229C7C4B073E67F472&amp;cmProperties%5BdefaultName%5D=CGRT101+-+TAB+1%3A+Students+Eligible+for+General+Purpose+Grant+Funding&amp;cmProperties%5Btype%5D=report&amp;cmProperties%5Bpermissions%5D%5B%5D=execute&amp;cmProperties%5Bpermissions%5D%5B%5D=read&amp;cmProperties%5Bpermissions%5D%5B%5D=traverse       http://intra.dev.edcs7.csc.gov.on.ca:82/uat1111/bi/?perspective=classicviewer&amp;pathRef=.public_folders%2FCGRT+Project%2FReports%2FTAB_Reports%2FCGRT102+-+TAB+2%3A+Students+Funded+Through+the+Second+Career+Initiative&amp;id=i8F2579D71F2F435697AA2CA0E834A46E&amp;objRef=i8F2579D71F2F435697AA2CA0E834A46E&amp;type=report&amp;prompt=&amp;drillFormLabel=drillForm1563385540749&amp;action=run&amp;format=HTML&amp;cmProperties%5Bid%5D=i8F2579D71F2F435697AA2CA0E834A46E&amp;cmProperties%5BdefaultName%5D=CGRT102+-+TAB+2%3A+Students+Funded+Through+the+Second+Career+Initiative&amp;cmProperties%5Btype%5D=report&amp;cmProperties%5Bpermissions%5D%5B%5D=execute&amp;cmProperties%5Bpermissions%5D%5B%5D=read&amp;cmProperties%5Bpermissions%5D%5B%5D=traverse                                                                                                                                                                                                                                                                                                                                   http://intra.dev.edcs7.csc.gov.on.ca:82/uat1111/bi/?perspective=classicviewer&amp;pathRef=.public_folders%2FCGRT+Project%2FReports%2FTAB_Reports%2FCGRT103+-+TAB+3%3A+Students+Funded+Through+the+CODA+Initiative&amp;id=i3EBFDEF6023F4989A5891FE79B830254&amp;objRef=i3EBFDEF6023F4989A5891FE79B830254&amp;type=report&amp;prompt=&amp;drillFormLabel=drillForm1563386928831&amp;action=run&amp;format=HTML&amp;cmProperties%5Bid%5D=i3EBFDEF6023F4989A5891FE79B830254&amp;cmProperties%5BdefaultName%5D=CGRT103+-+TAB+3%3A+Students+Funded+Through+the+CODA+Initiative&amp;cmProperties%5Btype%5D=report&amp;cmProperties%5Bpermissions%5D%5B%5D=execute&amp;cmProperties%5Bpermissions%5D%5B%5D=read&amp;cmProperties%5Bpermissions%5D%5B%5D=traverse     http://intra.dev.edcs7.csc.gov.on.ca:82/uat1111/bi/?perspective=classicviewer&amp;pathRef=.public_folders%2FCGRT+Project%2FReports%2FTAB_Reports%2FCGRT104+-+TAB+4%3A+International+Students&amp;id=i8967F506D93C4AF78EDAE0308BC1F784&amp;objRef=i8967F506D93C4AF78EDAE0308BC1F784&amp;type=report&amp;prompt=&amp;drillFormLabel=drillForm1563386931077&amp;action=run&amp;format=HTML&amp;cmProperties%5Bid%5D=i8967F506D93C4AF78EDAE0308BC1F784&amp;cmProperties%5BdefaultName%5D=CGRT104+-+TAB+4%3A+International+Students&amp;cmProperties%5Btype%5D=report&amp;cmProperties%5Bpermissions%5D%5B%5D=execute&amp;cmProperties%5Bpermissions%5D%5B%5D=read&amp;cmProperties%5Bpermissions%5D%5B%5D=traverse</t>
-  </si>
-  <si>
     <t>Doesn’t ensure &lt;meta name="viewport"&gt; does not disable text scaling and zooming</t>
   </si>
   <si>
@@ -2372,9 +2321,6 @@
   </si>
   <si>
     <t>Defect ID: 545 1.1.1 AODA - CGRT - PDF of Tab Report does not meet accessibility standard</t>
-  </si>
-  <si>
-    <t>Medium</t>
   </si>
   <si>
     <t>Methods and Tools :</t>
@@ -3752,121 +3698,22 @@
       <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="12" fillId="5" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="27" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -3909,6 +3756,105 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="27" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="12" fillId="5" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="2" borderId="25" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -5787,7 +5733,7 @@
   <sheetData>
     <row r="1" spans="1:7" s="60" customFormat="1" ht="63.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="63" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B1" s="64"/>
       <c r="C1" s="58"/>
@@ -5798,7 +5744,7 @@
     </row>
     <row r="2" spans="1:7" s="60" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A2" s="74" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B2" s="131"/>
       <c r="C2" s="58"/>
@@ -5809,7 +5755,7 @@
     </row>
     <row r="3" spans="1:7" s="74" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="71" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B3" s="72"/>
       <c r="C3" s="73"/>
@@ -5820,7 +5766,7 @@
     </row>
     <row r="4" spans="1:7" s="74" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="71" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B4" s="72"/>
       <c r="C4" s="73"/>
@@ -5831,7 +5777,7 @@
     </row>
     <row r="5" spans="1:7" s="74" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A5" s="130" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B5" s="72"/>
       <c r="C5" s="73"/>
@@ -5842,7 +5788,7 @@
     </row>
     <row r="6" spans="1:7" s="74" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="75" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B6" s="72"/>
       <c r="C6" s="73"/>
@@ -5853,7 +5799,7 @@
     </row>
     <row r="7" spans="1:7" s="74" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="76" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B7" s="72"/>
       <c r="C7" s="73"/>
@@ -5873,7 +5819,7 @@
     </row>
     <row r="9" spans="1:7" s="74" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A9" s="77" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B9" s="72"/>
       <c r="C9" s="73"/>
@@ -5884,7 +5830,7 @@
     </row>
     <row r="10" spans="1:7" s="74" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="76" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B10" s="72"/>
       <c r="C10" s="73"/>
@@ -5895,7 +5841,7 @@
     </row>
     <row r="11" spans="1:7" s="74" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="78" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B11" s="72"/>
       <c r="C11" s="73"/>
@@ -5906,7 +5852,7 @@
     </row>
     <row r="12" spans="1:7" s="74" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="79" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B12" s="72"/>
       <c r="C12" s="73"/>
@@ -5917,7 +5863,7 @@
     </row>
     <row r="13" spans="1:7" s="74" customFormat="1" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="76" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B13" s="72"/>
       <c r="C13" s="73"/>
@@ -5928,7 +5874,7 @@
     </row>
     <row r="14" spans="1:7" s="74" customFormat="1" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="76" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B14" s="72"/>
       <c r="C14" s="73"/>
@@ -5939,7 +5885,7 @@
     </row>
     <row r="15" spans="1:7" s="74" customFormat="1" ht="25.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="85" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B15" s="72"/>
       <c r="C15" s="73"/>
@@ -5950,19 +5896,19 @@
     </row>
     <row r="16" spans="1:7" s="61" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="65" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B16" s="66"/>
     </row>
     <row r="17" spans="1:7" s="80" customFormat="1" ht="22.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="77" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B17" s="72"/>
     </row>
     <row r="18" spans="1:7" s="74" customFormat="1" ht="24.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="76" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B18" s="72"/>
       <c r="C18" s="73"/>
@@ -5973,7 +5919,7 @@
     </row>
     <row r="19" spans="1:7" s="74" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="76" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B19" s="72"/>
       <c r="C19" s="73"/>
@@ -5984,7 +5930,7 @@
     </row>
     <row r="20" spans="1:7" s="128" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="76" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B20" s="126"/>
       <c r="C20" s="127"/>
@@ -5995,7 +5941,7 @@
     </row>
     <row r="21" spans="1:7" s="74" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="76" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B21" s="72"/>
       <c r="C21" s="73"/>
@@ -6015,7 +5961,7 @@
     </row>
     <row r="23" spans="1:7" s="74" customFormat="1" ht="24.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="77" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B23" s="72"/>
       <c r="C23" s="73"/>
@@ -6026,7 +5972,7 @@
     </row>
     <row r="24" spans="1:7" s="74" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="76" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B24" s="72"/>
       <c r="C24" s="73"/>
@@ -6037,7 +5983,7 @@
     </row>
     <row r="25" spans="1:7" s="74" customFormat="1" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="76" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B25" s="72"/>
       <c r="C25" s="73"/>
@@ -6048,7 +5994,7 @@
     </row>
     <row r="26" spans="1:7" s="74" customFormat="1" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="76" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B26" s="72"/>
       <c r="C26" s="73"/>
@@ -6059,7 +6005,7 @@
     </row>
     <row r="27" spans="1:7" s="74" customFormat="1" ht="31.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="85" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B27" s="72"/>
       <c r="C27" s="73"/>
@@ -6070,19 +6016,19 @@
     </row>
     <row r="28" spans="1:7" s="61" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="65" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B28" s="66"/>
     </row>
     <row r="29" spans="1:7" s="61" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="67" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B29" s="68"/>
     </row>
     <row r="30" spans="1:7" s="74" customFormat="1" ht="22.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="77" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B30" s="72"/>
       <c r="C30" s="73"/>
@@ -6093,7 +6039,7 @@
     </row>
     <row r="31" spans="1:7" s="74" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="81" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B31" s="72"/>
       <c r="C31" s="73"/>
@@ -6104,7 +6050,7 @@
     </row>
     <row r="32" spans="1:7" s="74" customFormat="1" ht="97.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="86" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B32" s="72"/>
       <c r="C32" s="73"/>
@@ -6115,19 +6061,19 @@
     </row>
     <row r="33" spans="1:7" ht="64.150000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="122" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B33" s="62"/>
     </row>
     <row r="34" spans="1:7" s="61" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="67" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B34" s="69"/>
     </row>
     <row r="35" spans="1:7" s="74" customFormat="1" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="77" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B35" s="72"/>
       <c r="C35" s="73"/>
@@ -6138,7 +6084,7 @@
     </row>
     <row r="36" spans="1:7" s="74" customFormat="1" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="77" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B36" s="72"/>
       <c r="C36" s="73"/>
@@ -6149,7 +6095,7 @@
     </row>
     <row r="37" spans="1:7" s="74" customFormat="1" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="77" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B37" s="72"/>
       <c r="C37" s="73"/>
@@ -6160,7 +6106,7 @@
     </row>
     <row r="38" spans="1:7" s="74" customFormat="1" ht="33.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="81" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B38" s="72"/>
       <c r="C38" s="73"/>
@@ -6171,7 +6117,7 @@
     </row>
     <row r="39" spans="1:7" s="74" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="86" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B39" s="72"/>
       <c r="C39" s="73"/>
@@ -6182,7 +6128,7 @@
     </row>
     <row r="40" spans="1:7" s="74" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="129" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B40" s="72"/>
       <c r="C40" s="73"/>
@@ -6193,13 +6139,13 @@
     </row>
     <row r="41" spans="1:7" s="61" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="67" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B41" s="69"/>
     </row>
     <row r="42" spans="1:7" s="74" customFormat="1" ht="22.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="77" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B42" s="72"/>
       <c r="C42" s="73"/>
@@ -6210,7 +6156,7 @@
     </row>
     <row r="43" spans="1:7" s="74" customFormat="1" ht="25.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="77" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B43" s="72"/>
       <c r="C43" s="73"/>
@@ -6221,7 +6167,7 @@
     </row>
     <row r="44" spans="1:7" s="74" customFormat="1" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="75" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B44" s="72"/>
       <c r="C44" s="73"/>
@@ -6232,7 +6178,7 @@
     </row>
     <row r="45" spans="1:7" s="74" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A45" s="75" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B45" s="72"/>
       <c r="C45" s="73"/>
@@ -6243,7 +6189,7 @@
     </row>
     <row r="46" spans="1:7" s="74" customFormat="1" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A46" s="82" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B46" s="83"/>
       <c r="C46" s="73"/>
@@ -6254,7 +6200,7 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" s="84" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2"/>
@@ -6306,7 +6252,7 @@
   <sheetData>
     <row r="1" spans="1:252" s="50" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="121" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B1" s="46"/>
       <c r="C1" s="46"/>
@@ -6339,7 +6285,7 @@
     </row>
     <row r="3" spans="1:252" s="54" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="87" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B3" s="53" t="e">
         <f>COUNTIF('[3]WCAG 2.0 Compliance Checklist'!D13:D56,"Criteria not applicable")</f>
@@ -6598,7 +6544,7 @@
     </row>
     <row r="4" spans="1:252" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="90" t="s">
-        <v>261</v>
+        <v>243</v>
       </c>
       <c r="B4" s="55"/>
       <c r="C4" s="55"/>
@@ -6611,7 +6557,7 @@
     </row>
     <row r="5" spans="1:252" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="88" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B5" s="51"/>
       <c r="C5" s="51"/>
@@ -6623,7 +6569,7 @@
     </row>
     <row r="6" spans="1:252" s="54" customFormat="1" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="87" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B6" s="53"/>
       <c r="C6" s="53"/>
@@ -6879,7 +6825,7 @@
     </row>
     <row r="7" spans="1:252" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="90" t="s">
-        <v>262</v>
+        <v>244</v>
       </c>
       <c r="B7" s="55"/>
       <c r="C7" s="55"/>
@@ -6892,7 +6838,7 @@
     </row>
     <row r="8" spans="1:252" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="88" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B8" s="51"/>
       <c r="C8" s="51"/>
@@ -6904,7 +6850,7 @@
     </row>
     <row r="9" spans="1:252" s="54" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="87" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B9" s="53"/>
       <c r="C9" s="53"/>
@@ -7160,7 +7106,7 @@
     </row>
     <row r="10" spans="1:252" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="90" t="s">
-        <v>269</v>
+        <v>251</v>
       </c>
       <c r="B10" s="55"/>
       <c r="C10" s="55"/>
@@ -7173,7 +7119,7 @@
     </row>
     <row r="11" spans="1:252" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="88" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B11" s="51"/>
       <c r="C11" s="51"/>
@@ -7185,7 +7131,7 @@
     </row>
     <row r="12" spans="1:252" s="54" customFormat="1" ht="37.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="89" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B12" s="56"/>
       <c r="C12" s="56"/>
@@ -7441,7 +7387,7 @@
     </row>
     <row r="13" spans="1:252" ht="366.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="90" t="s">
-        <v>267</v>
+        <v>249</v>
       </c>
       <c r="B13" s="55"/>
       <c r="C13" s="55"/>
@@ -7454,7 +7400,7 @@
     </row>
     <row r="14" spans="1:252" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="88" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B14" s="51"/>
       <c r="C14" s="51"/>
@@ -7466,7 +7412,7 @@
     </row>
     <row r="15" spans="1:252" s="54" customFormat="1" ht="34.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="89" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B15" s="56"/>
       <c r="C15" s="56"/>
@@ -7722,7 +7668,7 @@
     </row>
     <row r="16" spans="1:252" ht="171" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="90" t="s">
-        <v>268</v>
+        <v>250</v>
       </c>
       <c r="B16" s="55"/>
       <c r="C16" s="55"/>
@@ -7735,7 +7681,7 @@
     </row>
     <row r="17" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="88" t="s">
-        <v>254</v>
+        <v>236</v>
       </c>
       <c r="B17" s="51"/>
       <c r="C17" s="51"/>
@@ -7747,7 +7693,7 @@
     </row>
     <row r="18" spans="1:9" ht="50.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="89" t="s">
-        <v>255</v>
+        <v>237</v>
       </c>
       <c r="B18" s="55"/>
       <c r="C18" s="55"/>
@@ -7760,7 +7706,7 @@
     </row>
     <row r="19" spans="1:9" ht="348" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="90" t="s">
-        <v>266</v>
+        <v>248</v>
       </c>
       <c r="B19" s="51"/>
       <c r="C19" s="51"/>
@@ -7772,7 +7718,7 @@
     </row>
     <row r="20" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="88" t="s">
-        <v>256</v>
+        <v>238</v>
       </c>
       <c r="B20" s="55"/>
       <c r="C20" s="55"/>
@@ -7785,32 +7731,32 @@
     </row>
     <row r="21" spans="1:9" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="90" t="s">
-        <v>265</v>
+        <v>247</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="88" t="s">
-        <v>257</v>
+        <v>239</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="90" t="s">
-        <v>264</v>
+        <v>246</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="156" t="s">
-        <v>263</v>
+        <v>245</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="88" t="s">
-        <v>258</v>
+        <v>240</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="90" t="s">
-        <v>259</v>
+        <v>241</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="170.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -7818,7 +7764,7 @@
     </row>
     <row r="28" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="88" t="s">
-        <v>260</v>
+        <v>242</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
@@ -7829,7 +7775,7 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="158" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
   </sheetData>
@@ -7850,7 +7796,7 @@
   </sheetPr>
   <dimension ref="A1:XFC81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="115" zoomScalePageLayoutView="160" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="115" zoomScalePageLayoutView="160" workbookViewId="0">
       <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
@@ -7876,16 +7822,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="13" customFormat="1" ht="37.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="177" t="s">
-        <v>226</v>
-      </c>
-      <c r="B1" s="177"/>
-      <c r="C1" s="177"/>
-      <c r="D1" s="177"/>
-      <c r="E1" s="177"/>
-      <c r="F1" s="177"/>
-      <c r="G1" s="177"/>
-      <c r="H1" s="178"/>
+      <c r="A1" s="184" t="s">
+        <v>225</v>
+      </c>
+      <c r="B1" s="184"/>
+      <c r="C1" s="184"/>
+      <c r="D1" s="184"/>
+      <c r="E1" s="184"/>
+      <c r="F1" s="184"/>
+      <c r="G1" s="184"/>
+      <c r="H1" s="185"/>
       <c r="I1" s="11"/>
       <c r="J1" s="12"/>
       <c r="K1" s="1"/>
@@ -7899,13 +7845,13 @@
       <c r="S1" s="1"/>
     </row>
     <row r="2" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="179" t="s">
+      <c r="A2" s="165" t="s">
         <v>61</v>
       </c>
-      <c r="B2" s="179"/>
-      <c r="C2" s="180"/>
-      <c r="D2" s="180"/>
-      <c r="E2" s="181"/>
+      <c r="B2" s="165"/>
+      <c r="C2" s="188"/>
+      <c r="D2" s="188"/>
+      <c r="E2" s="189"/>
       <c r="F2" s="39"/>
       <c r="G2" s="1"/>
       <c r="H2" s="16"/>
@@ -7917,13 +7863,13 @@
       <c r="N2" s="13"/>
     </row>
     <row r="3" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="179" t="s">
+      <c r="A3" s="165" t="s">
         <v>63</v>
       </c>
-      <c r="B3" s="179"/>
-      <c r="C3" s="194"/>
-      <c r="D3" s="195"/>
-      <c r="E3" s="196"/>
+      <c r="B3" s="165"/>
+      <c r="C3" s="201"/>
+      <c r="D3" s="202"/>
+      <c r="E3" s="203"/>
       <c r="F3" s="39"/>
       <c r="G3" s="1"/>
       <c r="H3" s="16"/>
@@ -7935,12 +7881,12 @@
       <c r="N3" s="13"/>
     </row>
     <row r="4" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="179" t="s">
-        <v>78</v>
-      </c>
-      <c r="B4" s="179"/>
-      <c r="C4" s="160"/>
-      <c r="D4" s="160"/>
+      <c r="A4" s="165" t="s">
+        <v>77</v>
+      </c>
+      <c r="B4" s="165"/>
+      <c r="C4" s="211"/>
+      <c r="D4" s="211"/>
       <c r="E4" s="91"/>
       <c r="F4" s="39"/>
       <c r="G4" s="1"/>
@@ -7953,13 +7899,13 @@
       <c r="N4" s="13"/>
     </row>
     <row r="5" spans="1:19" ht="27" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="161" t="s">
-        <v>79</v>
-      </c>
-      <c r="B5" s="161"/>
-      <c r="C5" s="162"/>
-      <c r="D5" s="162"/>
-      <c r="E5" s="163"/>
+      <c r="A5" s="164" t="s">
+        <v>78</v>
+      </c>
+      <c r="B5" s="164"/>
+      <c r="C5" s="212"/>
+      <c r="D5" s="212"/>
+      <c r="E5" s="213"/>
       <c r="F5" s="39"/>
       <c r="G5" s="1"/>
       <c r="H5" s="16"/>
@@ -7971,13 +7917,13 @@
       <c r="N5" s="13"/>
     </row>
     <row r="6" spans="1:19" ht="27" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="161" t="s">
-        <v>80</v>
-      </c>
-      <c r="B6" s="161"/>
-      <c r="C6" s="164"/>
-      <c r="D6" s="164"/>
-      <c r="E6" s="165"/>
+      <c r="A6" s="164" t="s">
+        <v>79</v>
+      </c>
+      <c r="B6" s="164"/>
+      <c r="C6" s="162"/>
+      <c r="D6" s="162"/>
+      <c r="E6" s="163"/>
       <c r="F6" s="39"/>
       <c r="G6" s="1"/>
       <c r="H6" s="16"/>
@@ -7989,13 +7935,13 @@
       <c r="N6" s="13"/>
     </row>
     <row r="7" spans="1:19" ht="27" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="161" t="s">
-        <v>81</v>
-      </c>
-      <c r="B7" s="161"/>
-      <c r="C7" s="164"/>
-      <c r="D7" s="164"/>
-      <c r="E7" s="165"/>
+      <c r="A7" s="164" t="s">
+        <v>80</v>
+      </c>
+      <c r="B7" s="164"/>
+      <c r="C7" s="162"/>
+      <c r="D7" s="162"/>
+      <c r="E7" s="163"/>
       <c r="F7" s="39"/>
       <c r="G7" s="1"/>
       <c r="H7" s="16"/>
@@ -8007,13 +7953,13 @@
       <c r="N7" s="13"/>
     </row>
     <row r="8" spans="1:19" ht="27" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="161" t="s">
-        <v>82</v>
-      </c>
-      <c r="B8" s="161"/>
-      <c r="C8" s="164"/>
-      <c r="D8" s="164"/>
-      <c r="E8" s="165"/>
+      <c r="A8" s="164" t="s">
+        <v>81</v>
+      </c>
+      <c r="B8" s="164"/>
+      <c r="C8" s="162"/>
+      <c r="D8" s="162"/>
+      <c r="E8" s="163"/>
       <c r="F8" s="39"/>
       <c r="G8" s="1"/>
       <c r="H8" s="16"/>
@@ -8025,16 +7971,16 @@
       <c r="N8" s="13"/>
     </row>
     <row r="9" spans="1:19" s="37" customFormat="1" ht="52.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="183" t="s">
+      <c r="A9" s="192" t="s">
         <v>76</v>
       </c>
-      <c r="B9" s="184"/>
-      <c r="C9" s="184"/>
-      <c r="D9" s="184"/>
-      <c r="E9" s="184"/>
-      <c r="F9" s="184"/>
-      <c r="G9" s="184"/>
-      <c r="H9" s="184"/>
+      <c r="B9" s="193"/>
+      <c r="C9" s="193"/>
+      <c r="D9" s="193"/>
+      <c r="E9" s="193"/>
+      <c r="F9" s="193"/>
+      <c r="G9" s="193"/>
+      <c r="H9" s="193"/>
       <c r="I9" s="18"/>
       <c r="J9" s="18"/>
       <c r="K9" s="18"/>
@@ -8044,16 +7990,16 @@
       <c r="Q9" s="108"/>
     </row>
     <row r="10" spans="1:19" s="22" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="185" t="s">
-        <v>211</v>
-      </c>
-      <c r="B10" s="186"/>
-      <c r="C10" s="186"/>
-      <c r="D10" s="186"/>
-      <c r="E10" s="186"/>
-      <c r="F10" s="186"/>
-      <c r="G10" s="186"/>
-      <c r="H10" s="187"/>
+      <c r="A10" s="194" t="s">
+        <v>210</v>
+      </c>
+      <c r="B10" s="195"/>
+      <c r="C10" s="195"/>
+      <c r="D10" s="195"/>
+      <c r="E10" s="195"/>
+      <c r="F10" s="195"/>
+      <c r="G10" s="195"/>
+      <c r="H10" s="196"/>
       <c r="I10" s="21"/>
       <c r="J10" s="21"/>
       <c r="K10" s="21"/>
@@ -8063,23 +8009,23 @@
       <c r="Q10" s="23"/>
     </row>
     <row r="11" spans="1:19" ht="55.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="192" t="s">
+      <c r="A11" s="199" t="s">
         <v>54</v>
       </c>
-      <c r="B11" s="193"/>
+      <c r="B11" s="200"/>
       <c r="C11" s="123" t="s">
         <v>40</v>
       </c>
       <c r="D11" s="123" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E11" s="123" t="s">
-        <v>100</v>
-      </c>
-      <c r="F11" s="188" t="s">
+        <v>99</v>
+      </c>
+      <c r="F11" s="198" t="s">
         <v>52</v>
       </c>
-      <c r="G11" s="188"/>
+      <c r="G11" s="198"/>
       <c r="H11" s="124" t="s">
         <v>53</v>
       </c>
@@ -8091,18 +8037,18 @@
       <c r="N11" s="13"/>
     </row>
     <row r="12" spans="1:19" ht="69.599999999999994" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="171" t="s">
-        <v>84</v>
-      </c>
-      <c r="B12" s="182"/>
-      <c r="C12" s="189" t="s">
-        <v>180</v>
-      </c>
-      <c r="D12" s="190"/>
-      <c r="E12" s="190"/>
-      <c r="F12" s="190"/>
-      <c r="G12" s="190"/>
-      <c r="H12" s="191"/>
+      <c r="A12" s="190" t="s">
+        <v>83</v>
+      </c>
+      <c r="B12" s="191"/>
+      <c r="C12" s="181" t="s">
+        <v>179</v>
+      </c>
+      <c r="D12" s="182"/>
+      <c r="E12" s="182"/>
+      <c r="F12" s="182"/>
+      <c r="G12" s="182"/>
+      <c r="H12" s="183"/>
       <c r="I12" s="13"/>
       <c r="J12" s="13"/>
       <c r="K12" s="13"/>
@@ -8169,7 +8115,7 @@
         <v>2</v>
       </c>
       <c r="B15" s="93" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C15" s="94"/>
       <c r="D15" s="95"/>
@@ -8277,7 +8223,7 @@
         <v>6</v>
       </c>
       <c r="B19" s="93" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C19" s="94"/>
       <c r="D19" s="95"/>
@@ -8298,7 +8244,7 @@
       <c r="M19" s="100"/>
       <c r="N19" s="100"/>
       <c r="Q19" s="102" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="20" spans="1:17" s="101" customFormat="1" ht="49.9" customHeight="1" x14ac:dyDescent="0.2">
@@ -8306,7 +8252,7 @@
         <v>7</v>
       </c>
       <c r="B20" s="93" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C20" s="94"/>
       <c r="D20" s="95"/>
@@ -8327,7 +8273,7 @@
       <c r="M20" s="100"/>
       <c r="N20" s="100"/>
       <c r="Q20" s="102" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="21" spans="1:17" s="101" customFormat="1" ht="49.9" customHeight="1" x14ac:dyDescent="0.2">
@@ -8335,7 +8281,7 @@
         <v>8</v>
       </c>
       <c r="B21" s="93" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C21" s="94"/>
       <c r="D21" s="95"/>
@@ -8356,7 +8302,7 @@
       <c r="M21" s="100"/>
       <c r="N21" s="100"/>
       <c r="Q21" s="102" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="22" spans="1:17" s="101" customFormat="1" ht="49.9" customHeight="1" x14ac:dyDescent="0.2">
@@ -8385,7 +8331,7 @@
       <c r="M22" s="100"/>
       <c r="N22" s="100"/>
       <c r="Q22" s="102" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="23" spans="1:17" s="101" customFormat="1" ht="60" x14ac:dyDescent="0.2">
@@ -8393,7 +8339,7 @@
         <v>10</v>
       </c>
       <c r="B23" s="93" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C23" s="94"/>
       <c r="D23" s="95"/>
@@ -8420,7 +8366,7 @@
         <v>11</v>
       </c>
       <c r="B24" s="103" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C24" s="94"/>
       <c r="D24" s="95"/>
@@ -8449,7 +8395,7 @@
         <v>12</v>
       </c>
       <c r="B25" s="93" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C25" s="94"/>
       <c r="D25" s="95"/>
@@ -8476,7 +8422,7 @@
         <v>13</v>
       </c>
       <c r="B26" s="104" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C26" s="94"/>
       <c r="D26" s="95"/>
@@ -8499,14 +8445,14 @@
       <c r="Q26" s="102"/>
     </row>
     <row r="27" spans="1:17" ht="17.45" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="175" t="s">
+      <c r="A27" s="186" t="s">
         <v>67</v>
       </c>
-      <c r="B27" s="176"/>
-      <c r="C27" s="176"/>
-      <c r="D27" s="176"/>
-      <c r="E27" s="176"/>
-      <c r="F27" s="176"/>
+      <c r="B27" s="187"/>
+      <c r="C27" s="187"/>
+      <c r="D27" s="187"/>
+      <c r="E27" s="187"/>
+      <c r="F27" s="187"/>
       <c r="G27" s="24">
         <f>SUM(H13:H26)</f>
         <v>0</v>
@@ -8523,18 +8469,18 @@
       <c r="N27" s="13"/>
     </row>
     <row r="28" spans="1:17" ht="53.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="171" t="s">
-        <v>85</v>
-      </c>
-      <c r="B28" s="172"/>
-      <c r="C28" s="189" t="s">
-        <v>186</v>
-      </c>
-      <c r="D28" s="190"/>
-      <c r="E28" s="190"/>
-      <c r="F28" s="190"/>
-      <c r="G28" s="190"/>
-      <c r="H28" s="191"/>
+      <c r="A28" s="190" t="s">
+        <v>84</v>
+      </c>
+      <c r="B28" s="197"/>
+      <c r="C28" s="181" t="s">
+        <v>185</v>
+      </c>
+      <c r="D28" s="182"/>
+      <c r="E28" s="182"/>
+      <c r="F28" s="182"/>
+      <c r="G28" s="182"/>
+      <c r="H28" s="183"/>
       <c r="I28" s="13"/>
       <c r="J28" s="13"/>
       <c r="K28" s="13"/>
@@ -8574,7 +8520,7 @@
         <v>15</v>
       </c>
       <c r="B30" s="93" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C30" s="94"/>
       <c r="D30" s="95"/>
@@ -8628,7 +8574,7 @@
         <v>17</v>
       </c>
       <c r="B32" s="93" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C32" s="94"/>
       <c r="D32" s="95"/>
@@ -8652,7 +8598,7 @@
         <v>18</v>
       </c>
       <c r="B33" s="93" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C33" s="94"/>
       <c r="D33" s="95"/>
@@ -8679,7 +8625,7 @@
         <v>19</v>
       </c>
       <c r="B34" s="93" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C34" s="94"/>
       <c r="D34" s="95"/>
@@ -8706,7 +8652,7 @@
         <v>20</v>
       </c>
       <c r="B35" s="93" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C35" s="94"/>
       <c r="D35" s="95"/>
@@ -8733,7 +8679,7 @@
         <v>21</v>
       </c>
       <c r="B36" s="93" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C36" s="94"/>
       <c r="D36" s="95"/>
@@ -8787,7 +8733,7 @@
         <v>23</v>
       </c>
       <c r="B38" s="93" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C38" s="94"/>
       <c r="D38" s="95"/>
@@ -8814,7 +8760,7 @@
         <v>24</v>
       </c>
       <c r="B39" s="93" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C39" s="94"/>
       <c r="D39" s="95"/>
@@ -8864,14 +8810,14 @@
       <c r="Q40" s="102"/>
     </row>
     <row r="41" spans="1:17" ht="48.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="175" t="s">
+      <c r="A41" s="186" t="s">
         <v>66</v>
       </c>
-      <c r="B41" s="176"/>
-      <c r="C41" s="176"/>
-      <c r="D41" s="176"/>
-      <c r="E41" s="176"/>
-      <c r="F41" s="176"/>
+      <c r="B41" s="187"/>
+      <c r="C41" s="187"/>
+      <c r="D41" s="187"/>
+      <c r="E41" s="187"/>
+      <c r="F41" s="187"/>
       <c r="G41" s="24">
         <f>SUM(H29:H40)</f>
         <v>0</v>
@@ -8888,18 +8834,18 @@
       <c r="N41" s="13"/>
     </row>
     <row r="42" spans="1:17" ht="54.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="171" t="s">
-        <v>86</v>
-      </c>
-      <c r="B42" s="172"/>
-      <c r="C42" s="189" t="s">
-        <v>191</v>
-      </c>
-      <c r="D42" s="190"/>
-      <c r="E42" s="190"/>
-      <c r="F42" s="190"/>
-      <c r="G42" s="190"/>
-      <c r="H42" s="191"/>
+      <c r="A42" s="190" t="s">
+        <v>85</v>
+      </c>
+      <c r="B42" s="197"/>
+      <c r="C42" s="181" t="s">
+        <v>190</v>
+      </c>
+      <c r="D42" s="182"/>
+      <c r="E42" s="182"/>
+      <c r="F42" s="182"/>
+      <c r="G42" s="182"/>
+      <c r="H42" s="183"/>
       <c r="I42" s="13"/>
       <c r="J42" s="13"/>
       <c r="K42" s="13"/>
@@ -8912,7 +8858,7 @@
         <v>26</v>
       </c>
       <c r="B43" s="93" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C43" s="94"/>
       <c r="D43" s="95"/>
@@ -8966,7 +8912,7 @@
         <v>28</v>
       </c>
       <c r="B45" s="93" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C45" s="94"/>
       <c r="D45" s="95"/>
@@ -8993,7 +8939,7 @@
         <v>29</v>
       </c>
       <c r="B46" s="93" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C46" s="94"/>
       <c r="D46" s="95"/>
@@ -9020,7 +8966,7 @@
         <v>30</v>
       </c>
       <c r="B47" s="93" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C47" s="94"/>
       <c r="D47" s="95"/>
@@ -9047,7 +8993,7 @@
         <v>31</v>
       </c>
       <c r="B48" s="93" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C48" s="94"/>
       <c r="D48" s="95"/>
@@ -9074,7 +9020,7 @@
         <v>32</v>
       </c>
       <c r="B49" s="93" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C49" s="94"/>
       <c r="D49" s="95"/>
@@ -9101,7 +9047,7 @@
         <v>33</v>
       </c>
       <c r="B50" s="93" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C50" s="94"/>
       <c r="D50" s="95"/>
@@ -9128,7 +9074,7 @@
         <v>34</v>
       </c>
       <c r="B51" s="93" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C51" s="94"/>
       <c r="D51" s="95"/>
@@ -9155,7 +9101,7 @@
         <v>35</v>
       </c>
       <c r="B52" s="93" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C52" s="94"/>
       <c r="D52" s="95"/>
@@ -9178,14 +9124,14 @@
       <c r="Q52" s="102"/>
     </row>
     <row r="53" spans="1:17" ht="74.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="175" t="s">
+      <c r="A53" s="186" t="s">
         <v>65</v>
       </c>
-      <c r="B53" s="176"/>
-      <c r="C53" s="176"/>
-      <c r="D53" s="176"/>
-      <c r="E53" s="176"/>
-      <c r="F53" s="176"/>
+      <c r="B53" s="187"/>
+      <c r="C53" s="187"/>
+      <c r="D53" s="187"/>
+      <c r="E53" s="187"/>
+      <c r="F53" s="187"/>
       <c r="G53" s="25">
         <f>SUM(H43:H52)</f>
         <v>0</v>
@@ -9202,18 +9148,18 @@
       <c r="N53" s="13"/>
     </row>
     <row r="54" spans="1:17" ht="47.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="169" t="s">
-        <v>87</v>
-      </c>
-      <c r="B54" s="170"/>
-      <c r="C54" s="166" t="s">
-        <v>197</v>
-      </c>
-      <c r="D54" s="167"/>
-      <c r="E54" s="167"/>
-      <c r="F54" s="167"/>
-      <c r="G54" s="167"/>
-      <c r="H54" s="168"/>
+      <c r="A54" s="207" t="s">
+        <v>86</v>
+      </c>
+      <c r="B54" s="208"/>
+      <c r="C54" s="204" t="s">
+        <v>196</v>
+      </c>
+      <c r="D54" s="205"/>
+      <c r="E54" s="205"/>
+      <c r="F54" s="205"/>
+      <c r="G54" s="205"/>
+      <c r="H54" s="206"/>
       <c r="I54" s="13"/>
       <c r="J54" s="13"/>
       <c r="K54" s="13"/>
@@ -9276,14 +9222,14 @@
       <c r="Q56" s="102"/>
     </row>
     <row r="57" spans="1:17" ht="43.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="175" t="s">
+      <c r="A57" s="186" t="s">
         <v>64</v>
       </c>
-      <c r="B57" s="176"/>
-      <c r="C57" s="176"/>
-      <c r="D57" s="176"/>
-      <c r="E57" s="176"/>
-      <c r="F57" s="176"/>
+      <c r="B57" s="187"/>
+      <c r="C57" s="187"/>
+      <c r="D57" s="187"/>
+      <c r="E57" s="187"/>
+      <c r="F57" s="187"/>
       <c r="G57" s="24">
         <f>SUM(H55:H56)</f>
         <v>0</v>
@@ -9300,16 +9246,16 @@
       <c r="N57" s="13"/>
     </row>
     <row r="58" spans="1:17" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="173" t="s">
-        <v>89</v>
-      </c>
-      <c r="B58" s="174"/>
-      <c r="C58" s="174"/>
-      <c r="D58" s="174"/>
-      <c r="E58" s="174"/>
-      <c r="F58" s="211"/>
-      <c r="G58" s="212"/>
-      <c r="H58" s="213"/>
+      <c r="A58" s="209" t="s">
+        <v>88</v>
+      </c>
+      <c r="B58" s="210"/>
+      <c r="C58" s="210"/>
+      <c r="D58" s="210"/>
+      <c r="E58" s="210"/>
+      <c r="F58" s="178"/>
+      <c r="G58" s="179"/>
+      <c r="H58" s="180"/>
       <c r="I58" s="13"/>
       <c r="J58" s="13"/>
       <c r="K58" s="13"/>
@@ -9318,14 +9264,14 @@
       <c r="N58" s="13"/>
     </row>
     <row r="59" spans="1:17" ht="24.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A59" s="201"/>
-      <c r="B59" s="202"/>
+      <c r="A59" s="168"/>
+      <c r="B59" s="169"/>
       <c r="C59" s="28"/>
-      <c r="D59" s="208" t="s">
-        <v>88</v>
-      </c>
-      <c r="E59" s="209"/>
-      <c r="F59" s="210"/>
+      <c r="D59" s="175" t="s">
+        <v>87</v>
+      </c>
+      <c r="E59" s="176"/>
+      <c r="F59" s="177"/>
       <c r="G59" s="29">
         <f>SUM(H13:H26)+SUM(H29:H40)+SUM(H43:H52)+SUM(H55:H56)</f>
         <v>0</v>
@@ -9339,13 +9285,13 @@
       <c r="N59" s="13"/>
     </row>
     <row r="60" spans="1:17" ht="48" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="203"/>
-      <c r="B60" s="204"/>
+      <c r="A60" s="170"/>
+      <c r="B60" s="171"/>
       <c r="C60" s="31"/>
-      <c r="D60" s="205" t="s">
+      <c r="D60" s="172" t="s">
         <v>55</v>
       </c>
-      <c r="E60" s="206"/>
+      <c r="E60" s="173"/>
       <c r="F60" s="32"/>
       <c r="G60" s="33"/>
       <c r="H60" s="34"/>
@@ -9357,13 +9303,13 @@
       <c r="N60" s="13"/>
     </row>
     <row r="61" spans="1:17" ht="55.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="203"/>
-      <c r="B61" s="204"/>
+      <c r="A61" s="170"/>
+      <c r="B61" s="171"/>
       <c r="C61" s="31"/>
-      <c r="D61" s="205" t="s">
+      <c r="D61" s="172" t="s">
         <v>56</v>
       </c>
-      <c r="E61" s="206"/>
+      <c r="E61" s="173"/>
       <c r="F61" s="32"/>
       <c r="G61" s="33"/>
       <c r="H61" s="34"/>
@@ -9375,13 +9321,13 @@
       <c r="N61" s="13"/>
     </row>
     <row r="62" spans="1:17" ht="39.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="203"/>
-      <c r="B62" s="204"/>
+      <c r="A62" s="170"/>
+      <c r="B62" s="171"/>
       <c r="C62" s="35"/>
-      <c r="D62" s="207" t="s">
+      <c r="D62" s="174" t="s">
         <v>57</v>
       </c>
-      <c r="E62" s="206"/>
+      <c r="E62" s="173"/>
       <c r="F62" s="32"/>
       <c r="G62" s="33"/>
       <c r="H62" s="34"/>
@@ -9400,11 +9346,11 @@
         <f>SUM(H13:H26)+SUM(H29:H40)+SUM(H43:H52)+SUM(H55:H56)</f>
         <v>0</v>
       </c>
-      <c r="E63" s="199" t="s">
-        <v>155</v>
-      </c>
-      <c r="F63" s="199"/>
-      <c r="G63" s="200"/>
+      <c r="E63" s="166" t="s">
+        <v>154</v>
+      </c>
+      <c r="F63" s="166"/>
+      <c r="G63" s="167"/>
       <c r="H63" s="43"/>
       <c r="I63" s="13"/>
       <c r="J63" s="13"/>
@@ -9414,10 +9360,10 @@
       <c r="N63" s="13"/>
     </row>
     <row r="64" spans="1:17" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="197" t="s">
+      <c r="A64" s="160" t="s">
         <v>58</v>
       </c>
-      <c r="B64" s="198"/>
+      <c r="B64" s="161"/>
       <c r="C64" s="18"/>
       <c r="D64" s="19"/>
       <c r="E64" s="44"/>
@@ -9469,7 +9415,7 @@
     </row>
     <row r="67" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A67" s="109" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B67" s="110"/>
       <c r="C67" s="107"/>
@@ -9491,6 +9437,33 @@
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
   <mergeCells count="43">
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="C54:H54"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="A58:E58"/>
+    <mergeCell ref="A57:F57"/>
+    <mergeCell ref="A53:F53"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A41:F41"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="A27:F27"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A9:H9"/>
+    <mergeCell ref="A10:H10"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="C12:H12"/>
+    <mergeCell ref="C28:H28"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="A7:B7"/>
     <mergeCell ref="A64:B64"/>
     <mergeCell ref="C7:E7"/>
     <mergeCell ref="A8:B8"/>
@@ -9507,33 +9480,6 @@
     <mergeCell ref="D59:F59"/>
     <mergeCell ref="F58:H58"/>
     <mergeCell ref="C42:H42"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A41:F41"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="A27:F27"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A9:H9"/>
-    <mergeCell ref="A10:H10"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="C12:H12"/>
-    <mergeCell ref="C28:H28"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="C54:H54"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="A58:E58"/>
-    <mergeCell ref="A57:F57"/>
-    <mergeCell ref="A53:F53"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:E6"/>
   </mergeCells>
   <conditionalFormatting sqref="F43:F52 F55:F56 F13:F26 F29:F40">
     <cfRule type="cellIs" dxfId="136" priority="371" operator="equal">
@@ -10066,7 +10012,7 @@
     </row>
     <row r="11" spans="1:1" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A11" s="123" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="12" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
@@ -10074,7 +10020,7 @@
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" s="144" t="s">
-        <v>252</v>
+        <v>235</v>
       </c>
     </row>
     <row r="14" spans="1:1" ht="15" hidden="1" x14ac:dyDescent="0.2">
@@ -10094,7 +10040,7 @@
     </row>
     <row r="19" spans="1:1" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A19" s="145" t="s">
-        <v>250</v>
+        <v>233</v>
       </c>
     </row>
     <row r="20" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
@@ -10111,12 +10057,12 @@
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" s="144" t="s">
-        <v>245</v>
+        <v>228</v>
       </c>
     </row>
     <row r="25" spans="1:1" ht="30" x14ac:dyDescent="0.2">
       <c r="A25" s="96" t="s">
-        <v>243</v>
+        <v>226</v>
       </c>
     </row>
     <row r="26" spans="1:1" ht="15" hidden="1" x14ac:dyDescent="0.2">
@@ -10145,7 +10091,7 @@
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" s="144" t="s">
-        <v>247</v>
+        <v>230</v>
       </c>
     </row>
     <row r="35" spans="1:1" ht="15" hidden="1" x14ac:dyDescent="0.2">
@@ -10156,7 +10102,7 @@
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" s="144" t="s">
-        <v>248</v>
+        <v>231</v>
       </c>
     </row>
     <row r="38" spans="1:1" ht="15" hidden="1" x14ac:dyDescent="0.2">
@@ -10164,7 +10110,7 @@
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" s="144" t="s">
-        <v>251</v>
+        <v>234</v>
       </c>
     </row>
     <row r="40" spans="1:1" ht="15" hidden="1" x14ac:dyDescent="0.2">
@@ -10178,7 +10124,7 @@
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" s="144" t="s">
-        <v>246</v>
+        <v>229</v>
       </c>
     </row>
     <row r="44" spans="1:1" ht="15" hidden="1" x14ac:dyDescent="0.2">
@@ -10216,12 +10162,12 @@
     </row>
     <row r="55" spans="1:1" ht="51" x14ac:dyDescent="0.2">
       <c r="A55" s="145" t="s">
-        <v>249</v>
+        <v>232</v>
       </c>
     </row>
     <row r="56" spans="1:1" ht="30" x14ac:dyDescent="0.2">
       <c r="A56" s="96" t="s">
-        <v>244</v>
+        <v>227</v>
       </c>
     </row>
     <row r="57" spans="1:1" hidden="1" x14ac:dyDescent="0.2">
@@ -10322,8 +10268,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:T43"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -10344,7 +10290,7 @@
   <sheetData>
     <row r="1" spans="1:20" s="8" customFormat="1" ht="25.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="215" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B1" s="216"/>
       <c r="C1" s="216"/>
@@ -10365,7 +10311,7 @@
     </row>
     <row r="2" spans="1:20" s="4" customFormat="1" ht="60.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="214" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B2" s="214"/>
       <c r="C2" s="214"/>
@@ -10381,7 +10327,7 @@
       <c r="M2" s="5"/>
       <c r="N2" s="6"/>
       <c r="O2" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="T2" s="5"/>
     </row>
@@ -10393,19 +10339,19 @@
         <v>74</v>
       </c>
       <c r="C3" s="112" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D3" s="112" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E3" s="112" t="s">
         <v>73</v>
       </c>
       <c r="F3" s="112" t="s">
+        <v>198</v>
+      </c>
+      <c r="G3" s="112" t="s">
         <v>199</v>
-      </c>
-      <c r="G3" s="112" t="s">
-        <v>200</v>
       </c>
       <c r="H3" s="112" t="s">
         <v>72</v>
@@ -10414,579 +10360,273 @@
         <v>71</v>
       </c>
       <c r="O3" s="113" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20" s="113" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="136">
-        <v>1</v>
-      </c>
-      <c r="B4" s="133">
-        <v>43658</v>
-      </c>
-      <c r="C4" s="142" t="s">
-        <v>228</v>
-      </c>
-      <c r="D4" s="137" t="s">
-        <v>104</v>
-      </c>
-      <c r="E4" s="138" t="s">
-        <v>229</v>
-      </c>
-      <c r="F4" s="139" t="s">
-        <v>140</v>
-      </c>
-      <c r="G4" s="140" t="s">
-        <v>70</v>
-      </c>
-      <c r="H4" s="141" t="s">
-        <v>227</v>
-      </c>
+        <v>101</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" s="113" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="136"/>
+      <c r="B4" s="133"/>
+      <c r="C4" s="142"/>
+      <c r="D4" s="137"/>
+      <c r="E4" s="138"/>
+      <c r="F4" s="139"/>
+      <c r="G4" s="140"/>
+      <c r="H4" s="141"/>
       <c r="L4" s="118" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="M4" s="113" t="s">
         <v>70</v>
       </c>
       <c r="O4" s="113" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" s="117" customFormat="1" ht="30.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="114">
-        <v>3</v>
-      </c>
-      <c r="B5" s="133">
-        <v>43658</v>
-      </c>
-      <c r="C5" s="143" t="s">
-        <v>231</v>
-      </c>
-      <c r="D5" s="116" t="s">
-        <v>101</v>
-      </c>
-      <c r="E5" s="132" t="s">
-        <v>230</v>
-      </c>
-      <c r="F5" s="134" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" s="117" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="114"/>
+      <c r="B5" s="133"/>
+      <c r="C5" s="143"/>
+      <c r="D5" s="116"/>
+      <c r="E5" s="132"/>
+      <c r="F5" s="134"/>
+      <c r="G5" s="135"/>
+      <c r="H5" s="141"/>
+      <c r="L5" s="119" t="s">
         <v>140</v>
-      </c>
-      <c r="G5" s="135" t="s">
-        <v>70</v>
-      </c>
-      <c r="H5" s="141" t="s">
-        <v>227</v>
-      </c>
-      <c r="L5" s="119" t="s">
-        <v>141</v>
       </c>
       <c r="M5" s="117" t="s">
         <v>69</v>
       </c>
       <c r="O5" s="117" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20" s="117" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A6" s="114">
-        <v>4</v>
-      </c>
-      <c r="B6" s="133">
-        <v>43658</v>
-      </c>
-      <c r="C6" s="143" t="s">
-        <v>231</v>
-      </c>
-      <c r="D6" s="116" t="s">
-        <v>114</v>
-      </c>
-      <c r="E6" s="116" t="s">
-        <v>232</v>
-      </c>
-      <c r="F6" s="134" t="s">
-        <v>140</v>
-      </c>
-      <c r="G6" s="135" t="s">
-        <v>70</v>
-      </c>
-      <c r="H6" s="135" t="s">
-        <v>227</v>
-      </c>
+        <v>135</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" s="117" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A6" s="114"/>
+      <c r="B6" s="133"/>
+      <c r="C6" s="143"/>
+      <c r="D6" s="116"/>
+      <c r="E6" s="116"/>
+      <c r="F6" s="134"/>
+      <c r="G6" s="135"/>
+      <c r="H6" s="135"/>
       <c r="M6" s="117" t="s">
         <v>68</v>
       </c>
       <c r="O6" s="117" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20" s="117" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A7" s="114">
-        <v>5</v>
-      </c>
-      <c r="B7" s="133">
-        <v>43658</v>
-      </c>
-      <c r="C7" s="143" t="s">
-        <v>234</v>
-      </c>
-      <c r="D7" s="116" t="s">
         <v>134</v>
       </c>
-      <c r="E7" s="116" t="s">
-        <v>233</v>
-      </c>
-      <c r="F7" s="134" t="s">
-        <v>140</v>
-      </c>
-      <c r="G7" s="135" t="s">
-        <v>70</v>
-      </c>
-      <c r="H7" s="135" t="s">
-        <v>227</v>
-      </c>
+    </row>
+    <row r="7" spans="1:20" s="117" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A7" s="114"/>
+      <c r="B7" s="133"/>
+      <c r="C7" s="143"/>
+      <c r="D7" s="116"/>
+      <c r="E7" s="116"/>
+      <c r="F7" s="134"/>
+      <c r="G7" s="135"/>
+      <c r="H7" s="135"/>
       <c r="O7" s="117" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="8" spans="1:20" s="117" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A8" s="114">
-        <v>6</v>
-      </c>
-      <c r="B8" s="133">
-        <v>43661</v>
-      </c>
-      <c r="C8" s="143" t="s">
-        <v>236</v>
-      </c>
-      <c r="D8" s="116" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" s="117" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A8" s="114"/>
+      <c r="B8" s="133"/>
+      <c r="C8" s="143"/>
+      <c r="D8" s="116"/>
+      <c r="E8" s="116"/>
+      <c r="F8" s="134"/>
+      <c r="G8" s="135"/>
+      <c r="H8" s="135"/>
+      <c r="O8" s="117" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" s="117" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A9" s="114"/>
+      <c r="B9" s="133"/>
+      <c r="C9" s="143"/>
+      <c r="D9" s="116"/>
+      <c r="E9" s="116"/>
+      <c r="F9" s="134"/>
+      <c r="G9" s="135"/>
+      <c r="H9" s="135"/>
+      <c r="O9" s="117" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" s="117" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A10" s="114"/>
+      <c r="B10" s="133"/>
+      <c r="C10" s="143"/>
+      <c r="D10" s="116"/>
+      <c r="E10" s="116"/>
+      <c r="F10" s="134"/>
+      <c r="G10" s="135"/>
+      <c r="H10" s="135"/>
+      <c r="O10" s="117" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" s="117" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A11" s="114"/>
+      <c r="B11" s="133"/>
+      <c r="C11" s="143"/>
+      <c r="D11" s="116"/>
+      <c r="E11" s="116"/>
+      <c r="F11" s="134"/>
+      <c r="G11" s="135"/>
+      <c r="H11" s="135"/>
+      <c r="O11" s="117" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" s="117" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A12" s="114"/>
+      <c r="B12" s="133"/>
+      <c r="C12" s="143"/>
+      <c r="D12" s="116"/>
+      <c r="E12" s="116"/>
+      <c r="F12" s="134"/>
+      <c r="G12" s="135"/>
+      <c r="H12" s="135"/>
+      <c r="O12" s="117" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" s="117" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A13" s="114"/>
+      <c r="B13" s="133"/>
+      <c r="C13" s="142"/>
+      <c r="D13" s="116"/>
+      <c r="E13" s="144"/>
+      <c r="F13" s="146"/>
+      <c r="G13" s="135"/>
+      <c r="H13" s="135"/>
+      <c r="O13" s="117" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" s="117" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A14" s="114"/>
+      <c r="B14" s="133"/>
+      <c r="C14" s="143"/>
+      <c r="D14" s="116"/>
+      <c r="E14" s="145"/>
+      <c r="F14" s="146"/>
+      <c r="G14" s="135"/>
+      <c r="H14" s="135"/>
+      <c r="O14" s="117" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" s="117" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A15" s="114"/>
+      <c r="B15" s="133"/>
+      <c r="C15" s="143"/>
+      <c r="D15" s="116"/>
+      <c r="E15" s="144"/>
+      <c r="F15" s="146"/>
+      <c r="G15" s="135"/>
+      <c r="H15" s="135"/>
+      <c r="O15" s="117" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" s="117" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A16" s="114"/>
+      <c r="B16" s="133"/>
+      <c r="C16" s="143"/>
+      <c r="D16" s="116"/>
+      <c r="E16" s="96"/>
+      <c r="F16" s="146"/>
+      <c r="G16" s="135"/>
+      <c r="H16" s="135"/>
+      <c r="O16" s="117" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" s="117" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A17" s="114"/>
+      <c r="B17" s="133"/>
+      <c r="C17" s="143"/>
+      <c r="D17" s="116"/>
+      <c r="E17" s="144"/>
+      <c r="F17" s="146"/>
+      <c r="G17" s="135"/>
+      <c r="H17" s="135"/>
+      <c r="O17" s="117" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" s="117" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A18" s="114"/>
+      <c r="B18" s="133"/>
+      <c r="C18" s="143"/>
+      <c r="D18" s="116"/>
+      <c r="E18" s="144"/>
+      <c r="F18" s="146"/>
+      <c r="G18" s="135"/>
+      <c r="H18" s="135"/>
+      <c r="O18" s="117" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" s="117" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A19" s="114"/>
+      <c r="B19" s="133"/>
+      <c r="C19" s="143"/>
+      <c r="D19" s="116"/>
+      <c r="E19" s="144"/>
+      <c r="F19" s="146"/>
+      <c r="G19" s="135"/>
+      <c r="H19" s="135"/>
+      <c r="O19" s="117" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" s="117" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A20" s="114"/>
+      <c r="B20" s="133"/>
+      <c r="C20" s="143"/>
+      <c r="D20" s="116"/>
+      <c r="E20" s="144"/>
+      <c r="F20" s="146"/>
+      <c r="G20" s="135"/>
+      <c r="H20" s="135"/>
+      <c r="O20" s="117" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" s="117" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A21" s="120"/>
+      <c r="B21" s="133"/>
+      <c r="C21" s="143"/>
+      <c r="D21" s="116"/>
+      <c r="E21" s="145"/>
+      <c r="F21" s="146"/>
+      <c r="G21" s="135"/>
+      <c r="H21" s="135"/>
+      <c r="O21" s="117" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" s="117" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A22" s="114"/>
+      <c r="B22" s="133"/>
+      <c r="C22" s="143"/>
+      <c r="D22" s="116"/>
+      <c r="E22" s="96"/>
+      <c r="F22" s="146"/>
+      <c r="G22" s="135"/>
+      <c r="H22" s="135"/>
+      <c r="O22" s="117" t="s">
         <v>118</v>
       </c>
-      <c r="E8" s="116" t="s">
-        <v>235</v>
-      </c>
-      <c r="F8" s="134" t="s">
-        <v>140</v>
-      </c>
-      <c r="G8" s="135" t="s">
-        <v>70</v>
-      </c>
-      <c r="H8" s="135" t="s">
-        <v>227</v>
-      </c>
-      <c r="O8" s="117" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20" s="117" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A9" s="114">
-        <v>7</v>
-      </c>
-      <c r="B9" s="133">
-        <v>43662</v>
-      </c>
-      <c r="C9" s="143" t="s">
-        <v>238</v>
-      </c>
-      <c r="D9" s="116" t="s">
-        <v>128</v>
-      </c>
-      <c r="E9" s="116" t="s">
-        <v>237</v>
-      </c>
-      <c r="F9" s="134" t="s">
-        <v>140</v>
-      </c>
-      <c r="G9" s="135" t="s">
-        <v>70</v>
-      </c>
-      <c r="H9" s="135" t="s">
-        <v>227</v>
-      </c>
-      <c r="O9" s="117" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="10" spans="1:20" s="117" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A10" s="114">
-        <v>8</v>
-      </c>
-      <c r="B10" s="133">
-        <v>43663</v>
-      </c>
-      <c r="C10" s="143" t="s">
-        <v>240</v>
-      </c>
-      <c r="D10" s="116" t="s">
-        <v>121</v>
-      </c>
-      <c r="E10" s="116" t="s">
-        <v>239</v>
-      </c>
-      <c r="F10" s="134" t="s">
-        <v>140</v>
-      </c>
-      <c r="G10" s="135" t="s">
-        <v>70</v>
-      </c>
-      <c r="H10" s="135" t="s">
-        <v>227</v>
-      </c>
-      <c r="O10" s="117" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20" s="117" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A11" s="114">
-        <v>9</v>
-      </c>
-      <c r="B11" s="133">
-        <v>43663</v>
-      </c>
-      <c r="C11" s="143" t="s">
-        <v>240</v>
-      </c>
-      <c r="D11" s="116" t="s">
-        <v>103</v>
-      </c>
-      <c r="E11" s="116" t="s">
-        <v>239</v>
-      </c>
-      <c r="F11" s="134" t="s">
-        <v>140</v>
-      </c>
-      <c r="G11" s="135" t="s">
-        <v>70</v>
-      </c>
-      <c r="H11" s="135" t="s">
-        <v>227</v>
-      </c>
-      <c r="O11" s="117" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="12" spans="1:20" s="117" customFormat="1" ht="45" x14ac:dyDescent="0.2">
-      <c r="A12" s="114">
-        <v>10</v>
-      </c>
-      <c r="B12" s="133">
-        <v>43663</v>
-      </c>
-      <c r="C12" s="143" t="s">
-        <v>242</v>
-      </c>
-      <c r="D12" s="116" t="s">
-        <v>129</v>
-      </c>
-      <c r="E12" s="116" t="s">
-        <v>241</v>
-      </c>
-      <c r="F12" s="134" t="s">
-        <v>140</v>
-      </c>
-      <c r="G12" s="135" t="s">
-        <v>70</v>
-      </c>
-      <c r="H12" s="135" t="s">
-        <v>227</v>
-      </c>
-      <c r="O12" s="117" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="13" spans="1:20" s="117" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A13" s="114">
-        <v>11</v>
-      </c>
-      <c r="B13" s="133">
-        <v>43663</v>
-      </c>
-      <c r="C13" s="142" t="s">
-        <v>228</v>
-      </c>
-      <c r="D13" s="116" t="s">
-        <v>101</v>
-      </c>
-      <c r="E13" s="144" t="s">
-        <v>252</v>
-      </c>
-      <c r="F13" s="146" t="s">
-        <v>253</v>
-      </c>
-      <c r="G13" s="135" t="s">
-        <v>70</v>
-      </c>
-      <c r="H13" s="135" t="s">
-        <v>227</v>
-      </c>
-      <c r="O13" s="117" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="14" spans="1:20" s="117" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
-      <c r="A14" s="114">
-        <v>12</v>
-      </c>
-      <c r="B14" s="133">
-        <v>43663</v>
-      </c>
-      <c r="C14" s="143" t="s">
-        <v>231</v>
-      </c>
-      <c r="D14" s="116" t="s">
-        <v>134</v>
-      </c>
-      <c r="E14" s="145" t="s">
-        <v>250</v>
-      </c>
-      <c r="F14" s="146" t="s">
-        <v>253</v>
-      </c>
-      <c r="G14" s="135" t="s">
-        <v>70</v>
-      </c>
-      <c r="H14" s="135" t="s">
-        <v>227</v>
-      </c>
-      <c r="O14" s="117" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="15" spans="1:20" s="117" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A15" s="114">
-        <v>13</v>
-      </c>
-      <c r="B15" s="133">
-        <v>43663</v>
-      </c>
-      <c r="C15" s="143" t="s">
-        <v>231</v>
-      </c>
-      <c r="D15" s="116" t="s">
-        <v>129</v>
-      </c>
-      <c r="E15" s="144" t="s">
-        <v>245</v>
-      </c>
-      <c r="F15" s="146" t="s">
-        <v>253</v>
-      </c>
-      <c r="G15" s="135" t="s">
-        <v>70</v>
-      </c>
-      <c r="H15" s="135" t="s">
-        <v>227</v>
-      </c>
-      <c r="O15" s="117" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="16" spans="1:20" s="117" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A16" s="114">
-        <v>14</v>
-      </c>
-      <c r="B16" s="133">
-        <v>43663</v>
-      </c>
-      <c r="C16" s="143" t="s">
-        <v>234</v>
-      </c>
-      <c r="D16" s="116" t="s">
-        <v>128</v>
-      </c>
-      <c r="E16" s="96" t="s">
-        <v>243</v>
-      </c>
-      <c r="F16" s="146" t="s">
-        <v>253</v>
-      </c>
-      <c r="G16" s="135" t="s">
-        <v>70</v>
-      </c>
-      <c r="H16" s="135" t="s">
-        <v>227</v>
-      </c>
-      <c r="O16" s="117" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" s="117" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A17" s="114">
-        <v>15</v>
-      </c>
-      <c r="B17" s="133">
-        <v>43663</v>
-      </c>
-      <c r="C17" s="143" t="s">
-        <v>236</v>
-      </c>
-      <c r="D17" s="116" t="s">
-        <v>119</v>
-      </c>
-      <c r="E17" s="144" t="s">
-        <v>247</v>
-      </c>
-      <c r="F17" s="146" t="s">
-        <v>253</v>
-      </c>
-      <c r="G17" s="135" t="s">
-        <v>70</v>
-      </c>
-      <c r="H17" s="135" t="s">
-        <v>227</v>
-      </c>
-      <c r="O17" s="117" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" s="117" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A18" s="114">
-        <v>16</v>
-      </c>
-      <c r="B18" s="133">
-        <v>43663</v>
-      </c>
-      <c r="C18" s="143" t="s">
-        <v>238</v>
-      </c>
-      <c r="D18" s="116" t="s">
-        <v>118</v>
-      </c>
-      <c r="E18" s="144" t="s">
-        <v>248</v>
-      </c>
-      <c r="F18" s="146" t="s">
-        <v>253</v>
-      </c>
-      <c r="G18" s="135" t="s">
-        <v>70</v>
-      </c>
-      <c r="H18" s="135" t="s">
-        <v>227</v>
-      </c>
-      <c r="O18" s="117" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" s="117" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A19" s="114">
-        <v>17</v>
-      </c>
-      <c r="B19" s="133">
-        <v>43663</v>
-      </c>
-      <c r="C19" s="143" t="s">
-        <v>240</v>
-      </c>
-      <c r="D19" s="116" t="s">
-        <v>116</v>
-      </c>
-      <c r="E19" s="144" t="s">
-        <v>251</v>
-      </c>
-      <c r="F19" s="146" t="s">
-        <v>253</v>
-      </c>
-      <c r="G19" s="135" t="s">
-        <v>70</v>
-      </c>
-      <c r="H19" s="135" t="s">
-        <v>227</v>
-      </c>
-      <c r="O19" s="117" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" s="117" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A20" s="114">
-        <v>18</v>
-      </c>
-      <c r="B20" s="133">
-        <v>43663</v>
-      </c>
-      <c r="C20" s="143" t="s">
-        <v>240</v>
-      </c>
-      <c r="D20" s="116" t="s">
-        <v>114</v>
-      </c>
-      <c r="E20" s="144" t="s">
-        <v>246</v>
-      </c>
-      <c r="F20" s="146" t="s">
-        <v>253</v>
-      </c>
-      <c r="G20" s="135" t="s">
-        <v>70</v>
-      </c>
-      <c r="H20" s="135" t="s">
-        <v>227</v>
-      </c>
-      <c r="O20" s="117" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" s="117" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A21" s="120">
-        <v>19</v>
-      </c>
-      <c r="B21" s="133">
-        <v>43663</v>
-      </c>
-      <c r="C21" s="143" t="s">
-        <v>242</v>
-      </c>
-      <c r="D21" s="116" t="s">
-        <v>104</v>
-      </c>
-      <c r="E21" s="145" t="s">
-        <v>249</v>
-      </c>
-      <c r="F21" s="146" t="s">
-        <v>253</v>
-      </c>
-      <c r="G21" s="135" t="s">
-        <v>70</v>
-      </c>
-      <c r="H21" s="135" t="s">
-        <v>227</v>
-      </c>
-      <c r="O21" s="117" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" s="117" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A22" s="114">
-        <v>20</v>
-      </c>
-      <c r="B22" s="133">
-        <v>43663</v>
-      </c>
-      <c r="C22" s="143" t="s">
-        <v>242</v>
-      </c>
-      <c r="D22" s="116" t="s">
-        <v>103</v>
-      </c>
-      <c r="E22" s="96" t="s">
-        <v>244</v>
-      </c>
-      <c r="F22" s="146" t="s">
-        <v>253</v>
-      </c>
-      <c r="G22" s="135" t="s">
-        <v>70</v>
-      </c>
-      <c r="H22" s="135" t="s">
-        <v>227</v>
-      </c>
-      <c r="O22" s="117" t="s">
-        <v>119</v>
-      </c>
     </row>
     <row r="23" spans="1:15" s="117" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A23" s="114">
-        <v>21</v>
-      </c>
+      <c r="A23" s="114"/>
       <c r="B23" s="115"/>
       <c r="C23" s="115"/>
       <c r="D23" s="116"/>
@@ -10995,13 +10635,11 @@
       <c r="G23" s="114"/>
       <c r="H23" s="114"/>
       <c r="O23" s="117" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="24" spans="1:15" s="117" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A24" s="114">
-        <v>22</v>
-      </c>
+      <c r="A24" s="114"/>
       <c r="B24" s="115"/>
       <c r="C24" s="115"/>
       <c r="D24" s="116"/>
@@ -11010,13 +10648,11 @@
       <c r="G24" s="114"/>
       <c r="H24" s="114"/>
       <c r="O24" s="117" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="25" spans="1:15" s="117" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A25" s="114">
-        <v>23</v>
-      </c>
+      <c r="A25" s="114"/>
       <c r="B25" s="115"/>
       <c r="C25" s="115"/>
       <c r="D25" s="116"/>
@@ -11025,13 +10661,11 @@
       <c r="G25" s="114"/>
       <c r="H25" s="114"/>
       <c r="O25" s="117" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="26" spans="1:15" s="117" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A26" s="114">
-        <v>24</v>
-      </c>
+      <c r="A26" s="114"/>
       <c r="B26" s="115"/>
       <c r="C26" s="115"/>
       <c r="D26" s="116"/>
@@ -11040,13 +10674,11 @@
       <c r="G26" s="114"/>
       <c r="H26" s="114"/>
       <c r="O26" s="117" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="27" spans="1:15" s="117" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A27" s="114">
-        <v>25</v>
-      </c>
+      <c r="A27" s="114"/>
       <c r="B27" s="115"/>
       <c r="C27" s="115"/>
       <c r="D27" s="116"/>
@@ -11055,13 +10687,11 @@
       <c r="G27" s="114"/>
       <c r="H27" s="114"/>
       <c r="O27" s="117" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="28" spans="1:15" s="117" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A28" s="114">
-        <v>26</v>
-      </c>
+      <c r="A28" s="114"/>
       <c r="B28" s="115"/>
       <c r="C28" s="115"/>
       <c r="D28" s="116"/>
@@ -11070,13 +10700,11 @@
       <c r="G28" s="114"/>
       <c r="H28" s="114"/>
       <c r="O28" s="117" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="29" spans="1:15" s="117" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A29" s="114">
-        <v>27</v>
-      </c>
+      <c r="A29" s="114"/>
       <c r="B29" s="115"/>
       <c r="C29" s="115"/>
       <c r="D29" s="116"/>
@@ -11085,13 +10713,11 @@
       <c r="G29" s="114"/>
       <c r="H29" s="114"/>
       <c r="O29" s="117" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="30" spans="1:15" s="117" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A30" s="114">
-        <v>28</v>
-      </c>
+      <c r="A30" s="114"/>
       <c r="B30" s="115"/>
       <c r="C30" s="115"/>
       <c r="D30" s="116"/>
@@ -11100,13 +10726,11 @@
       <c r="G30" s="114"/>
       <c r="H30" s="114"/>
       <c r="O30" s="117" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="31" spans="1:15" s="117" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A31" s="114">
-        <v>29</v>
-      </c>
+      <c r="A31" s="114"/>
       <c r="B31" s="115"/>
       <c r="C31" s="115"/>
       <c r="D31" s="116"/>
@@ -11115,13 +10739,11 @@
       <c r="G31" s="114"/>
       <c r="H31" s="114"/>
       <c r="O31" s="117" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="32" spans="1:15" s="117" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A32" s="114">
-        <v>30</v>
-      </c>
+      <c r="A32" s="114"/>
       <c r="B32" s="115"/>
       <c r="C32" s="115"/>
       <c r="D32" s="116"/>
@@ -11130,13 +10752,11 @@
       <c r="G32" s="114"/>
       <c r="H32" s="114"/>
       <c r="O32" s="117" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="33" spans="1:15" s="117" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A33" s="114">
-        <v>31</v>
-      </c>
+      <c r="A33" s="114"/>
       <c r="B33" s="115"/>
       <c r="C33" s="115"/>
       <c r="D33" s="116"/>
@@ -11145,13 +10765,11 @@
       <c r="G33" s="114"/>
       <c r="H33" s="114"/>
       <c r="O33" s="117" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="34" spans="1:15" s="117" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A34" s="114">
-        <v>32</v>
-      </c>
+      <c r="A34" s="114"/>
       <c r="B34" s="115"/>
       <c r="C34" s="115"/>
       <c r="D34" s="116"/>
@@ -11160,13 +10778,11 @@
       <c r="G34" s="114"/>
       <c r="H34" s="114"/>
       <c r="O34" s="117" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="35" spans="1:15" s="117" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A35" s="114">
-        <v>33</v>
-      </c>
+      <c r="A35" s="114"/>
       <c r="B35" s="115"/>
       <c r="C35" s="115"/>
       <c r="D35" s="116"/>
@@ -11175,13 +10791,11 @@
       <c r="G35" s="114"/>
       <c r="H35" s="114"/>
       <c r="O35" s="117" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="36" spans="1:15" s="117" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A36" s="114">
-        <v>34</v>
-      </c>
+      <c r="A36" s="114"/>
       <c r="B36" s="115"/>
       <c r="C36" s="115"/>
       <c r="D36" s="116"/>
@@ -11190,13 +10804,11 @@
       <c r="G36" s="114"/>
       <c r="H36" s="114"/>
       <c r="O36" s="117" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="37" spans="1:15" s="117" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A37" s="114">
-        <v>35</v>
-      </c>
+      <c r="A37" s="114"/>
       <c r="B37" s="115"/>
       <c r="C37" s="115"/>
       <c r="D37" s="116"/>
@@ -11205,13 +10817,11 @@
       <c r="G37" s="114"/>
       <c r="H37" s="114"/>
       <c r="O37" s="117" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="38" spans="1:15" s="117" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A38" s="114">
-        <v>36</v>
-      </c>
+      <c r="A38" s="114"/>
       <c r="B38" s="115"/>
       <c r="C38" s="115"/>
       <c r="D38" s="116"/>
@@ -11220,13 +10830,11 @@
       <c r="G38" s="114"/>
       <c r="H38" s="114"/>
       <c r="O38" s="117" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="39" spans="1:15" s="117" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A39" s="120" t="s">
-        <v>77</v>
-      </c>
+      <c r="A39" s="120"/>
       <c r="B39" s="115"/>
       <c r="C39" s="115"/>
       <c r="D39" s="116"/>
@@ -11236,14 +10844,12 @@
       <c r="H39" s="114"/>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A40" s="125" t="s">
-        <v>177</v>
-      </c>
+      <c r="A40" s="125"/>
       <c r="D40" s="3"/>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B43" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -11304,37 +10910,8 @@
       <formula1>$L$3:$L$5</formula1>
     </dataValidation>
   </dataValidations>
-  <hyperlinks>
-    <hyperlink ref="C4" r:id="rId1" display="https://intra.hhbi.mah.gov.on.ca/sites/hhbi/SitePages/Home.aspx" xr:uid="{0B626540-4BE2-4906-9816-F2A99C655FCB}"/>
-    <hyperlink ref="C5" r:id="rId2" xr:uid="{FA934FF9-203E-4D2A-AA89-947E96734BB8}"/>
-    <hyperlink ref="C8" r:id="rId3" display="http://cscdikdcapmsp01:7777/_admin/WebApplicationList.aspx" xr:uid="{7FE4CE1B-84AF-4A34-9D75-ED140C4907E1}"/>
-    <hyperlink ref="C9" r:id="rId4" display="http://cscdikdcapmsp01:7777/applications.aspx" xr:uid="{5DA472BC-D325-4E22-AFC7-0C30DFCB8A6E}"/>
-    <hyperlink ref="C7" r:id="rId5" display="http://cscdikdcapmsp01:7777/_admin/WebApplicationList.aspx" xr:uid="{9A67F195-1B56-419C-B435-923A8FF16F8E}"/>
-    <hyperlink ref="C10" r:id="rId6" display="http://cscdikdcapmsp01:7777/apps.aspx" xr:uid="{8317C075-5776-4266-AA83-848A1F1BDCAD}"/>
-    <hyperlink ref="C12" r:id="rId7" display="http://cscdikdcapmsp01:7777/default.aspx" xr:uid="{58431B13-5A90-4096-9965-2E3FF324183C}"/>
-    <hyperlink ref="C6" r:id="rId8" xr:uid="{FE93ABA9-6A35-4844-B27E-C1707F38D402}"/>
-    <hyperlink ref="C11" r:id="rId9" display="http://cscdikdcapmsp01:7777/apps.aspx" xr:uid="{1C8B244C-4300-4C43-8F89-913FEA46AB37}"/>
-    <hyperlink ref="E13" r:id="rId10" display="td://rv.oa.intra.dev.hpqualitycenter.csc.gov.on.ca:8080/qcbin/DefectsModule-000000004243046514?EntityType=IBug&amp;EntityID=545" xr:uid="{A2FFDC56-5555-4D05-9205-03670AA3FF00}"/>
-    <hyperlink ref="E14" r:id="rId11" display="td://rv.oa.intra.dev.hpqualitycenter.csc.gov.on.ca:8080/qcbin/DefectsModule-000000004243046514?EntityType=IBug&amp;EntityID=957" xr:uid="{00E5FA44-2A3A-41E0-A56C-DAE2471400FD}"/>
-    <hyperlink ref="E15" r:id="rId12" display="td://rv.oa.intra.dev.hpqualitycenter.csc.gov.on.ca:8080/qcbin/DefectsModule-000000004243046514?EntityType=IBug&amp;EntityID=929" xr:uid="{722B0439-FDA9-4060-8C3F-A8DD1275C140}"/>
-    <hyperlink ref="E17" r:id="rId13" display="td://rv.oa.intra.dev.hpqualitycenter.csc.gov.on.ca:8080/qcbin/DefectsModule-000000004243046514?EntityType=IBug&amp;EntityID=931" xr:uid="{80881EE2-D7AF-4A9A-8284-6FEC68C83506}"/>
-    <hyperlink ref="E18" r:id="rId14" display="td://rv.oa.intra.dev.hpqualitycenter.csc.gov.on.ca:8080/qcbin/DefectsModule-000000004243046514?EntityType=IBug&amp;EntityID=936" xr:uid="{9510838A-A0C2-4C0D-B96B-3A98A17B5954}"/>
-    <hyperlink ref="E19" r:id="rId15" display="td://rv.oa.intra.dev.hpqualitycenter.csc.gov.on.ca:8080/qcbin/DefectsModule-000000004243046514?EntityType=IBug&amp;EntityID=532" xr:uid="{20B0B585-187A-4ECB-951C-1A6FD2F9821D}"/>
-    <hyperlink ref="E20" r:id="rId16" display="td://rv.oa.intra.dev.hpqualitycenter.csc.gov.on.ca:8080/qcbin/DefectsModule-000000004243046514?EntityType=IBug&amp;EntityID=938" xr:uid="{53537E33-4F95-4A85-A9A1-510A0BF9FCB3}"/>
-    <hyperlink ref="E21" r:id="rId17" display="td://rv.oa.intra.dev.hpqualitycenter.csc.gov.on.ca:8080/qcbin/DefectsModule-000000004243046514?EntityType=IBug&amp;EntityID=930" xr:uid="{94B98066-2C1F-478C-8A60-43327F609D57}"/>
-    <hyperlink ref="C13" r:id="rId18" display="https://intra.hhbi.mah.gov.on.ca/sites/hhbi/SitePages/Home.aspx" xr:uid="{82E3BB38-B225-41CC-BB69-55162C1321F4}"/>
-    <hyperlink ref="C14" r:id="rId19" xr:uid="{6A4E99F2-9B02-4D2C-B9B7-FDDE585ED6E1}"/>
-    <hyperlink ref="C17" r:id="rId20" display="http://cscdikdcapmsp01:7777/_admin/WebApplicationList.aspx" xr:uid="{ED575AB4-32E3-494E-8581-4A2059C5E2C4}"/>
-    <hyperlink ref="C18" r:id="rId21" display="http://cscdikdcapmsp01:7777/applications.aspx" xr:uid="{94918830-41B5-4731-972E-7B524CF91CD8}"/>
-    <hyperlink ref="C16" r:id="rId22" display="http://cscdikdcapmsp01:7777/_admin/WebApplicationList.aspx" xr:uid="{B1B22C69-1014-4DBB-89C9-9AB18D5E5D1A}"/>
-    <hyperlink ref="C19" r:id="rId23" display="http://cscdikdcapmsp01:7777/apps.aspx" xr:uid="{E9FB98AF-C2DC-4E26-B452-B673BCF3B79D}"/>
-    <hyperlink ref="C21" r:id="rId24" display="http://cscdikdcapmsp01:7777/default.aspx" xr:uid="{330B493F-D4EC-408A-A02C-86B8B19FDE9E}"/>
-    <hyperlink ref="C15" r:id="rId25" xr:uid="{E0692E05-9154-42C4-8D55-C07B741FC057}"/>
-    <hyperlink ref="C20" r:id="rId26" display="http://cscdikdcapmsp01:7777/apps.aspx" xr:uid="{4EC88483-CEA0-4536-BDD3-F4F91323A292}"/>
-    <hyperlink ref="C22" r:id="rId27" display="http://cscdikdcapmsp01:7777/default.aspx" xr:uid="{8680A7CD-16B4-47F1-AB0D-EDA0AB385A54}"/>
-  </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup scale="60" orientation="landscape" horizontalDpi="4294967292" verticalDpi="300" r:id="rId28"/>
+  <pageSetup scale="60" orientation="landscape" horizontalDpi="4294967292" verticalDpi="300" r:id="rId1"/>
   <headerFooter alignWithMargins="0">
     <oddFooter>&amp;L&amp;F&amp;R&amp;P of &amp;N</oddFooter>
   </headerFooter>
@@ -11392,36 +10969,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="039bc2d6-e16a-4b4d-b61d-73ee5a6b5720"/>
-    <n8bc46b862004554b29f25437dcecdb2 xmlns="93977a9a-7c70-4c47-a38b-6f123b62dce6">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </n8bc46b862004554b29f25437dcecdb2>
-    <Fiscal_x0020_Year xmlns="17eb8759-252b-418d-a649-70aff91fc5df" xsi:nil="true"/>
-    <Archive xmlns="17eb8759-252b-418d-a649-70aff91fc5df">false</Archive>
-    <b348aa9236b94ac88332be997039b018 xmlns="17eb8759-252b-418d-a649-70aff91fc5df">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </b348aa9236b94ac88332be997039b018>
-    <_dlc_DocId xmlns="039bc2d6-e16a-4b4d-b61d-73ee5a6b5720">QWPW5C3C64YX-694079015-91</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="039bc2d6-e16a-4b4d-b61d-73ee5a6b5720">
-      <Url>http://cscgikdcapmdw40/ProjectsLab/AODACompliance/_layouts/15/DocIdRedir.aspx?ID=QWPW5C3C64YX-694079015-91</Url>
-      <Description>QWPW5C3C64YX-694079015-91</Description>
-    </_dlc_DocIdUrl>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001B7F6C1E041661428C0804F60FDF9579" ma:contentTypeVersion="1" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="269e77b516f09928499b1be999970057">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="17eb8759-252b-418d-a649-70aff91fc5df" xmlns:ns3="039bc2d6-e16a-4b4d-b61d-73ee5a6b5720" xmlns:ns4="93977a9a-7c70-4c47-a38b-6f123b62dce6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="41b65eea62d023978f15f5547645abd7" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="17eb8759-252b-418d-a649-70aff91fc5df"/>
@@ -11642,6 +11189,36 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="039bc2d6-e16a-4b4d-b61d-73ee5a6b5720"/>
+    <n8bc46b862004554b29f25437dcecdb2 xmlns="93977a9a-7c70-4c47-a38b-6f123b62dce6">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </n8bc46b862004554b29f25437dcecdb2>
+    <Fiscal_x0020_Year xmlns="17eb8759-252b-418d-a649-70aff91fc5df" xsi:nil="true"/>
+    <Archive xmlns="17eb8759-252b-418d-a649-70aff91fc5df">false</Archive>
+    <b348aa9236b94ac88332be997039b018 xmlns="17eb8759-252b-418d-a649-70aff91fc5df">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </b348aa9236b94ac88332be997039b018>
+    <_dlc_DocId xmlns="039bc2d6-e16a-4b4d-b61d-73ee5a6b5720">QWPW5C3C64YX-694079015-91</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="039bc2d6-e16a-4b4d-b61d-73ee5a6b5720">
+      <Url>http://cscgikdcapmdw40/ProjectsLab/AODACompliance/_layouts/15/DocIdRedir.aspx?ID=QWPW5C3C64YX-694079015-91</Url>
+      <Description>QWPW5C3C64YX-694079015-91</Description>
+    </_dlc_DocIdUrl>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2E5D2D22-6D00-46CD-B7EA-B8CE8E1546D9}">
   <ds:schemaRefs>
@@ -11651,32 +11228,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C507B214-A4AD-4147-9668-C65BAB18F1D2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="17eb8759-252b-418d-a649-70aff91fc5df"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="93977a9a-7c70-4c47-a38b-6f123b62dce6"/>
-    <ds:schemaRef ds:uri="039bc2d6-e16a-4b4d-b61d-73ee5a6b5720"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D6D3747C-BDC7-48F7-9B5A-BD9117F21569}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3C5CD16F-1A82-4BAB-88E6-9D42833A2748}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11694,4 +11245,30 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D6D3747C-BDC7-48F7-9B5A-BD9117F21569}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C507B214-A4AD-4147-9668-C65BAB18F1D2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="17eb8759-252b-418d-a649-70aff91fc5df"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="93977a9a-7c70-4c47-a38b-6f123b62dce6"/>
+    <ds:schemaRef ds:uri="039bc2d6-e16a-4b4d-b61d-73ee5a6b5720"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added medium option to issue tracking log
</commit_message>
<xml_diff>
--- a/AxeAccessibilityDriver/AxeAccessibilityDriver/AODA_Template.xlsx
+++ b/AxeAccessibilityDriver/AxeAccessibilityDriver/AODA_Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DUONGCH\Projects\AxeAccessibilityDriver\AxeAccessibilityDriver\AxeAccessibilityDriver\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{742EF0C8-6EB1-44D1-A0ED-0C9622A6974A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{022454C8-B3EE-4128-9E4E-65EA85C1CAF0}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="760" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="760" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="5" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="253">
   <si>
     <t>1.1.1</t>
   </si>
@@ -2431,6 +2431,9 @@
     <t xml:space="preserve">Evaluation has been carrying on from 2016, has been tested multiple times in Cognos Version 10, then in Version 11 and the last time was tested on: 8/14/2019
 Every release will be AODA tested as part of our software development lifecycle, issues will be evaluated and remediated in accordance with WCAG2.00 AA guideline. </t>
   </si>
+  <si>
+    <t>Medium</t>
+  </si>
 </sst>
 </file>
 
@@ -2443,12 +2446,19 @@
     <numFmt numFmtId="167" formatCode="m/d/yyyy;@"/>
     <numFmt numFmtId="168" formatCode="mm/dd/yy;@"/>
   </numFmts>
-  <fonts count="48" x14ac:knownFonts="1">
+  <fonts count="50" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -2766,8 +2776,16 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2836,6 +2854,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF002060"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
       </patternFill>
     </fill>
   </fills>
@@ -3247,72 +3271,73 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="16">
+  <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="10" borderId="0" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="10" borderId="0" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="27" fillId="12" borderId="32" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="23" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="12" borderId="32" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="218">
+  <cellXfs count="219">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="3" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="3" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="3" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="2" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="2" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
@@ -3330,44 +3355,44 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="166" fontId="10" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="14" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="11" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="12" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
@@ -3379,16 +3404,16 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -3397,52 +3422,52 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="29" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="29" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="2" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="2" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="2" applyFill="1" applyProtection="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="2" applyFill="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyProtection="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="0" xfId="10" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="0" xfId="10" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -3450,99 +3475,99 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="33" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="24" fillId="6" borderId="15" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="25" fillId="6" borderId="15" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="16" xfId="10" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="16" xfId="10" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="4" borderId="12" xfId="9" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="4" borderId="12" xfId="9" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="27" fillId="12" borderId="32" xfId="14"/>
-    <xf numFmtId="0" fontId="26" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="12" borderId="32" xfId="14"/>
+    <xf numFmtId="0" fontId="27" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="2" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="28" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="29" fillId="2" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="29" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="2" borderId="30" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="30" fillId="2" borderId="30" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="2" borderId="1" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="33" fillId="2" borderId="1" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="2" borderId="30" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="30" fillId="2" borderId="30" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="15" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="14" fontId="16" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="15" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="167" fontId="16" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -3551,325 +3576,329 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="28" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="29" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="25" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="29" fillId="0" borderId="25" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="25" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="25" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="30" fillId="0" borderId="25" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="25" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="41" fillId="8" borderId="0" xfId="12" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="42" fillId="8" borderId="0" xfId="12" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="9" borderId="0" xfId="13" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="42" fillId="9" borderId="0" xfId="13" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="25" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="25" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="33" fillId="6" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="29" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="30" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="2" xfId="10" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="2" xfId="10" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="14" fontId="29" fillId="0" borderId="25" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="30" fillId="0" borderId="25" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="29" fillId="0" borderId="25" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="30" fillId="0" borderId="25" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="25" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="25" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="25" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="25" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="25" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="25" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="25" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="25" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="29" fillId="0" borderId="25" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="30" fillId="0" borderId="25" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="25" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="25" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="25" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="25" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="29" fillId="0" borderId="25" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="30" fillId="0" borderId="25" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="8" fillId="0" borderId="25" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="168" fontId="9" fillId="0" borderId="25" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="8" fillId="0" borderId="25" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="168" fontId="9" fillId="0" borderId="25" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="25" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="25" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="15" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="15" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="15" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="15" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="15" applyFill="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="15" applyFill="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="15" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="15" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="15" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="15" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="15" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="15" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="15" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="15" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="15" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="15" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="15" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="15" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="15" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="15" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="15" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="15" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="49" fillId="13" borderId="0" xfId="16" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="34" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="33" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="33" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="43" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="27" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="27" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="34" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="167" fontId="12" fillId="5" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="167" fontId="13" fillId="5" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="25" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="25" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="26" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="6" borderId="26" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="6" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="21" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="6" borderId="21" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="16">
+  <cellStyles count="17">
+    <cellStyle name="40% - Accent6" xfId="16" builtinId="51"/>
     <cellStyle name="Bad" xfId="12" builtinId="27"/>
     <cellStyle name="Heading 1 2" xfId="10" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Heading 2 2" xfId="9" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
@@ -7796,8 +7825,8 @@
   </sheetPr>
   <dimension ref="A1:XFC81"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="115" zoomScalePageLayoutView="160" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="115" zoomScalePageLayoutView="160" workbookViewId="0">
+      <selection activeCell="XFD1" sqref="F1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="12.75" zeroHeight="1" x14ac:dyDescent="0.2"/>
@@ -7806,32 +7835,32 @@
     <col min="2" max="2" width="88.42578125" style="20" customWidth="1"/>
     <col min="3" max="3" width="10.7109375" style="37" customWidth="1"/>
     <col min="4" max="4" width="27.5703125" style="38" customWidth="1"/>
-    <col min="5" max="5" width="67.5703125" style="45" customWidth="1"/>
-    <col min="6" max="7" width="0" style="37" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="0" style="36" hidden="1" customWidth="1"/>
-    <col min="9" max="16" width="0" style="14" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="0" style="15" hidden="1" customWidth="1"/>
-    <col min="18" max="19" width="0" style="14" hidden="1" customWidth="1"/>
-    <col min="20" max="16378" width="6.140625" style="14" hidden="1"/>
-    <col min="16379" max="16379" width="25.7109375" style="14" hidden="1" customWidth="1"/>
-    <col min="16380" max="16380" width="28.42578125" style="14" hidden="1" customWidth="1"/>
-    <col min="16381" max="16381" width="34" style="14" hidden="1" customWidth="1"/>
-    <col min="16382" max="16382" width="29.28515625" style="14" hidden="1" customWidth="1"/>
-    <col min="16383" max="16383" width="16.5703125" style="14" hidden="1" customWidth="1"/>
-    <col min="16384" max="16384" width="85.85546875" style="14" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="85.85546875" style="45" customWidth="1"/>
+    <col min="6" max="7" width="0" style="37" hidden="1"/>
+    <col min="8" max="8" width="0" style="36" hidden="1"/>
+    <col min="9" max="16" width="0" style="14" hidden="1"/>
+    <col min="17" max="17" width="0" style="15" hidden="1"/>
+    <col min="18" max="19" width="0" style="14" hidden="1"/>
+    <col min="20" max="16378" width="85.85546875" style="14" hidden="1"/>
+    <col min="16379" max="16379" width="25.7109375" style="14" hidden="1"/>
+    <col min="16380" max="16380" width="28.42578125" style="14" hidden="1"/>
+    <col min="16381" max="16381" width="34" style="14" hidden="1"/>
+    <col min="16382" max="16382" width="29.28515625" style="14" hidden="1"/>
+    <col min="16383" max="16383" width="16.5703125" style="14" hidden="1"/>
+    <col min="16384" max="16384" width="85.85546875" style="14" hidden="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="13" customFormat="1" ht="37.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="184" t="s">
+      <c r="A1" s="185" t="s">
         <v>225</v>
       </c>
-      <c r="B1" s="184"/>
-      <c r="C1" s="184"/>
-      <c r="D1" s="184"/>
-      <c r="E1" s="184"/>
-      <c r="F1" s="184"/>
-      <c r="G1" s="184"/>
-      <c r="H1" s="185"/>
+      <c r="B1" s="185"/>
+      <c r="C1" s="185"/>
+      <c r="D1" s="185"/>
+      <c r="E1" s="185"/>
+      <c r="F1" s="185"/>
+      <c r="G1" s="185"/>
+      <c r="H1" s="186"/>
       <c r="I1" s="11"/>
       <c r="J1" s="12"/>
       <c r="K1" s="1"/>
@@ -7845,13 +7874,13 @@
       <c r="S1" s="1"/>
     </row>
     <row r="2" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="165" t="s">
+      <c r="A2" s="166" t="s">
         <v>61</v>
       </c>
-      <c r="B2" s="165"/>
-      <c r="C2" s="188"/>
-      <c r="D2" s="188"/>
-      <c r="E2" s="189"/>
+      <c r="B2" s="166"/>
+      <c r="C2" s="189"/>
+      <c r="D2" s="189"/>
+      <c r="E2" s="190"/>
       <c r="F2" s="39"/>
       <c r="G2" s="1"/>
       <c r="H2" s="16"/>
@@ -7863,13 +7892,13 @@
       <c r="N2" s="13"/>
     </row>
     <row r="3" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="165" t="s">
+      <c r="A3" s="166" t="s">
         <v>63</v>
       </c>
-      <c r="B3" s="165"/>
-      <c r="C3" s="201"/>
-      <c r="D3" s="202"/>
-      <c r="E3" s="203"/>
+      <c r="B3" s="166"/>
+      <c r="C3" s="202"/>
+      <c r="D3" s="203"/>
+      <c r="E3" s="204"/>
       <c r="F3" s="39"/>
       <c r="G3" s="1"/>
       <c r="H3" s="16"/>
@@ -7881,12 +7910,12 @@
       <c r="N3" s="13"/>
     </row>
     <row r="4" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="165" t="s">
+      <c r="A4" s="166" t="s">
         <v>77</v>
       </c>
-      <c r="B4" s="165"/>
-      <c r="C4" s="211"/>
-      <c r="D4" s="211"/>
+      <c r="B4" s="166"/>
+      <c r="C4" s="212"/>
+      <c r="D4" s="212"/>
       <c r="E4" s="91"/>
       <c r="F4" s="39"/>
       <c r="G4" s="1"/>
@@ -7899,13 +7928,13 @@
       <c r="N4" s="13"/>
     </row>
     <row r="5" spans="1:19" ht="27" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="164" t="s">
+      <c r="A5" s="165" t="s">
         <v>78</v>
       </c>
-      <c r="B5" s="164"/>
-      <c r="C5" s="212"/>
-      <c r="D5" s="212"/>
-      <c r="E5" s="213"/>
+      <c r="B5" s="165"/>
+      <c r="C5" s="213"/>
+      <c r="D5" s="213"/>
+      <c r="E5" s="214"/>
       <c r="F5" s="39"/>
       <c r="G5" s="1"/>
       <c r="H5" s="16"/>
@@ -7917,13 +7946,13 @@
       <c r="N5" s="13"/>
     </row>
     <row r="6" spans="1:19" ht="27" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="164" t="s">
+      <c r="A6" s="165" t="s">
         <v>79</v>
       </c>
-      <c r="B6" s="164"/>
-      <c r="C6" s="162"/>
-      <c r="D6" s="162"/>
-      <c r="E6" s="163"/>
+      <c r="B6" s="165"/>
+      <c r="C6" s="163"/>
+      <c r="D6" s="163"/>
+      <c r="E6" s="164"/>
       <c r="F6" s="39"/>
       <c r="G6" s="1"/>
       <c r="H6" s="16"/>
@@ -7935,13 +7964,13 @@
       <c r="N6" s="13"/>
     </row>
     <row r="7" spans="1:19" ht="27" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="164" t="s">
+      <c r="A7" s="165" t="s">
         <v>80</v>
       </c>
-      <c r="B7" s="164"/>
-      <c r="C7" s="162"/>
-      <c r="D7" s="162"/>
-      <c r="E7" s="163"/>
+      <c r="B7" s="165"/>
+      <c r="C7" s="163"/>
+      <c r="D7" s="163"/>
+      <c r="E7" s="164"/>
       <c r="F7" s="39"/>
       <c r="G7" s="1"/>
       <c r="H7" s="16"/>
@@ -7953,13 +7982,13 @@
       <c r="N7" s="13"/>
     </row>
     <row r="8" spans="1:19" ht="27" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="164" t="s">
+      <c r="A8" s="165" t="s">
         <v>81</v>
       </c>
-      <c r="B8" s="164"/>
-      <c r="C8" s="162"/>
-      <c r="D8" s="162"/>
-      <c r="E8" s="163"/>
+      <c r="B8" s="165"/>
+      <c r="C8" s="163"/>
+      <c r="D8" s="163"/>
+      <c r="E8" s="164"/>
       <c r="F8" s="39"/>
       <c r="G8" s="1"/>
       <c r="H8" s="16"/>
@@ -7971,16 +8000,16 @@
       <c r="N8" s="13"/>
     </row>
     <row r="9" spans="1:19" s="37" customFormat="1" ht="52.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="192" t="s">
+      <c r="A9" s="193" t="s">
         <v>76</v>
       </c>
-      <c r="B9" s="193"/>
-      <c r="C9" s="193"/>
-      <c r="D9" s="193"/>
-      <c r="E9" s="193"/>
-      <c r="F9" s="193"/>
-      <c r="G9" s="193"/>
-      <c r="H9" s="193"/>
+      <c r="B9" s="194"/>
+      <c r="C9" s="194"/>
+      <c r="D9" s="194"/>
+      <c r="E9" s="194"/>
+      <c r="F9" s="194"/>
+      <c r="G9" s="194"/>
+      <c r="H9" s="194"/>
       <c r="I9" s="18"/>
       <c r="J9" s="18"/>
       <c r="K9" s="18"/>
@@ -7990,16 +8019,16 @@
       <c r="Q9" s="108"/>
     </row>
     <row r="10" spans="1:19" s="22" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="194" t="s">
+      <c r="A10" s="195" t="s">
         <v>210</v>
       </c>
-      <c r="B10" s="195"/>
-      <c r="C10" s="195"/>
-      <c r="D10" s="195"/>
-      <c r="E10" s="195"/>
-      <c r="F10" s="195"/>
-      <c r="G10" s="195"/>
-      <c r="H10" s="196"/>
+      <c r="B10" s="196"/>
+      <c r="C10" s="196"/>
+      <c r="D10" s="196"/>
+      <c r="E10" s="196"/>
+      <c r="F10" s="196"/>
+      <c r="G10" s="196"/>
+      <c r="H10" s="197"/>
       <c r="I10" s="21"/>
       <c r="J10" s="21"/>
       <c r="K10" s="21"/>
@@ -8009,10 +8038,10 @@
       <c r="Q10" s="23"/>
     </row>
     <row r="11" spans="1:19" ht="55.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="199" t="s">
+      <c r="A11" s="200" t="s">
         <v>54</v>
       </c>
-      <c r="B11" s="200"/>
+      <c r="B11" s="201"/>
       <c r="C11" s="123" t="s">
         <v>40</v>
       </c>
@@ -8022,10 +8051,10 @@
       <c r="E11" s="123" t="s">
         <v>99</v>
       </c>
-      <c r="F11" s="198" t="s">
+      <c r="F11" s="199" t="s">
         <v>52</v>
       </c>
-      <c r="G11" s="198"/>
+      <c r="G11" s="199"/>
       <c r="H11" s="124" t="s">
         <v>53</v>
       </c>
@@ -8037,18 +8066,18 @@
       <c r="N11" s="13"/>
     </row>
     <row r="12" spans="1:19" ht="69.599999999999994" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="190" t="s">
+      <c r="A12" s="191" t="s">
         <v>83</v>
       </c>
-      <c r="B12" s="191"/>
-      <c r="C12" s="181" t="s">
+      <c r="B12" s="192"/>
+      <c r="C12" s="182" t="s">
         <v>179</v>
       </c>
-      <c r="D12" s="182"/>
-      <c r="E12" s="182"/>
-      <c r="F12" s="182"/>
-      <c r="G12" s="182"/>
-      <c r="H12" s="183"/>
+      <c r="D12" s="183"/>
+      <c r="E12" s="183"/>
+      <c r="F12" s="183"/>
+      <c r="G12" s="183"/>
+      <c r="H12" s="184"/>
       <c r="I12" s="13"/>
       <c r="J12" s="13"/>
       <c r="K12" s="13"/>
@@ -8445,14 +8474,14 @@
       <c r="Q26" s="102"/>
     </row>
     <row r="27" spans="1:17" ht="17.45" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="186" t="s">
+      <c r="A27" s="187" t="s">
         <v>67</v>
       </c>
-      <c r="B27" s="187"/>
-      <c r="C27" s="187"/>
-      <c r="D27" s="187"/>
-      <c r="E27" s="187"/>
-      <c r="F27" s="187"/>
+      <c r="B27" s="188"/>
+      <c r="C27" s="188"/>
+      <c r="D27" s="188"/>
+      <c r="E27" s="188"/>
+      <c r="F27" s="188"/>
       <c r="G27" s="24">
         <f>SUM(H13:H26)</f>
         <v>0</v>
@@ -8469,18 +8498,18 @@
       <c r="N27" s="13"/>
     </row>
     <row r="28" spans="1:17" ht="53.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="190" t="s">
+      <c r="A28" s="191" t="s">
         <v>84</v>
       </c>
-      <c r="B28" s="197"/>
-      <c r="C28" s="181" t="s">
+      <c r="B28" s="198"/>
+      <c r="C28" s="182" t="s">
         <v>185</v>
       </c>
-      <c r="D28" s="182"/>
-      <c r="E28" s="182"/>
-      <c r="F28" s="182"/>
-      <c r="G28" s="182"/>
-      <c r="H28" s="183"/>
+      <c r="D28" s="183"/>
+      <c r="E28" s="183"/>
+      <c r="F28" s="183"/>
+      <c r="G28" s="183"/>
+      <c r="H28" s="184"/>
       <c r="I28" s="13"/>
       <c r="J28" s="13"/>
       <c r="K28" s="13"/>
@@ -8810,14 +8839,14 @@
       <c r="Q40" s="102"/>
     </row>
     <row r="41" spans="1:17" ht="48.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="186" t="s">
+      <c r="A41" s="187" t="s">
         <v>66</v>
       </c>
-      <c r="B41" s="187"/>
-      <c r="C41" s="187"/>
-      <c r="D41" s="187"/>
-      <c r="E41" s="187"/>
-      <c r="F41" s="187"/>
+      <c r="B41" s="188"/>
+      <c r="C41" s="188"/>
+      <c r="D41" s="188"/>
+      <c r="E41" s="188"/>
+      <c r="F41" s="188"/>
       <c r="G41" s="24">
         <f>SUM(H29:H40)</f>
         <v>0</v>
@@ -8834,18 +8863,18 @@
       <c r="N41" s="13"/>
     </row>
     <row r="42" spans="1:17" ht="54.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="190" t="s">
+      <c r="A42" s="191" t="s">
         <v>85</v>
       </c>
-      <c r="B42" s="197"/>
-      <c r="C42" s="181" t="s">
+      <c r="B42" s="198"/>
+      <c r="C42" s="182" t="s">
         <v>190</v>
       </c>
-      <c r="D42" s="182"/>
-      <c r="E42" s="182"/>
-      <c r="F42" s="182"/>
-      <c r="G42" s="182"/>
-      <c r="H42" s="183"/>
+      <c r="D42" s="183"/>
+      <c r="E42" s="183"/>
+      <c r="F42" s="183"/>
+      <c r="G42" s="183"/>
+      <c r="H42" s="184"/>
       <c r="I42" s="13"/>
       <c r="J42" s="13"/>
       <c r="K42" s="13"/>
@@ -9124,14 +9153,14 @@
       <c r="Q52" s="102"/>
     </row>
     <row r="53" spans="1:17" ht="74.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="186" t="s">
+      <c r="A53" s="187" t="s">
         <v>65</v>
       </c>
-      <c r="B53" s="187"/>
-      <c r="C53" s="187"/>
-      <c r="D53" s="187"/>
-      <c r="E53" s="187"/>
-      <c r="F53" s="187"/>
+      <c r="B53" s="188"/>
+      <c r="C53" s="188"/>
+      <c r="D53" s="188"/>
+      <c r="E53" s="188"/>
+      <c r="F53" s="188"/>
       <c r="G53" s="25">
         <f>SUM(H43:H52)</f>
         <v>0</v>
@@ -9148,18 +9177,18 @@
       <c r="N53" s="13"/>
     </row>
     <row r="54" spans="1:17" ht="47.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="207" t="s">
+      <c r="A54" s="208" t="s">
         <v>86</v>
       </c>
-      <c r="B54" s="208"/>
-      <c r="C54" s="204" t="s">
+      <c r="B54" s="209"/>
+      <c r="C54" s="205" t="s">
         <v>196</v>
       </c>
-      <c r="D54" s="205"/>
-      <c r="E54" s="205"/>
-      <c r="F54" s="205"/>
-      <c r="G54" s="205"/>
-      <c r="H54" s="206"/>
+      <c r="D54" s="206"/>
+      <c r="E54" s="206"/>
+      <c r="F54" s="206"/>
+      <c r="G54" s="206"/>
+      <c r="H54" s="207"/>
       <c r="I54" s="13"/>
       <c r="J54" s="13"/>
       <c r="K54" s="13"/>
@@ -9222,14 +9251,14 @@
       <c r="Q56" s="102"/>
     </row>
     <row r="57" spans="1:17" ht="43.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="186" t="s">
+      <c r="A57" s="187" t="s">
         <v>64</v>
       </c>
-      <c r="B57" s="187"/>
-      <c r="C57" s="187"/>
-      <c r="D57" s="187"/>
-      <c r="E57" s="187"/>
-      <c r="F57" s="187"/>
+      <c r="B57" s="188"/>
+      <c r="C57" s="188"/>
+      <c r="D57" s="188"/>
+      <c r="E57" s="188"/>
+      <c r="F57" s="188"/>
       <c r="G57" s="24">
         <f>SUM(H55:H56)</f>
         <v>0</v>
@@ -9246,16 +9275,16 @@
       <c r="N57" s="13"/>
     </row>
     <row r="58" spans="1:17" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="209" t="s">
+      <c r="A58" s="210" t="s">
         <v>88</v>
       </c>
-      <c r="B58" s="210"/>
-      <c r="C58" s="210"/>
-      <c r="D58" s="210"/>
-      <c r="E58" s="210"/>
-      <c r="F58" s="178"/>
-      <c r="G58" s="179"/>
-      <c r="H58" s="180"/>
+      <c r="B58" s="211"/>
+      <c r="C58" s="211"/>
+      <c r="D58" s="211"/>
+      <c r="E58" s="211"/>
+      <c r="F58" s="179"/>
+      <c r="G58" s="180"/>
+      <c r="H58" s="181"/>
       <c r="I58" s="13"/>
       <c r="J58" s="13"/>
       <c r="K58" s="13"/>
@@ -9264,14 +9293,14 @@
       <c r="N58" s="13"/>
     </row>
     <row r="59" spans="1:17" ht="24.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A59" s="168"/>
-      <c r="B59" s="169"/>
+      <c r="A59" s="169"/>
+      <c r="B59" s="170"/>
       <c r="C59" s="28"/>
-      <c r="D59" s="175" t="s">
+      <c r="D59" s="176" t="s">
         <v>87</v>
       </c>
-      <c r="E59" s="176"/>
-      <c r="F59" s="177"/>
+      <c r="E59" s="177"/>
+      <c r="F59" s="178"/>
       <c r="G59" s="29">
         <f>SUM(H13:H26)+SUM(H29:H40)+SUM(H43:H52)+SUM(H55:H56)</f>
         <v>0</v>
@@ -9285,13 +9314,13 @@
       <c r="N59" s="13"/>
     </row>
     <row r="60" spans="1:17" ht="48" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="170"/>
-      <c r="B60" s="171"/>
+      <c r="A60" s="171"/>
+      <c r="B60" s="172"/>
       <c r="C60" s="31"/>
-      <c r="D60" s="172" t="s">
+      <c r="D60" s="173" t="s">
         <v>55</v>
       </c>
-      <c r="E60" s="173"/>
+      <c r="E60" s="174"/>
       <c r="F60" s="32"/>
       <c r="G60" s="33"/>
       <c r="H60" s="34"/>
@@ -9303,13 +9332,13 @@
       <c r="N60" s="13"/>
     </row>
     <row r="61" spans="1:17" ht="55.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="170"/>
-      <c r="B61" s="171"/>
+      <c r="A61" s="171"/>
+      <c r="B61" s="172"/>
       <c r="C61" s="31"/>
-      <c r="D61" s="172" t="s">
+      <c r="D61" s="173" t="s">
         <v>56</v>
       </c>
-      <c r="E61" s="173"/>
+      <c r="E61" s="174"/>
       <c r="F61" s="32"/>
       <c r="G61" s="33"/>
       <c r="H61" s="34"/>
@@ -9321,13 +9350,13 @@
       <c r="N61" s="13"/>
     </row>
     <row r="62" spans="1:17" ht="39.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="170"/>
-      <c r="B62" s="171"/>
+      <c r="A62" s="171"/>
+      <c r="B62" s="172"/>
       <c r="C62" s="35"/>
-      <c r="D62" s="174" t="s">
+      <c r="D62" s="175" t="s">
         <v>57</v>
       </c>
-      <c r="E62" s="173"/>
+      <c r="E62" s="174"/>
       <c r="F62" s="32"/>
       <c r="G62" s="33"/>
       <c r="H62" s="34"/>
@@ -9346,11 +9375,11 @@
         <f>SUM(H13:H26)+SUM(H29:H40)+SUM(H43:H52)+SUM(H55:H56)</f>
         <v>0</v>
       </c>
-      <c r="E63" s="166" t="s">
+      <c r="E63" s="167" t="s">
         <v>154</v>
       </c>
-      <c r="F63" s="166"/>
-      <c r="G63" s="167"/>
+      <c r="F63" s="167"/>
+      <c r="G63" s="168"/>
       <c r="H63" s="43"/>
       <c r="I63" s="13"/>
       <c r="J63" s="13"/>
@@ -9360,10 +9389,10 @@
       <c r="N63" s="13"/>
     </row>
     <row r="64" spans="1:17" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="160" t="s">
+      <c r="A64" s="161" t="s">
         <v>58</v>
       </c>
-      <c r="B64" s="161"/>
+      <c r="B64" s="162"/>
       <c r="C64" s="18"/>
       <c r="D64" s="19"/>
       <c r="E64" s="44"/>
@@ -10268,8 +10297,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:T43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -10283,22 +10312,20 @@
     <col min="7" max="7" width="29.5703125" style="2" customWidth="1"/>
     <col min="8" max="8" width="22.7109375" style="2" customWidth="1"/>
     <col min="9" max="9" width="9.140625" style="2" hidden="1" customWidth="1"/>
-    <col min="10" max="13" width="2.42578125" style="2" hidden="1" customWidth="1"/>
-    <col min="14" max="20" width="0" style="2" hidden="1" customWidth="1"/>
-    <col min="21" max="16384" width="2.42578125" style="2" hidden="1"/>
+    <col min="10" max="16384" width="2.42578125" style="2" hidden="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" s="8" customFormat="1" ht="25.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="215" t="s">
+      <c r="A1" s="216" t="s">
         <v>82</v>
       </c>
-      <c r="B1" s="216"/>
-      <c r="C1" s="216"/>
-      <c r="D1" s="216"/>
-      <c r="E1" s="216"/>
-      <c r="F1" s="216"/>
-      <c r="G1" s="216"/>
-      <c r="H1" s="217"/>
+      <c r="B1" s="217"/>
+      <c r="C1" s="217"/>
+      <c r="D1" s="217"/>
+      <c r="E1" s="217"/>
+      <c r="F1" s="217"/>
+      <c r="G1" s="217"/>
+      <c r="H1" s="218"/>
       <c r="I1" s="10"/>
       <c r="J1" s="10"/>
       <c r="K1" s="10"/>
@@ -10310,16 +10337,16 @@
       <c r="Q1" s="9"/>
     </row>
     <row r="2" spans="1:20" s="4" customFormat="1" ht="60.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="214" t="s">
+      <c r="A2" s="215" t="s">
         <v>200</v>
       </c>
-      <c r="B2" s="214"/>
-      <c r="C2" s="214"/>
-      <c r="D2" s="214"/>
-      <c r="E2" s="214"/>
-      <c r="F2" s="214"/>
-      <c r="G2" s="214"/>
-      <c r="H2" s="214"/>
+      <c r="B2" s="215"/>
+      <c r="C2" s="215"/>
+      <c r="D2" s="215"/>
+      <c r="E2" s="215"/>
+      <c r="F2" s="215"/>
+      <c r="G2" s="215"/>
+      <c r="H2" s="215"/>
       <c r="I2" s="7"/>
       <c r="J2" s="5"/>
       <c r="K2" s="5"/>
@@ -10369,7 +10396,9 @@
       <c r="C4" s="142"/>
       <c r="D4" s="137"/>
       <c r="E4" s="138"/>
-      <c r="F4" s="139"/>
+      <c r="F4" s="139" t="s">
+        <v>252</v>
+      </c>
       <c r="G4" s="140"/>
       <c r="H4" s="141"/>
       <c r="L4" s="118" t="s">
@@ -10391,8 +10420,8 @@
       <c r="F5" s="134"/>
       <c r="G5" s="135"/>
       <c r="H5" s="141"/>
-      <c r="L5" s="119" t="s">
-        <v>140</v>
+      <c r="L5" s="160" t="s">
+        <v>252</v>
       </c>
       <c r="M5" s="117" t="s">
         <v>69</v>
@@ -10401,7 +10430,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="6" spans="1:20" s="117" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:20" s="117" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="114"/>
       <c r="B6" s="133"/>
       <c r="C6" s="143"/>
@@ -10410,6 +10439,9 @@
       <c r="F6" s="134"/>
       <c r="G6" s="135"/>
       <c r="H6" s="135"/>
+      <c r="L6" s="119" t="s">
+        <v>140</v>
+      </c>
       <c r="M6" s="117" t="s">
         <v>68</v>
       </c>
@@ -10907,7 +10939,7 @@
       <formula1>$O$2:$O$38</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4:F12 F23:F39" xr:uid="{00000000-0002-0000-0300-000002000000}">
-      <formula1>$L$3:$L$5</formula1>
+      <formula1>$L$3:$L$6</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.25" right="0.25" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -10919,6 +10951,27 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="039bc2d6-e16a-4b4d-b61d-73ee5a6b5720"/>
+    <n8bc46b862004554b29f25437dcecdb2 xmlns="93977a9a-7c70-4c47-a38b-6f123b62dce6">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </n8bc46b862004554b29f25437dcecdb2>
+    <Fiscal_x0020_Year xmlns="17eb8759-252b-418d-a649-70aff91fc5df" xsi:nil="true"/>
+    <Archive xmlns="17eb8759-252b-418d-a649-70aff91fc5df">false</Archive>
+    <b348aa9236b94ac88332be997039b018 xmlns="17eb8759-252b-418d-a649-70aff91fc5df">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </b348aa9236b94ac88332be997039b018>
+    <_dlc_DocId xmlns="039bc2d6-e16a-4b4d-b61d-73ee5a6b5720">QWPW5C3C64YX-694079015-91</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="039bc2d6-e16a-4b4d-b61d-73ee5a6b5720">
+      <Url>http://cscgikdcapmdw40/ProjectsLab/AODACompliance/_layouts/15/DocIdRedir.aspx?ID=QWPW5C3C64YX-694079015-91</Url>
+      <Description>QWPW5C3C64YX-694079015-91</Description>
+    </_dlc_DocIdUrl>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
   <Receiver>
@@ -10968,7 +11021,7 @@
 </spe:Receivers>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001B7F6C1E041661428C0804F60FDF9579" ma:contentTypeVersion="1" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="269e77b516f09928499b1be999970057">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="17eb8759-252b-418d-a649-70aff91fc5df" xmlns:ns3="039bc2d6-e16a-4b4d-b61d-73ee5a6b5720" xmlns:ns4="93977a9a-7c70-4c47-a38b-6f123b62dce6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="41b65eea62d023978f15f5547645abd7" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="17eb8759-252b-418d-a649-70aff91fc5df"/>
@@ -11189,7 +11242,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -11198,28 +11251,25 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="039bc2d6-e16a-4b4d-b61d-73ee5a6b5720"/>
-    <n8bc46b862004554b29f25437dcecdb2 xmlns="93977a9a-7c70-4c47-a38b-6f123b62dce6">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </n8bc46b862004554b29f25437dcecdb2>
-    <Fiscal_x0020_Year xmlns="17eb8759-252b-418d-a649-70aff91fc5df" xsi:nil="true"/>
-    <Archive xmlns="17eb8759-252b-418d-a649-70aff91fc5df">false</Archive>
-    <b348aa9236b94ac88332be997039b018 xmlns="17eb8759-252b-418d-a649-70aff91fc5df">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </b348aa9236b94ac88332be997039b018>
-    <_dlc_DocId xmlns="039bc2d6-e16a-4b4d-b61d-73ee5a6b5720">QWPW5C3C64YX-694079015-91</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="039bc2d6-e16a-4b4d-b61d-73ee5a6b5720">
-      <Url>http://cscgikdcapmdw40/ProjectsLab/AODACompliance/_layouts/15/DocIdRedir.aspx?ID=QWPW5C3C64YX-694079015-91</Url>
-      <Description>QWPW5C3C64YX-694079015-91</Description>
-    </_dlc_DocIdUrl>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C507B214-A4AD-4147-9668-C65BAB18F1D2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="93977a9a-7c70-4c47-a38b-6f123b62dce6"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="039bc2d6-e16a-4b4d-b61d-73ee5a6b5720"/>
+    <ds:schemaRef ds:uri="17eb8759-252b-418d-a649-70aff91fc5df"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2E5D2D22-6D00-46CD-B7EA-B8CE8E1546D9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
@@ -11227,7 +11277,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3C5CD16F-1A82-4BAB-88E6-9D42833A2748}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11247,28 +11297,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D6D3747C-BDC7-48F7-9B5A-BD9117F21569}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C507B214-A4AD-4147-9668-C65BAB18F1D2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="17eb8759-252b-418d-a649-70aff91fc5df"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="93977a9a-7c70-4c47-a38b-6f123b62dce6"/>
-    <ds:schemaRef ds:uri="039bc2d6-e16a-4b4d-b61d-73ee5a6b5720"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Removed level column as it is now static data
</commit_message>
<xml_diff>
--- a/AxeAccessibilityDriver/AxeAccessibilityDriver/AODA_Template.xlsx
+++ b/AxeAccessibilityDriver/AxeAccessibilityDriver/AODA_Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DUONGCH\Projects\AxeAccessibilityDriver\AxeAccessibilityDriver\AxeAccessibilityDriver\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{022454C8-B3EE-4128-9E4E-65EA85C1CAF0}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C951448F-29A6-4435-B53C-E5186062A37C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="760" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" tabRatio="760" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="5" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="255">
   <si>
     <t>1.1.1</t>
   </si>
@@ -2433,6 +2433,12 @@
   </si>
   <si>
     <t>Medium</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>AA</t>
   </si>
 </sst>
 </file>
@@ -3726,22 +3732,121 @@
     <xf numFmtId="0" fontId="49" fillId="13" borderId="0" xfId="16" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="167" fontId="13" fillId="5" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="27" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -3784,105 +3889,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="27" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="13" fillId="5" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="2" borderId="25" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -7825,8 +7831,8 @@
   </sheetPr>
   <dimension ref="A1:XFC81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="115" zoomScalePageLayoutView="160" workbookViewId="0">
-      <selection activeCell="XFD1" sqref="F1:XFD1048576"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="115" zoomScalePageLayoutView="160" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="12.75" zeroHeight="1" x14ac:dyDescent="0.2"/>
@@ -7851,16 +7857,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="13" customFormat="1" ht="37.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="185" t="s">
+      <c r="A1" s="178" t="s">
         <v>225</v>
       </c>
-      <c r="B1" s="185"/>
-      <c r="C1" s="185"/>
-      <c r="D1" s="185"/>
-      <c r="E1" s="185"/>
-      <c r="F1" s="185"/>
-      <c r="G1" s="185"/>
-      <c r="H1" s="186"/>
+      <c r="B1" s="178"/>
+      <c r="C1" s="178"/>
+      <c r="D1" s="178"/>
+      <c r="E1" s="178"/>
+      <c r="F1" s="178"/>
+      <c r="G1" s="178"/>
+      <c r="H1" s="179"/>
       <c r="I1" s="11"/>
       <c r="J1" s="12"/>
       <c r="K1" s="1"/>
@@ -7874,13 +7880,13 @@
       <c r="S1" s="1"/>
     </row>
     <row r="2" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="166" t="s">
+      <c r="A2" s="180" t="s">
         <v>61</v>
       </c>
-      <c r="B2" s="166"/>
-      <c r="C2" s="189"/>
-      <c r="D2" s="189"/>
-      <c r="E2" s="190"/>
+      <c r="B2" s="180"/>
+      <c r="C2" s="181"/>
+      <c r="D2" s="181"/>
+      <c r="E2" s="182"/>
       <c r="F2" s="39"/>
       <c r="G2" s="1"/>
       <c r="H2" s="16"/>
@@ -7892,13 +7898,13 @@
       <c r="N2" s="13"/>
     </row>
     <row r="3" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="166" t="s">
+      <c r="A3" s="180" t="s">
         <v>63</v>
       </c>
-      <c r="B3" s="166"/>
-      <c r="C3" s="202"/>
-      <c r="D3" s="203"/>
-      <c r="E3" s="204"/>
+      <c r="B3" s="180"/>
+      <c r="C3" s="195"/>
+      <c r="D3" s="196"/>
+      <c r="E3" s="197"/>
       <c r="F3" s="39"/>
       <c r="G3" s="1"/>
       <c r="H3" s="16"/>
@@ -7910,12 +7916,12 @@
       <c r="N3" s="13"/>
     </row>
     <row r="4" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="166" t="s">
+      <c r="A4" s="180" t="s">
         <v>77</v>
       </c>
-      <c r="B4" s="166"/>
-      <c r="C4" s="212"/>
-      <c r="D4" s="212"/>
+      <c r="B4" s="180"/>
+      <c r="C4" s="161"/>
+      <c r="D4" s="161"/>
       <c r="E4" s="91"/>
       <c r="F4" s="39"/>
       <c r="G4" s="1"/>
@@ -7928,13 +7934,13 @@
       <c r="N4" s="13"/>
     </row>
     <row r="5" spans="1:19" ht="27" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="165" t="s">
+      <c r="A5" s="162" t="s">
         <v>78</v>
       </c>
-      <c r="B5" s="165"/>
-      <c r="C5" s="213"/>
-      <c r="D5" s="213"/>
-      <c r="E5" s="214"/>
+      <c r="B5" s="162"/>
+      <c r="C5" s="163"/>
+      <c r="D5" s="163"/>
+      <c r="E5" s="164"/>
       <c r="F5" s="39"/>
       <c r="G5" s="1"/>
       <c r="H5" s="16"/>
@@ -7946,13 +7952,13 @@
       <c r="N5" s="13"/>
     </row>
     <row r="6" spans="1:19" ht="27" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="165" t="s">
+      <c r="A6" s="162" t="s">
         <v>79</v>
       </c>
-      <c r="B6" s="165"/>
-      <c r="C6" s="163"/>
-      <c r="D6" s="163"/>
-      <c r="E6" s="164"/>
+      <c r="B6" s="162"/>
+      <c r="C6" s="165"/>
+      <c r="D6" s="165"/>
+      <c r="E6" s="166"/>
       <c r="F6" s="39"/>
       <c r="G6" s="1"/>
       <c r="H6" s="16"/>
@@ -7964,13 +7970,13 @@
       <c r="N6" s="13"/>
     </row>
     <row r="7" spans="1:19" ht="27" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="165" t="s">
+      <c r="A7" s="162" t="s">
         <v>80</v>
       </c>
-      <c r="B7" s="165"/>
-      <c r="C7" s="163"/>
-      <c r="D7" s="163"/>
-      <c r="E7" s="164"/>
+      <c r="B7" s="162"/>
+      <c r="C7" s="165"/>
+      <c r="D7" s="165"/>
+      <c r="E7" s="166"/>
       <c r="F7" s="39"/>
       <c r="G7" s="1"/>
       <c r="H7" s="16"/>
@@ -7982,13 +7988,13 @@
       <c r="N7" s="13"/>
     </row>
     <row r="8" spans="1:19" ht="27" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="165" t="s">
+      <c r="A8" s="162" t="s">
         <v>81</v>
       </c>
-      <c r="B8" s="165"/>
-      <c r="C8" s="163"/>
-      <c r="D8" s="163"/>
-      <c r="E8" s="164"/>
+      <c r="B8" s="162"/>
+      <c r="C8" s="165"/>
+      <c r="D8" s="165"/>
+      <c r="E8" s="166"/>
       <c r="F8" s="39"/>
       <c r="G8" s="1"/>
       <c r="H8" s="16"/>
@@ -8000,16 +8006,16 @@
       <c r="N8" s="13"/>
     </row>
     <row r="9" spans="1:19" s="37" customFormat="1" ht="52.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="193" t="s">
+      <c r="A9" s="184" t="s">
         <v>76</v>
       </c>
-      <c r="B9" s="194"/>
-      <c r="C9" s="194"/>
-      <c r="D9" s="194"/>
-      <c r="E9" s="194"/>
-      <c r="F9" s="194"/>
-      <c r="G9" s="194"/>
-      <c r="H9" s="194"/>
+      <c r="B9" s="185"/>
+      <c r="C9" s="185"/>
+      <c r="D9" s="185"/>
+      <c r="E9" s="185"/>
+      <c r="F9" s="185"/>
+      <c r="G9" s="185"/>
+      <c r="H9" s="185"/>
       <c r="I9" s="18"/>
       <c r="J9" s="18"/>
       <c r="K9" s="18"/>
@@ -8019,16 +8025,16 @@
       <c r="Q9" s="108"/>
     </row>
     <row r="10" spans="1:19" s="22" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="195" t="s">
+      <c r="A10" s="186" t="s">
         <v>210</v>
       </c>
-      <c r="B10" s="196"/>
-      <c r="C10" s="196"/>
-      <c r="D10" s="196"/>
-      <c r="E10" s="196"/>
-      <c r="F10" s="196"/>
-      <c r="G10" s="196"/>
-      <c r="H10" s="197"/>
+      <c r="B10" s="187"/>
+      <c r="C10" s="187"/>
+      <c r="D10" s="187"/>
+      <c r="E10" s="187"/>
+      <c r="F10" s="187"/>
+      <c r="G10" s="187"/>
+      <c r="H10" s="188"/>
       <c r="I10" s="21"/>
       <c r="J10" s="21"/>
       <c r="K10" s="21"/>
@@ -8038,10 +8044,10 @@
       <c r="Q10" s="23"/>
     </row>
     <row r="11" spans="1:19" ht="55.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="200" t="s">
+      <c r="A11" s="193" t="s">
         <v>54</v>
       </c>
-      <c r="B11" s="201"/>
+      <c r="B11" s="194"/>
       <c r="C11" s="123" t="s">
         <v>40</v>
       </c>
@@ -8051,10 +8057,10 @@
       <c r="E11" s="123" t="s">
         <v>99</v>
       </c>
-      <c r="F11" s="199" t="s">
+      <c r="F11" s="189" t="s">
         <v>52</v>
       </c>
-      <c r="G11" s="199"/>
+      <c r="G11" s="189"/>
       <c r="H11" s="124" t="s">
         <v>53</v>
       </c>
@@ -8066,18 +8072,18 @@
       <c r="N11" s="13"/>
     </row>
     <row r="12" spans="1:19" ht="69.599999999999994" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="191" t="s">
+      <c r="A12" s="172" t="s">
         <v>83</v>
       </c>
-      <c r="B12" s="192"/>
-      <c r="C12" s="182" t="s">
+      <c r="B12" s="183"/>
+      <c r="C12" s="190" t="s">
         <v>179</v>
       </c>
-      <c r="D12" s="183"/>
-      <c r="E12" s="183"/>
-      <c r="F12" s="183"/>
-      <c r="G12" s="183"/>
-      <c r="H12" s="184"/>
+      <c r="D12" s="191"/>
+      <c r="E12" s="191"/>
+      <c r="F12" s="191"/>
+      <c r="G12" s="191"/>
+      <c r="H12" s="192"/>
       <c r="I12" s="13"/>
       <c r="J12" s="13"/>
       <c r="K12" s="13"/>
@@ -8092,7 +8098,9 @@
       <c r="B13" s="93" t="s">
         <v>41</v>
       </c>
-      <c r="C13" s="94"/>
+      <c r="C13" s="94" t="s">
+        <v>253</v>
+      </c>
       <c r="D13" s="95"/>
       <c r="E13"/>
       <c r="F13" s="97">
@@ -8119,7 +8127,9 @@
       <c r="B14" s="93" t="s">
         <v>42</v>
       </c>
-      <c r="C14" s="94"/>
+      <c r="C14" s="94" t="s">
+        <v>253</v>
+      </c>
       <c r="D14" s="95"/>
       <c r="E14"/>
       <c r="F14" s="97">
@@ -8146,7 +8156,9 @@
       <c r="B15" s="93" t="s">
         <v>152</v>
       </c>
-      <c r="C15" s="94"/>
+      <c r="C15" s="94" t="s">
+        <v>253</v>
+      </c>
       <c r="D15" s="95"/>
       <c r="E15"/>
       <c r="F15" s="97">
@@ -8173,7 +8185,9 @@
       <c r="B16" s="93" t="s">
         <v>43</v>
       </c>
-      <c r="C16" s="94"/>
+      <c r="C16" s="94" t="s">
+        <v>253</v>
+      </c>
       <c r="D16" s="95"/>
       <c r="E16"/>
       <c r="F16" s="97">
@@ -8200,7 +8214,9 @@
       <c r="B17" s="93" t="s">
         <v>44</v>
       </c>
-      <c r="C17" s="94"/>
+      <c r="C17" s="94" t="s">
+        <v>254</v>
+      </c>
       <c r="D17" s="95"/>
       <c r="E17"/>
       <c r="F17" s="97">
@@ -8227,7 +8243,9 @@
       <c r="B18" s="93" t="s">
         <v>45</v>
       </c>
-      <c r="C18" s="94"/>
+      <c r="C18" s="94" t="s">
+        <v>254</v>
+      </c>
       <c r="D18" s="95"/>
       <c r="E18"/>
       <c r="F18" s="97">
@@ -8254,7 +8272,9 @@
       <c r="B19" s="93" t="s">
         <v>224</v>
       </c>
-      <c r="C19" s="94"/>
+      <c r="C19" s="94" t="s">
+        <v>253</v>
+      </c>
       <c r="D19" s="95"/>
       <c r="E19"/>
       <c r="F19" s="97">
@@ -8283,7 +8303,9 @@
       <c r="B20" s="93" t="s">
         <v>180</v>
       </c>
-      <c r="C20" s="94"/>
+      <c r="C20" s="94" t="s">
+        <v>253</v>
+      </c>
       <c r="D20" s="95"/>
       <c r="E20"/>
       <c r="F20" s="97">
@@ -8312,7 +8334,9 @@
       <c r="B21" s="93" t="s">
         <v>181</v>
       </c>
-      <c r="C21" s="94"/>
+      <c r="C21" s="94" t="s">
+        <v>253</v>
+      </c>
       <c r="D21" s="95"/>
       <c r="E21"/>
       <c r="F21" s="97">
@@ -8341,7 +8365,9 @@
       <c r="B22" s="93" t="s">
         <v>46</v>
       </c>
-      <c r="C22" s="94"/>
+      <c r="C22" s="94" t="s">
+        <v>253</v>
+      </c>
       <c r="D22" s="95"/>
       <c r="E22"/>
       <c r="F22" s="97">
@@ -8370,7 +8396,9 @@
       <c r="B23" s="93" t="s">
         <v>201</v>
       </c>
-      <c r="C23" s="94"/>
+      <c r="C23" s="94" t="s">
+        <v>253</v>
+      </c>
       <c r="D23" s="95"/>
       <c r="E23"/>
       <c r="F23" s="97">
@@ -8397,7 +8425,9 @@
       <c r="B24" s="103" t="s">
         <v>182</v>
       </c>
-      <c r="C24" s="94"/>
+      <c r="C24" s="94" t="s">
+        <v>254</v>
+      </c>
       <c r="D24" s="95"/>
       <c r="E24"/>
       <c r="F24" s="97">
@@ -8426,7 +8456,9 @@
       <c r="B25" s="93" t="s">
         <v>183</v>
       </c>
-      <c r="C25" s="94"/>
+      <c r="C25" s="94" t="s">
+        <v>254</v>
+      </c>
       <c r="D25" s="95"/>
       <c r="E25"/>
       <c r="F25" s="97">
@@ -8453,7 +8485,9 @@
       <c r="B26" s="104" t="s">
         <v>184</v>
       </c>
-      <c r="C26" s="94"/>
+      <c r="C26" s="94" t="s">
+        <v>254</v>
+      </c>
       <c r="D26" s="95"/>
       <c r="E26"/>
       <c r="F26" s="97">
@@ -8474,14 +8508,14 @@
       <c r="Q26" s="102"/>
     </row>
     <row r="27" spans="1:17" ht="17.45" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="187" t="s">
+      <c r="A27" s="176" t="s">
         <v>67</v>
       </c>
-      <c r="B27" s="188"/>
-      <c r="C27" s="188"/>
-      <c r="D27" s="188"/>
-      <c r="E27" s="188"/>
-      <c r="F27" s="188"/>
+      <c r="B27" s="177"/>
+      <c r="C27" s="177"/>
+      <c r="D27" s="177"/>
+      <c r="E27" s="177"/>
+      <c r="F27" s="177"/>
       <c r="G27" s="24">
         <f>SUM(H13:H26)</f>
         <v>0</v>
@@ -8498,18 +8532,18 @@
       <c r="N27" s="13"/>
     </row>
     <row r="28" spans="1:17" ht="53.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="191" t="s">
+      <c r="A28" s="172" t="s">
         <v>84</v>
       </c>
-      <c r="B28" s="198"/>
-      <c r="C28" s="182" t="s">
+      <c r="B28" s="173"/>
+      <c r="C28" s="190" t="s">
         <v>185</v>
       </c>
-      <c r="D28" s="183"/>
-      <c r="E28" s="183"/>
-      <c r="F28" s="183"/>
-      <c r="G28" s="183"/>
-      <c r="H28" s="184"/>
+      <c r="D28" s="191"/>
+      <c r="E28" s="191"/>
+      <c r="F28" s="191"/>
+      <c r="G28" s="191"/>
+      <c r="H28" s="192"/>
       <c r="I28" s="13"/>
       <c r="J28" s="13"/>
       <c r="K28" s="13"/>
@@ -8524,7 +8558,9 @@
       <c r="B29" s="93" t="s">
         <v>47</v>
       </c>
-      <c r="C29" s="94"/>
+      <c r="C29" s="94" t="s">
+        <v>253</v>
+      </c>
       <c r="D29" s="95"/>
       <c r="E29"/>
       <c r="F29" s="97">
@@ -8551,7 +8587,9 @@
       <c r="B30" s="93" t="s">
         <v>202</v>
       </c>
-      <c r="C30" s="94"/>
+      <c r="C30" s="94" t="s">
+        <v>253</v>
+      </c>
       <c r="D30" s="95"/>
       <c r="E30"/>
       <c r="F30" s="97">
@@ -8578,7 +8616,9 @@
       <c r="B31" s="93" t="s">
         <v>62</v>
       </c>
-      <c r="C31" s="94"/>
+      <c r="C31" s="94" t="s">
+        <v>253</v>
+      </c>
       <c r="D31" s="95"/>
       <c r="E31"/>
       <c r="F31" s="97">
@@ -8605,7 +8645,9 @@
       <c r="B32" s="93" t="s">
         <v>203</v>
       </c>
-      <c r="C32" s="94"/>
+      <c r="C32" s="94" t="s">
+        <v>253</v>
+      </c>
       <c r="D32" s="95"/>
       <c r="E32"/>
       <c r="F32" s="97"/>
@@ -8629,7 +8671,9 @@
       <c r="B33" s="93" t="s">
         <v>186</v>
       </c>
-      <c r="C33" s="94"/>
+      <c r="C33" s="94" t="s">
+        <v>253</v>
+      </c>
       <c r="D33" s="95"/>
       <c r="E33"/>
       <c r="F33" s="97">
@@ -8656,7 +8700,9 @@
       <c r="B34" s="93" t="s">
         <v>187</v>
       </c>
-      <c r="C34" s="94"/>
+      <c r="C34" s="94" t="s">
+        <v>253</v>
+      </c>
       <c r="D34" s="95"/>
       <c r="E34"/>
       <c r="F34" s="97">
@@ -8683,7 +8729,9 @@
       <c r="B35" s="93" t="s">
         <v>204</v>
       </c>
-      <c r="C35" s="94"/>
+      <c r="C35" s="94" t="s">
+        <v>253</v>
+      </c>
       <c r="D35" s="95"/>
       <c r="E35"/>
       <c r="F35" s="97">
@@ -8710,7 +8758,9 @@
       <c r="B36" s="93" t="s">
         <v>188</v>
       </c>
-      <c r="C36" s="94"/>
+      <c r="C36" s="94" t="s">
+        <v>253</v>
+      </c>
       <c r="D36" s="95"/>
       <c r="E36"/>
       <c r="F36" s="97">
@@ -8737,7 +8787,9 @@
       <c r="B37" s="93" t="s">
         <v>48</v>
       </c>
-      <c r="C37" s="94"/>
+      <c r="C37" s="94" t="s">
+        <v>253</v>
+      </c>
       <c r="D37" s="95"/>
       <c r="E37"/>
       <c r="F37" s="97">
@@ -8764,7 +8816,9 @@
       <c r="B38" s="93" t="s">
         <v>189</v>
       </c>
-      <c r="C38" s="94"/>
+      <c r="C38" s="94" t="s">
+        <v>254</v>
+      </c>
       <c r="D38" s="95"/>
       <c r="E38"/>
       <c r="F38" s="97">
@@ -8791,7 +8845,9 @@
       <c r="B39" s="93" t="s">
         <v>205</v>
       </c>
-      <c r="C39" s="94"/>
+      <c r="C39" s="94" t="s">
+        <v>254</v>
+      </c>
       <c r="D39" s="95"/>
       <c r="E39"/>
       <c r="F39" s="97">
@@ -8818,7 +8874,9 @@
       <c r="B40" s="93" t="s">
         <v>49</v>
       </c>
-      <c r="C40" s="94"/>
+      <c r="C40" s="94" t="s">
+        <v>254</v>
+      </c>
       <c r="D40" s="95"/>
       <c r="E40"/>
       <c r="F40" s="97">
@@ -8839,14 +8897,14 @@
       <c r="Q40" s="102"/>
     </row>
     <row r="41" spans="1:17" ht="48.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="187" t="s">
+      <c r="A41" s="176" t="s">
         <v>66</v>
       </c>
-      <c r="B41" s="188"/>
-      <c r="C41" s="188"/>
-      <c r="D41" s="188"/>
-      <c r="E41" s="188"/>
-      <c r="F41" s="188"/>
+      <c r="B41" s="177"/>
+      <c r="C41" s="177"/>
+      <c r="D41" s="177"/>
+      <c r="E41" s="177"/>
+      <c r="F41" s="177"/>
       <c r="G41" s="24">
         <f>SUM(H29:H40)</f>
         <v>0</v>
@@ -8863,18 +8921,18 @@
       <c r="N41" s="13"/>
     </row>
     <row r="42" spans="1:17" ht="54.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="191" t="s">
+      <c r="A42" s="172" t="s">
         <v>85</v>
       </c>
-      <c r="B42" s="198"/>
-      <c r="C42" s="182" t="s">
+      <c r="B42" s="173"/>
+      <c r="C42" s="190" t="s">
         <v>190</v>
       </c>
-      <c r="D42" s="183"/>
-      <c r="E42" s="183"/>
-      <c r="F42" s="183"/>
-      <c r="G42" s="183"/>
-      <c r="H42" s="184"/>
+      <c r="D42" s="191"/>
+      <c r="E42" s="191"/>
+      <c r="F42" s="191"/>
+      <c r="G42" s="191"/>
+      <c r="H42" s="192"/>
       <c r="I42" s="13"/>
       <c r="J42" s="13"/>
       <c r="K42" s="13"/>
@@ -8889,7 +8947,9 @@
       <c r="B43" s="93" t="s">
         <v>191</v>
       </c>
-      <c r="C43" s="94"/>
+      <c r="C43" s="94" t="s">
+        <v>253</v>
+      </c>
       <c r="D43" s="95"/>
       <c r="E43"/>
       <c r="F43" s="97">
@@ -8916,7 +8976,9 @@
       <c r="B44" s="93" t="s">
         <v>38</v>
       </c>
-      <c r="C44" s="94"/>
+      <c r="C44" s="94" t="s">
+        <v>254</v>
+      </c>
       <c r="D44" s="95"/>
       <c r="E44"/>
       <c r="F44" s="97">
@@ -8943,7 +9005,9 @@
       <c r="B45" s="93" t="s">
         <v>206</v>
       </c>
-      <c r="C45" s="94"/>
+      <c r="C45" s="94" t="s">
+        <v>253</v>
+      </c>
       <c r="D45" s="95"/>
       <c r="E45"/>
       <c r="F45" s="97">
@@ -8970,7 +9034,9 @@
       <c r="B46" s="93" t="s">
         <v>192</v>
       </c>
-      <c r="C46" s="94"/>
+      <c r="C46" s="94" t="s">
+        <v>253</v>
+      </c>
       <c r="D46" s="95"/>
       <c r="E46"/>
       <c r="F46" s="97">
@@ -8997,7 +9063,9 @@
       <c r="B47" s="93" t="s">
         <v>193</v>
       </c>
-      <c r="C47" s="94"/>
+      <c r="C47" s="94" t="s">
+        <v>254</v>
+      </c>
       <c r="D47" s="95"/>
       <c r="E47"/>
       <c r="F47" s="97">
@@ -9024,7 +9092,9 @@
       <c r="B48" s="93" t="s">
         <v>194</v>
       </c>
-      <c r="C48" s="94"/>
+      <c r="C48" s="94" t="s">
+        <v>254</v>
+      </c>
       <c r="D48" s="95"/>
       <c r="E48"/>
       <c r="F48" s="97">
@@ -9051,7 +9121,9 @@
       <c r="B49" s="93" t="s">
         <v>207</v>
       </c>
-      <c r="C49" s="94"/>
+      <c r="C49" s="94" t="s">
+        <v>253</v>
+      </c>
       <c r="D49" s="95"/>
       <c r="E49"/>
       <c r="F49" s="97">
@@ -9078,7 +9150,9 @@
       <c r="B50" s="93" t="s">
         <v>208</v>
       </c>
-      <c r="C50" s="94"/>
+      <c r="C50" s="94" t="s">
+        <v>253</v>
+      </c>
       <c r="D50" s="95"/>
       <c r="E50"/>
       <c r="F50" s="97">
@@ -9105,7 +9179,9 @@
       <c r="B51" s="93" t="s">
         <v>209</v>
       </c>
-      <c r="C51" s="94"/>
+      <c r="C51" s="94" t="s">
+        <v>254</v>
+      </c>
       <c r="D51" s="95"/>
       <c r="E51"/>
       <c r="F51" s="97">
@@ -9132,7 +9208,9 @@
       <c r="B52" s="93" t="s">
         <v>195</v>
       </c>
-      <c r="C52" s="94"/>
+      <c r="C52" s="94" t="s">
+        <v>254</v>
+      </c>
       <c r="D52" s="95"/>
       <c r="E52"/>
       <c r="F52" s="97">
@@ -9153,14 +9231,14 @@
       <c r="Q52" s="102"/>
     </row>
     <row r="53" spans="1:17" ht="74.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="187" t="s">
+      <c r="A53" s="176" t="s">
         <v>65</v>
       </c>
-      <c r="B53" s="188"/>
-      <c r="C53" s="188"/>
-      <c r="D53" s="188"/>
-      <c r="E53" s="188"/>
-      <c r="F53" s="188"/>
+      <c r="B53" s="177"/>
+      <c r="C53" s="177"/>
+      <c r="D53" s="177"/>
+      <c r="E53" s="177"/>
+      <c r="F53" s="177"/>
       <c r="G53" s="25">
         <f>SUM(H43:H52)</f>
         <v>0</v>
@@ -9177,18 +9255,18 @@
       <c r="N53" s="13"/>
     </row>
     <row r="54" spans="1:17" ht="47.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="208" t="s">
+      <c r="A54" s="170" t="s">
         <v>86</v>
       </c>
-      <c r="B54" s="209"/>
-      <c r="C54" s="205" t="s">
+      <c r="B54" s="171"/>
+      <c r="C54" s="167" t="s">
         <v>196</v>
       </c>
-      <c r="D54" s="206"/>
-      <c r="E54" s="206"/>
-      <c r="F54" s="206"/>
-      <c r="G54" s="206"/>
-      <c r="H54" s="207"/>
+      <c r="D54" s="168"/>
+      <c r="E54" s="168"/>
+      <c r="F54" s="168"/>
+      <c r="G54" s="168"/>
+      <c r="H54" s="169"/>
       <c r="I54" s="13"/>
       <c r="J54" s="13"/>
       <c r="K54" s="13"/>
@@ -9203,7 +9281,9 @@
       <c r="B55" s="105" t="s">
         <v>50</v>
       </c>
-      <c r="C55" s="94"/>
+      <c r="C55" s="94" t="s">
+        <v>253</v>
+      </c>
       <c r="D55" s="95"/>
       <c r="E55"/>
       <c r="F55" s="97">
@@ -9230,7 +9310,9 @@
       <c r="B56" s="105" t="s">
         <v>51</v>
       </c>
-      <c r="C56" s="94"/>
+      <c r="C56" s="94" t="s">
+        <v>253</v>
+      </c>
       <c r="D56" s="95"/>
       <c r="E56"/>
       <c r="F56" s="97">
@@ -9251,14 +9333,14 @@
       <c r="Q56" s="102"/>
     </row>
     <row r="57" spans="1:17" ht="43.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="187" t="s">
+      <c r="A57" s="176" t="s">
         <v>64</v>
       </c>
-      <c r="B57" s="188"/>
-      <c r="C57" s="188"/>
-      <c r="D57" s="188"/>
-      <c r="E57" s="188"/>
-      <c r="F57" s="188"/>
+      <c r="B57" s="177"/>
+      <c r="C57" s="177"/>
+      <c r="D57" s="177"/>
+      <c r="E57" s="177"/>
+      <c r="F57" s="177"/>
       <c r="G57" s="24">
         <f>SUM(H55:H56)</f>
         <v>0</v>
@@ -9275,16 +9357,16 @@
       <c r="N57" s="13"/>
     </row>
     <row r="58" spans="1:17" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="210" t="s">
+      <c r="A58" s="174" t="s">
         <v>88</v>
       </c>
-      <c r="B58" s="211"/>
-      <c r="C58" s="211"/>
-      <c r="D58" s="211"/>
-      <c r="E58" s="211"/>
-      <c r="F58" s="179"/>
-      <c r="G58" s="180"/>
-      <c r="H58" s="181"/>
+      <c r="B58" s="175"/>
+      <c r="C58" s="175"/>
+      <c r="D58" s="175"/>
+      <c r="E58" s="175"/>
+      <c r="F58" s="212"/>
+      <c r="G58" s="213"/>
+      <c r="H58" s="214"/>
       <c r="I58" s="13"/>
       <c r="J58" s="13"/>
       <c r="K58" s="13"/>
@@ -9293,14 +9375,14 @@
       <c r="N58" s="13"/>
     </row>
     <row r="59" spans="1:17" ht="24.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A59" s="169"/>
-      <c r="B59" s="170"/>
+      <c r="A59" s="202"/>
+      <c r="B59" s="203"/>
       <c r="C59" s="28"/>
-      <c r="D59" s="176" t="s">
+      <c r="D59" s="209" t="s">
         <v>87</v>
       </c>
-      <c r="E59" s="177"/>
-      <c r="F59" s="178"/>
+      <c r="E59" s="210"/>
+      <c r="F59" s="211"/>
       <c r="G59" s="29">
         <f>SUM(H13:H26)+SUM(H29:H40)+SUM(H43:H52)+SUM(H55:H56)</f>
         <v>0</v>
@@ -9314,13 +9396,13 @@
       <c r="N59" s="13"/>
     </row>
     <row r="60" spans="1:17" ht="48" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="171"/>
-      <c r="B60" s="172"/>
+      <c r="A60" s="204"/>
+      <c r="B60" s="205"/>
       <c r="C60" s="31"/>
-      <c r="D60" s="173" t="s">
+      <c r="D60" s="206" t="s">
         <v>55</v>
       </c>
-      <c r="E60" s="174"/>
+      <c r="E60" s="207"/>
       <c r="F60" s="32"/>
       <c r="G60" s="33"/>
       <c r="H60" s="34"/>
@@ -9332,13 +9414,13 @@
       <c r="N60" s="13"/>
     </row>
     <row r="61" spans="1:17" ht="55.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="171"/>
-      <c r="B61" s="172"/>
+      <c r="A61" s="204"/>
+      <c r="B61" s="205"/>
       <c r="C61" s="31"/>
-      <c r="D61" s="173" t="s">
+      <c r="D61" s="206" t="s">
         <v>56</v>
       </c>
-      <c r="E61" s="174"/>
+      <c r="E61" s="207"/>
       <c r="F61" s="32"/>
       <c r="G61" s="33"/>
       <c r="H61" s="34"/>
@@ -9350,13 +9432,13 @@
       <c r="N61" s="13"/>
     </row>
     <row r="62" spans="1:17" ht="39.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="171"/>
-      <c r="B62" s="172"/>
+      <c r="A62" s="204"/>
+      <c r="B62" s="205"/>
       <c r="C62" s="35"/>
-      <c r="D62" s="175" t="s">
+      <c r="D62" s="208" t="s">
         <v>57</v>
       </c>
-      <c r="E62" s="174"/>
+      <c r="E62" s="207"/>
       <c r="F62" s="32"/>
       <c r="G62" s="33"/>
       <c r="H62" s="34"/>
@@ -9375,11 +9457,11 @@
         <f>SUM(H13:H26)+SUM(H29:H40)+SUM(H43:H52)+SUM(H55:H56)</f>
         <v>0</v>
       </c>
-      <c r="E63" s="167" t="s">
+      <c r="E63" s="200" t="s">
         <v>154</v>
       </c>
-      <c r="F63" s="167"/>
-      <c r="G63" s="168"/>
+      <c r="F63" s="200"/>
+      <c r="G63" s="201"/>
       <c r="H63" s="43"/>
       <c r="I63" s="13"/>
       <c r="J63" s="13"/>
@@ -9389,10 +9471,10 @@
       <c r="N63" s="13"/>
     </row>
     <row r="64" spans="1:17" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="161" t="s">
+      <c r="A64" s="198" t="s">
         <v>58</v>
       </c>
-      <c r="B64" s="162"/>
+      <c r="B64" s="199"/>
       <c r="C64" s="18"/>
       <c r="D64" s="19"/>
       <c r="E64" s="44"/>
@@ -9466,17 +9548,22 @@
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
   <mergeCells count="43">
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="C54:H54"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="A58:E58"/>
-    <mergeCell ref="A57:F57"/>
-    <mergeCell ref="A53:F53"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="E63:G63"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="D60:E60"/>
+    <mergeCell ref="D61:E61"/>
+    <mergeCell ref="D62:E62"/>
+    <mergeCell ref="D59:F59"/>
+    <mergeCell ref="F58:H58"/>
+    <mergeCell ref="C42:H42"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="A41:F41"/>
     <mergeCell ref="A2:B2"/>
@@ -9493,22 +9580,17 @@
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="C3:E3"/>
     <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="E63:G63"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="D60:E60"/>
-    <mergeCell ref="D61:E61"/>
-    <mergeCell ref="D62:E62"/>
-    <mergeCell ref="D59:F59"/>
-    <mergeCell ref="F58:H58"/>
-    <mergeCell ref="C42:H42"/>
+    <mergeCell ref="C54:H54"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="A58:E58"/>
+    <mergeCell ref="A57:F57"/>
+    <mergeCell ref="A53:F53"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:E6"/>
   </mergeCells>
   <conditionalFormatting sqref="F43:F52 F55:F56 F13:F26 F29:F40">
     <cfRule type="cellIs" dxfId="136" priority="371" operator="equal">
@@ -10951,77 +11033,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="039bc2d6-e16a-4b4d-b61d-73ee5a6b5720"/>
-    <n8bc46b862004554b29f25437dcecdb2 xmlns="93977a9a-7c70-4c47-a38b-6f123b62dce6">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </n8bc46b862004554b29f25437dcecdb2>
-    <Fiscal_x0020_Year xmlns="17eb8759-252b-418d-a649-70aff91fc5df" xsi:nil="true"/>
-    <Archive xmlns="17eb8759-252b-418d-a649-70aff91fc5df">false</Archive>
-    <b348aa9236b94ac88332be997039b018 xmlns="17eb8759-252b-418d-a649-70aff91fc5df">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </b348aa9236b94ac88332be997039b018>
-    <_dlc_DocId xmlns="039bc2d6-e16a-4b4d-b61d-73ee5a6b5720">QWPW5C3C64YX-694079015-91</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="039bc2d6-e16a-4b4d-b61d-73ee5a6b5720">
-      <Url>http://cscgikdcapmdw40/ProjectsLab/AODACompliance/_layouts/15/DocIdRedir.aspx?ID=QWPW5C3C64YX-694079015-91</Url>
-      <Description>QWPW5C3C64YX-694079015-91</Description>
-    </_dlc_DocIdUrl>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001B7F6C1E041661428C0804F60FDF9579" ma:contentTypeVersion="1" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="269e77b516f09928499b1be999970057">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="17eb8759-252b-418d-a649-70aff91fc5df" xmlns:ns3="039bc2d6-e16a-4b4d-b61d-73ee5a6b5720" xmlns:ns4="93977a9a-7c70-4c47-a38b-6f123b62dce6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="41b65eea62d023978f15f5547645abd7" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="17eb8759-252b-418d-a649-70aff91fc5df"/>
@@ -11242,42 +11262,86 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
+</file>
+
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="039bc2d6-e16a-4b4d-b61d-73ee5a6b5720"/>
+    <n8bc46b862004554b29f25437dcecdb2 xmlns="93977a9a-7c70-4c47-a38b-6f123b62dce6">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </n8bc46b862004554b29f25437dcecdb2>
+    <Fiscal_x0020_Year xmlns="17eb8759-252b-418d-a649-70aff91fc5df" xsi:nil="true"/>
+    <Archive xmlns="17eb8759-252b-418d-a649-70aff91fc5df">false</Archive>
+    <b348aa9236b94ac88332be997039b018 xmlns="17eb8759-252b-418d-a649-70aff91fc5df">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </b348aa9236b94ac88332be997039b018>
+    <_dlc_DocId xmlns="039bc2d6-e16a-4b4d-b61d-73ee5a6b5720">QWPW5C3C64YX-694079015-91</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="039bc2d6-e16a-4b4d-b61d-73ee5a6b5720">
+      <Url>http://cscgikdcapmdw40/ProjectsLab/AODACompliance/_layouts/15/DocIdRedir.aspx?ID=QWPW5C3C64YX-694079015-91</Url>
+      <Description>QWPW5C3C64YX-694079015-91</Description>
+    </_dlc_DocIdUrl>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C507B214-A4AD-4147-9668-C65BAB18F1D2}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D6D3747C-BDC7-48F7-9B5A-BD9117F21569}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="93977a9a-7c70-4c47-a38b-6f123b62dce6"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="039bc2d6-e16a-4b4d-b61d-73ee5a6b5720"/>
-    <ds:schemaRef ds:uri="17eb8759-252b-418d-a649-70aff91fc5df"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2E5D2D22-6D00-46CD-B7EA-B8CE8E1546D9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3C5CD16F-1A82-4BAB-88E6-9D42833A2748}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11297,10 +11361,28 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2E5D2D22-6D00-46CD-B7EA-B8CE8E1546D9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D6D3747C-BDC7-48F7-9B5A-BD9117F21569}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C507B214-A4AD-4147-9668-C65BAB18F1D2}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="93977a9a-7c70-4c47-a38b-6f123b62dce6"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="039bc2d6-e16a-4b4d-b61d-73ee5a6b5720"/>
+    <ds:schemaRef ds:uri="17eb8759-252b-418d-a649-70aff91fc5df"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
added some colour formatting
</commit_message>
<xml_diff>
--- a/AxeAccessibilityDriver/AxeAccessibilityDriver/AODA_Template.xlsx
+++ b/AxeAccessibilityDriver/AxeAccessibilityDriver/AODA_Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DUONGCH\Projects\AxeAccessibilityDriver\AxeAccessibilityDriver\AxeAccessibilityDriver\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C951448F-29A6-4435-B53C-E5186062A37C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{901D25B9-0CAA-4794-80B0-E5F9C042FEB5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" tabRatio="760" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4620" yWindow="780" windowWidth="21600" windowHeight="11385" tabRatio="760" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="5" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="255">
   <si>
     <t>1.1.1</t>
   </si>
@@ -3732,121 +3732,22 @@
     <xf numFmtId="0" fontId="49" fillId="13" borderId="0" xfId="16" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="13" fillId="5" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="27" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -3889,6 +3790,105 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="27" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="13" fillId="5" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="2" borderId="25" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -7831,7 +7831,7 @@
   </sheetPr>
   <dimension ref="A1:XFC81"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="115" zoomScalePageLayoutView="160" workbookViewId="0">
+    <sheetView topLeftCell="A24" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="115" zoomScalePageLayoutView="160" workbookViewId="0">
       <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
@@ -7857,16 +7857,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="13" customFormat="1" ht="37.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="178" t="s">
+      <c r="A1" s="185" t="s">
         <v>225</v>
       </c>
-      <c r="B1" s="178"/>
-      <c r="C1" s="178"/>
-      <c r="D1" s="178"/>
-      <c r="E1" s="178"/>
-      <c r="F1" s="178"/>
-      <c r="G1" s="178"/>
-      <c r="H1" s="179"/>
+      <c r="B1" s="185"/>
+      <c r="C1" s="185"/>
+      <c r="D1" s="185"/>
+      <c r="E1" s="185"/>
+      <c r="F1" s="185"/>
+      <c r="G1" s="185"/>
+      <c r="H1" s="186"/>
       <c r="I1" s="11"/>
       <c r="J1" s="12"/>
       <c r="K1" s="1"/>
@@ -7880,13 +7880,13 @@
       <c r="S1" s="1"/>
     </row>
     <row r="2" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="180" t="s">
+      <c r="A2" s="166" t="s">
         <v>61</v>
       </c>
-      <c r="B2" s="180"/>
-      <c r="C2" s="181"/>
-      <c r="D2" s="181"/>
-      <c r="E2" s="182"/>
+      <c r="B2" s="166"/>
+      <c r="C2" s="189"/>
+      <c r="D2" s="189"/>
+      <c r="E2" s="190"/>
       <c r="F2" s="39"/>
       <c r="G2" s="1"/>
       <c r="H2" s="16"/>
@@ -7898,13 +7898,13 @@
       <c r="N2" s="13"/>
     </row>
     <row r="3" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="180" t="s">
+      <c r="A3" s="166" t="s">
         <v>63</v>
       </c>
-      <c r="B3" s="180"/>
-      <c r="C3" s="195"/>
-      <c r="D3" s="196"/>
-      <c r="E3" s="197"/>
+      <c r="B3" s="166"/>
+      <c r="C3" s="202"/>
+      <c r="D3" s="203"/>
+      <c r="E3" s="204"/>
       <c r="F3" s="39"/>
       <c r="G3" s="1"/>
       <c r="H3" s="16"/>
@@ -7916,12 +7916,12 @@
       <c r="N3" s="13"/>
     </row>
     <row r="4" spans="1:19" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="180" t="s">
+      <c r="A4" s="166" t="s">
         <v>77</v>
       </c>
-      <c r="B4" s="180"/>
-      <c r="C4" s="161"/>
-      <c r="D4" s="161"/>
+      <c r="B4" s="166"/>
+      <c r="C4" s="212"/>
+      <c r="D4" s="212"/>
       <c r="E4" s="91"/>
       <c r="F4" s="39"/>
       <c r="G4" s="1"/>
@@ -7934,13 +7934,13 @@
       <c r="N4" s="13"/>
     </row>
     <row r="5" spans="1:19" ht="27" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="162" t="s">
+      <c r="A5" s="165" t="s">
         <v>78</v>
       </c>
-      <c r="B5" s="162"/>
-      <c r="C5" s="163"/>
-      <c r="D5" s="163"/>
-      <c r="E5" s="164"/>
+      <c r="B5" s="165"/>
+      <c r="C5" s="213"/>
+      <c r="D5" s="213"/>
+      <c r="E5" s="214"/>
       <c r="F5" s="39"/>
       <c r="G5" s="1"/>
       <c r="H5" s="16"/>
@@ -7952,13 +7952,13 @@
       <c r="N5" s="13"/>
     </row>
     <row r="6" spans="1:19" ht="27" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="162" t="s">
+      <c r="A6" s="165" t="s">
         <v>79</v>
       </c>
-      <c r="B6" s="162"/>
-      <c r="C6" s="165"/>
-      <c r="D6" s="165"/>
-      <c r="E6" s="166"/>
+      <c r="B6" s="165"/>
+      <c r="C6" s="163"/>
+      <c r="D6" s="163"/>
+      <c r="E6" s="164"/>
       <c r="F6" s="39"/>
       <c r="G6" s="1"/>
       <c r="H6" s="16"/>
@@ -7970,13 +7970,13 @@
       <c r="N6" s="13"/>
     </row>
     <row r="7" spans="1:19" ht="27" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="162" t="s">
+      <c r="A7" s="165" t="s">
         <v>80</v>
       </c>
-      <c r="B7" s="162"/>
-      <c r="C7" s="165"/>
-      <c r="D7" s="165"/>
-      <c r="E7" s="166"/>
+      <c r="B7" s="165"/>
+      <c r="C7" s="163"/>
+      <c r="D7" s="163"/>
+      <c r="E7" s="164"/>
       <c r="F7" s="39"/>
       <c r="G7" s="1"/>
       <c r="H7" s="16"/>
@@ -7988,13 +7988,13 @@
       <c r="N7" s="13"/>
     </row>
     <row r="8" spans="1:19" ht="27" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="162" t="s">
+      <c r="A8" s="165" t="s">
         <v>81</v>
       </c>
-      <c r="B8" s="162"/>
-      <c r="C8" s="165"/>
-      <c r="D8" s="165"/>
-      <c r="E8" s="166"/>
+      <c r="B8" s="165"/>
+      <c r="C8" s="163"/>
+      <c r="D8" s="163"/>
+      <c r="E8" s="164"/>
       <c r="F8" s="39"/>
       <c r="G8" s="1"/>
       <c r="H8" s="16"/>
@@ -8006,16 +8006,16 @@
       <c r="N8" s="13"/>
     </row>
     <row r="9" spans="1:19" s="37" customFormat="1" ht="52.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="184" t="s">
+      <c r="A9" s="193" t="s">
         <v>76</v>
       </c>
-      <c r="B9" s="185"/>
-      <c r="C9" s="185"/>
-      <c r="D9" s="185"/>
-      <c r="E9" s="185"/>
-      <c r="F9" s="185"/>
-      <c r="G9" s="185"/>
-      <c r="H9" s="185"/>
+      <c r="B9" s="194"/>
+      <c r="C9" s="194"/>
+      <c r="D9" s="194"/>
+      <c r="E9" s="194"/>
+      <c r="F9" s="194"/>
+      <c r="G9" s="194"/>
+      <c r="H9" s="194"/>
       <c r="I9" s="18"/>
       <c r="J9" s="18"/>
       <c r="K9" s="18"/>
@@ -8025,16 +8025,16 @@
       <c r="Q9" s="108"/>
     </row>
     <row r="10" spans="1:19" s="22" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="186" t="s">
+      <c r="A10" s="195" t="s">
         <v>210</v>
       </c>
-      <c r="B10" s="187"/>
-      <c r="C10" s="187"/>
-      <c r="D10" s="187"/>
-      <c r="E10" s="187"/>
-      <c r="F10" s="187"/>
-      <c r="G10" s="187"/>
-      <c r="H10" s="188"/>
+      <c r="B10" s="196"/>
+      <c r="C10" s="196"/>
+      <c r="D10" s="196"/>
+      <c r="E10" s="196"/>
+      <c r="F10" s="196"/>
+      <c r="G10" s="196"/>
+      <c r="H10" s="197"/>
       <c r="I10" s="21"/>
       <c r="J10" s="21"/>
       <c r="K10" s="21"/>
@@ -8044,10 +8044,10 @@
       <c r="Q10" s="23"/>
     </row>
     <row r="11" spans="1:19" ht="55.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="193" t="s">
+      <c r="A11" s="200" t="s">
         <v>54</v>
       </c>
-      <c r="B11" s="194"/>
+      <c r="B11" s="201"/>
       <c r="C11" s="123" t="s">
         <v>40</v>
       </c>
@@ -8057,10 +8057,10 @@
       <c r="E11" s="123" t="s">
         <v>99</v>
       </c>
-      <c r="F11" s="189" t="s">
+      <c r="F11" s="199" t="s">
         <v>52</v>
       </c>
-      <c r="G11" s="189"/>
+      <c r="G11" s="199"/>
       <c r="H11" s="124" t="s">
         <v>53</v>
       </c>
@@ -8072,18 +8072,18 @@
       <c r="N11" s="13"/>
     </row>
     <row r="12" spans="1:19" ht="69.599999999999994" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="172" t="s">
+      <c r="A12" s="191" t="s">
         <v>83</v>
       </c>
-      <c r="B12" s="183"/>
-      <c r="C12" s="190" t="s">
+      <c r="B12" s="192"/>
+      <c r="C12" s="182" t="s">
         <v>179</v>
       </c>
-      <c r="D12" s="191"/>
-      <c r="E12" s="191"/>
-      <c r="F12" s="191"/>
-      <c r="G12" s="191"/>
-      <c r="H12" s="192"/>
+      <c r="D12" s="183"/>
+      <c r="E12" s="183"/>
+      <c r="F12" s="183"/>
+      <c r="G12" s="183"/>
+      <c r="H12" s="184"/>
       <c r="I12" s="13"/>
       <c r="J12" s="13"/>
       <c r="K12" s="13"/>
@@ -8508,14 +8508,14 @@
       <c r="Q26" s="102"/>
     </row>
     <row r="27" spans="1:17" ht="17.45" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="176" t="s">
+      <c r="A27" s="187" t="s">
         <v>67</v>
       </c>
-      <c r="B27" s="177"/>
-      <c r="C27" s="177"/>
-      <c r="D27" s="177"/>
-      <c r="E27" s="177"/>
-      <c r="F27" s="177"/>
+      <c r="B27" s="188"/>
+      <c r="C27" s="188"/>
+      <c r="D27" s="188"/>
+      <c r="E27" s="188"/>
+      <c r="F27" s="188"/>
       <c r="G27" s="24">
         <f>SUM(H13:H26)</f>
         <v>0</v>
@@ -8532,18 +8532,18 @@
       <c r="N27" s="13"/>
     </row>
     <row r="28" spans="1:17" ht="53.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="172" t="s">
+      <c r="A28" s="191" t="s">
         <v>84</v>
       </c>
-      <c r="B28" s="173"/>
-      <c r="C28" s="190" t="s">
+      <c r="B28" s="198"/>
+      <c r="C28" s="182" t="s">
         <v>185</v>
       </c>
-      <c r="D28" s="191"/>
-      <c r="E28" s="191"/>
-      <c r="F28" s="191"/>
-      <c r="G28" s="191"/>
-      <c r="H28" s="192"/>
+      <c r="D28" s="183"/>
+      <c r="E28" s="183"/>
+      <c r="F28" s="183"/>
+      <c r="G28" s="183"/>
+      <c r="H28" s="184"/>
       <c r="I28" s="13"/>
       <c r="J28" s="13"/>
       <c r="K28" s="13"/>
@@ -8897,14 +8897,14 @@
       <c r="Q40" s="102"/>
     </row>
     <row r="41" spans="1:17" ht="48.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="176" t="s">
+      <c r="A41" s="187" t="s">
         <v>66</v>
       </c>
-      <c r="B41" s="177"/>
-      <c r="C41" s="177"/>
-      <c r="D41" s="177"/>
-      <c r="E41" s="177"/>
-      <c r="F41" s="177"/>
+      <c r="B41" s="188"/>
+      <c r="C41" s="188"/>
+      <c r="D41" s="188"/>
+      <c r="E41" s="188"/>
+      <c r="F41" s="188"/>
       <c r="G41" s="24">
         <f>SUM(H29:H40)</f>
         <v>0</v>
@@ -8921,18 +8921,18 @@
       <c r="N41" s="13"/>
     </row>
     <row r="42" spans="1:17" ht="54.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="172" t="s">
+      <c r="A42" s="191" t="s">
         <v>85</v>
       </c>
-      <c r="B42" s="173"/>
-      <c r="C42" s="190" t="s">
+      <c r="B42" s="198"/>
+      <c r="C42" s="182" t="s">
         <v>190</v>
       </c>
-      <c r="D42" s="191"/>
-      <c r="E42" s="191"/>
-      <c r="F42" s="191"/>
-      <c r="G42" s="191"/>
-      <c r="H42" s="192"/>
+      <c r="D42" s="183"/>
+      <c r="E42" s="183"/>
+      <c r="F42" s="183"/>
+      <c r="G42" s="183"/>
+      <c r="H42" s="184"/>
       <c r="I42" s="13"/>
       <c r="J42" s="13"/>
       <c r="K42" s="13"/>
@@ -9231,14 +9231,14 @@
       <c r="Q52" s="102"/>
     </row>
     <row r="53" spans="1:17" ht="74.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="176" t="s">
+      <c r="A53" s="187" t="s">
         <v>65</v>
       </c>
-      <c r="B53" s="177"/>
-      <c r="C53" s="177"/>
-      <c r="D53" s="177"/>
-      <c r="E53" s="177"/>
-      <c r="F53" s="177"/>
+      <c r="B53" s="188"/>
+      <c r="C53" s="188"/>
+      <c r="D53" s="188"/>
+      <c r="E53" s="188"/>
+      <c r="F53" s="188"/>
       <c r="G53" s="25">
         <f>SUM(H43:H52)</f>
         <v>0</v>
@@ -9255,18 +9255,18 @@
       <c r="N53" s="13"/>
     </row>
     <row r="54" spans="1:17" ht="47.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="170" t="s">
+      <c r="A54" s="208" t="s">
         <v>86</v>
       </c>
-      <c r="B54" s="171"/>
-      <c r="C54" s="167" t="s">
+      <c r="B54" s="209"/>
+      <c r="C54" s="205" t="s">
         <v>196</v>
       </c>
-      <c r="D54" s="168"/>
-      <c r="E54" s="168"/>
-      <c r="F54" s="168"/>
-      <c r="G54" s="168"/>
-      <c r="H54" s="169"/>
+      <c r="D54" s="206"/>
+      <c r="E54" s="206"/>
+      <c r="F54" s="206"/>
+      <c r="G54" s="206"/>
+      <c r="H54" s="207"/>
       <c r="I54" s="13"/>
       <c r="J54" s="13"/>
       <c r="K54" s="13"/>
@@ -9333,14 +9333,14 @@
       <c r="Q56" s="102"/>
     </row>
     <row r="57" spans="1:17" ht="43.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="176" t="s">
+      <c r="A57" s="187" t="s">
         <v>64</v>
       </c>
-      <c r="B57" s="177"/>
-      <c r="C57" s="177"/>
-      <c r="D57" s="177"/>
-      <c r="E57" s="177"/>
-      <c r="F57" s="177"/>
+      <c r="B57" s="188"/>
+      <c r="C57" s="188"/>
+      <c r="D57" s="188"/>
+      <c r="E57" s="188"/>
+      <c r="F57" s="188"/>
       <c r="G57" s="24">
         <f>SUM(H55:H56)</f>
         <v>0</v>
@@ -9357,16 +9357,16 @@
       <c r="N57" s="13"/>
     </row>
     <row r="58" spans="1:17" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="174" t="s">
+      <c r="A58" s="210" t="s">
         <v>88</v>
       </c>
-      <c r="B58" s="175"/>
-      <c r="C58" s="175"/>
-      <c r="D58" s="175"/>
-      <c r="E58" s="175"/>
-      <c r="F58" s="212"/>
-      <c r="G58" s="213"/>
-      <c r="H58" s="214"/>
+      <c r="B58" s="211"/>
+      <c r="C58" s="211"/>
+      <c r="D58" s="211"/>
+      <c r="E58" s="211"/>
+      <c r="F58" s="179"/>
+      <c r="G58" s="180"/>
+      <c r="H58" s="181"/>
       <c r="I58" s="13"/>
       <c r="J58" s="13"/>
       <c r="K58" s="13"/>
@@ -9375,14 +9375,14 @@
       <c r="N58" s="13"/>
     </row>
     <row r="59" spans="1:17" ht="24.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A59" s="202"/>
-      <c r="B59" s="203"/>
+      <c r="A59" s="169"/>
+      <c r="B59" s="170"/>
       <c r="C59" s="28"/>
-      <c r="D59" s="209" t="s">
+      <c r="D59" s="176" t="s">
         <v>87</v>
       </c>
-      <c r="E59" s="210"/>
-      <c r="F59" s="211"/>
+      <c r="E59" s="177"/>
+      <c r="F59" s="178"/>
       <c r="G59" s="29">
         <f>SUM(H13:H26)+SUM(H29:H40)+SUM(H43:H52)+SUM(H55:H56)</f>
         <v>0</v>
@@ -9396,13 +9396,13 @@
       <c r="N59" s="13"/>
     </row>
     <row r="60" spans="1:17" ht="48" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="204"/>
-      <c r="B60" s="205"/>
+      <c r="A60" s="171"/>
+      <c r="B60" s="172"/>
       <c r="C60" s="31"/>
-      <c r="D60" s="206" t="s">
+      <c r="D60" s="173" t="s">
         <v>55</v>
       </c>
-      <c r="E60" s="207"/>
+      <c r="E60" s="174"/>
       <c r="F60" s="32"/>
       <c r="G60" s="33"/>
       <c r="H60" s="34"/>
@@ -9414,13 +9414,13 @@
       <c r="N60" s="13"/>
     </row>
     <row r="61" spans="1:17" ht="55.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="204"/>
-      <c r="B61" s="205"/>
+      <c r="A61" s="171"/>
+      <c r="B61" s="172"/>
       <c r="C61" s="31"/>
-      <c r="D61" s="206" t="s">
+      <c r="D61" s="173" t="s">
         <v>56</v>
       </c>
-      <c r="E61" s="207"/>
+      <c r="E61" s="174"/>
       <c r="F61" s="32"/>
       <c r="G61" s="33"/>
       <c r="H61" s="34"/>
@@ -9432,13 +9432,13 @@
       <c r="N61" s="13"/>
     </row>
     <row r="62" spans="1:17" ht="39.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="204"/>
-      <c r="B62" s="205"/>
+      <c r="A62" s="171"/>
+      <c r="B62" s="172"/>
       <c r="C62" s="35"/>
-      <c r="D62" s="208" t="s">
+      <c r="D62" s="175" t="s">
         <v>57</v>
       </c>
-      <c r="E62" s="207"/>
+      <c r="E62" s="174"/>
       <c r="F62" s="32"/>
       <c r="G62" s="33"/>
       <c r="H62" s="34"/>
@@ -9457,11 +9457,11 @@
         <f>SUM(H13:H26)+SUM(H29:H40)+SUM(H43:H52)+SUM(H55:H56)</f>
         <v>0</v>
       </c>
-      <c r="E63" s="200" t="s">
+      <c r="E63" s="167" t="s">
         <v>154</v>
       </c>
-      <c r="F63" s="200"/>
-      <c r="G63" s="201"/>
+      <c r="F63" s="167"/>
+      <c r="G63" s="168"/>
       <c r="H63" s="43"/>
       <c r="I63" s="13"/>
       <c r="J63" s="13"/>
@@ -9471,10 +9471,10 @@
       <c r="N63" s="13"/>
     </row>
     <row r="64" spans="1:17" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="198" t="s">
+      <c r="A64" s="161" t="s">
         <v>58</v>
       </c>
-      <c r="B64" s="199"/>
+      <c r="B64" s="162"/>
       <c r="C64" s="18"/>
       <c r="D64" s="19"/>
       <c r="E64" s="44"/>
@@ -9548,6 +9548,33 @@
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
   <mergeCells count="43">
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="C54:H54"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="A58:E58"/>
+    <mergeCell ref="A57:F57"/>
+    <mergeCell ref="A53:F53"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A41:F41"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="A27:F27"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A9:H9"/>
+    <mergeCell ref="A10:H10"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="C12:H12"/>
+    <mergeCell ref="C28:H28"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="A7:B7"/>
     <mergeCell ref="A64:B64"/>
     <mergeCell ref="C7:E7"/>
     <mergeCell ref="A8:B8"/>
@@ -9564,33 +9591,6 @@
     <mergeCell ref="D59:F59"/>
     <mergeCell ref="F58:H58"/>
     <mergeCell ref="C42:H42"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A41:F41"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="A27:F27"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A9:H9"/>
-    <mergeCell ref="A10:H10"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="C12:H12"/>
-    <mergeCell ref="C28:H28"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="C54:H54"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="A58:E58"/>
-    <mergeCell ref="A57:F57"/>
-    <mergeCell ref="A53:F53"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:E6"/>
   </mergeCells>
   <conditionalFormatting sqref="F43:F52 F55:F56 F13:F26 F29:F40">
     <cfRule type="cellIs" dxfId="136" priority="371" operator="equal">
@@ -10379,7 +10379,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:T43"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
@@ -10478,9 +10478,7 @@
       <c r="C4" s="142"/>
       <c r="D4" s="137"/>
       <c r="E4" s="138"/>
-      <c r="F4" s="139" t="s">
-        <v>252</v>
-      </c>
+      <c r="F4" s="139"/>
       <c r="G4" s="140"/>
       <c r="H4" s="141"/>
       <c r="L4" s="118" t="s">
@@ -11033,15 +11031,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001B7F6C1E041661428C0804F60FDF9579" ma:contentTypeVersion="1" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="269e77b516f09928499b1be999970057">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="17eb8759-252b-418d-a649-70aff91fc5df" xmlns:ns3="039bc2d6-e16a-4b4d-b61d-73ee5a6b5720" xmlns:ns4="93977a9a-7c70-4c47-a38b-6f123b62dce6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="41b65eea62d023978f15f5547645abd7" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="17eb8759-252b-418d-a649-70aff91fc5df"/>
@@ -11262,7 +11251,37 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="039bc2d6-e16a-4b4d-b61d-73ee5a6b5720"/>
+    <n8bc46b862004554b29f25437dcecdb2 xmlns="93977a9a-7c70-4c47-a38b-6f123b62dce6">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </n8bc46b862004554b29f25437dcecdb2>
+    <Fiscal_x0020_Year xmlns="17eb8759-252b-418d-a649-70aff91fc5df" xsi:nil="true"/>
+    <Archive xmlns="17eb8759-252b-418d-a649-70aff91fc5df">false</Archive>
+    <b348aa9236b94ac88332be997039b018 xmlns="17eb8759-252b-418d-a649-70aff91fc5df">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </b348aa9236b94ac88332be997039b018>
+    <_dlc_DocId xmlns="039bc2d6-e16a-4b4d-b61d-73ee5a6b5720">QWPW5C3C64YX-694079015-91</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="039bc2d6-e16a-4b4d-b61d-73ee5a6b5720">
+      <Url>http://cscgikdcapmdw40/ProjectsLab/AODACompliance/_layouts/15/DocIdRedir.aspx?ID=QWPW5C3C64YX-694079015-91</Url>
+      <Description>QWPW5C3C64YX-694079015-91</Description>
+    </_dlc_DocIdUrl>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
   <Receiver>
@@ -11312,36 +11331,7 @@
 </spe:Receivers>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="039bc2d6-e16a-4b4d-b61d-73ee5a6b5720"/>
-    <n8bc46b862004554b29f25437dcecdb2 xmlns="93977a9a-7c70-4c47-a38b-6f123b62dce6">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </n8bc46b862004554b29f25437dcecdb2>
-    <Fiscal_x0020_Year xmlns="17eb8759-252b-418d-a649-70aff91fc5df" xsi:nil="true"/>
-    <Archive xmlns="17eb8759-252b-418d-a649-70aff91fc5df">false</Archive>
-    <b348aa9236b94ac88332be997039b018 xmlns="17eb8759-252b-418d-a649-70aff91fc5df">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </b348aa9236b94ac88332be997039b018>
-    <_dlc_DocId xmlns="039bc2d6-e16a-4b4d-b61d-73ee5a6b5720">QWPW5C3C64YX-694079015-91</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="039bc2d6-e16a-4b4d-b61d-73ee5a6b5720">
-      <Url>http://cscgikdcapmdw40/ProjectsLab/AODACompliance/_layouts/15/DocIdRedir.aspx?ID=QWPW5C3C64YX-694079015-91</Url>
-      <Description>QWPW5C3C64YX-694079015-91</Description>
-    </_dlc_DocIdUrl>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D6D3747C-BDC7-48F7-9B5A-BD9117F21569}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3C5CD16F-1A82-4BAB-88E6-9D42833A2748}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11361,15 +11351,15 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2E5D2D22-6D00-46CD-B7EA-B8CE8E1546D9}">
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D6D3747C-BDC7-48F7-9B5A-BD9117F21569}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C507B214-A4AD-4147-9668-C65BAB18F1D2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
@@ -11385,4 +11375,12 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2E5D2D22-6D00-46CD-B7EA-B8CE8E1546D9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>